<commit_message>
Separando objetos de animacion y luces puntuales
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\REPO\Pachanga-Time\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85546ED6-A313-437A-9703-D8F3CE6F4BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A612C52-3D27-4AF4-86B9-A7D437858FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>FASES</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Nombre: Cervantes Rubí Brandon</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="43">
     <border>
@@ -905,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1064,6 +1073,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2054,7 +2065,9 @@
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="86"/>
+      <c r="L16" s="86">
+        <v>1</v>
+      </c>
       <c r="M16" s="81"/>
       <c r="N16" s="81"/>
       <c r="O16" s="81"/>
@@ -2542,7 +2555,7 @@
       <c r="L29" s="83"/>
       <c r="M29" s="81"/>
       <c r="N29" s="81"/>
-      <c r="O29" s="85"/>
+      <c r="O29" s="117"/>
       <c r="P29" s="81"/>
       <c r="Q29" s="81"/>
       <c r="R29" s="82"/>
@@ -3100,7 +3113,9 @@
       <c r="Q44" s="81"/>
       <c r="R44" s="82"/>
       <c r="S44" s="83"/>
-      <c r="T44" s="81"/>
+      <c r="T44" s="81" t="s">
+        <v>78</v>
+      </c>
       <c r="U44" s="85"/>
       <c r="V44" s="81"/>
       <c r="W44" s="81"/>
@@ -3251,7 +3266,9 @@
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="R48" s="82"/>
-      <c r="S48" s="83"/>
+      <c r="S48" s="83" t="s">
+        <v>78</v>
+      </c>
       <c r="T48" s="89"/>
       <c r="U48" s="84"/>
       <c r="V48" s="81"/>
@@ -3327,7 +3344,9 @@
       <c r="R50" s="82"/>
       <c r="S50" s="83"/>
       <c r="T50" s="81"/>
-      <c r="U50" s="84"/>
+      <c r="U50" s="84" t="s">
+        <v>78</v>
+      </c>
       <c r="V50" s="90"/>
       <c r="W50" s="81"/>
       <c r="X50" s="81"/>
@@ -3803,7 +3822,9 @@
       <c r="U63" s="84"/>
       <c r="V63" s="81"/>
       <c r="W63" s="81"/>
-      <c r="X63" s="87"/>
+      <c r="X63" s="87">
+        <v>1</v>
+      </c>
       <c r="Y63" s="82"/>
       <c r="Z63" s="83"/>
       <c r="AA63" s="84"/>
@@ -4200,7 +4221,7 @@
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="39"/>
-      <c r="L74" s="80"/>
+      <c r="L74" s="120"/>
       <c r="M74" s="81"/>
       <c r="N74" s="81"/>
       <c r="O74" s="81"/>
@@ -4348,14 +4369,14 @@
       <c r="K78" s="70"/>
       <c r="L78" s="80"/>
       <c r="M78" s="85"/>
-      <c r="N78" s="85"/>
-      <c r="O78" s="85"/>
-      <c r="P78" s="85"/>
-      <c r="Q78" s="85"/>
-      <c r="R78" s="85"/>
-      <c r="S78" s="80"/>
+      <c r="N78" s="117"/>
+      <c r="O78" s="117"/>
+      <c r="P78" s="117"/>
+      <c r="Q78" s="117"/>
+      <c r="R78" s="117"/>
+      <c r="S78" s="120"/>
       <c r="T78" s="85"/>
-      <c r="U78" s="85"/>
+      <c r="U78" s="121"/>
       <c r="V78" s="85"/>
       <c r="W78" s="85"/>
       <c r="X78" s="85"/>

</xml_diff>

<commit_message>
Animacion del personaje sobre el agua y las nubes
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A612C52-3D27-4AF4-86B9-A7D437858FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195A88F9-45D6-450D-9F74-22113D6B1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1043,10 +1043,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1075,6 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1391,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="Y46" sqref="Y46"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="T49" sqref="T48:T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1717,9 +1716,9 @@
       <c r="AA6" s="76"/>
       <c r="AB6" s="74"/>
       <c r="AC6" s="74"/>
-      <c r="AD6" s="95"/>
-      <c r="AE6" s="96"/>
-      <c r="AF6" s="97"/>
+      <c r="AD6" s="93"/>
+      <c r="AE6" s="94"/>
+      <c r="AF6" s="95"/>
       <c r="AG6" s="10"/>
     </row>
     <row r="7" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1754,9 +1753,9 @@
       <c r="AA7" s="84"/>
       <c r="AB7" s="81"/>
       <c r="AC7" s="85"/>
-      <c r="AD7" s="98"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="100"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="97"/>
+      <c r="AF7" s="98"/>
       <c r="AG7" s="10"/>
     </row>
     <row r="8" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1791,9 +1790,9 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="68"/>
       <c r="AC8" s="79"/>
-      <c r="AD8" s="101"/>
-      <c r="AE8" s="102"/>
-      <c r="AF8" s="103"/>
+      <c r="AD8" s="99"/>
+      <c r="AE8" s="100"/>
+      <c r="AF8" s="101"/>
       <c r="AG8" s="10"/>
     </row>
     <row r="9" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1828,9 +1827,9 @@
       <c r="AA9" s="84"/>
       <c r="AB9" s="81"/>
       <c r="AC9" s="81"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="99"/>
-      <c r="AF9" s="100"/>
+      <c r="AD9" s="96"/>
+      <c r="AE9" s="97"/>
+      <c r="AF9" s="98"/>
       <c r="AG9" s="10"/>
     </row>
     <row r="10" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1863,9 +1862,9 @@
       <c r="AA10" s="84"/>
       <c r="AB10" s="81"/>
       <c r="AC10" s="81"/>
-      <c r="AD10" s="98"/>
-      <c r="AE10" s="99"/>
-      <c r="AF10" s="100"/>
+      <c r="AD10" s="96"/>
+      <c r="AE10" s="97"/>
+      <c r="AF10" s="98"/>
       <c r="AG10" s="10"/>
     </row>
     <row r="11" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1900,9 +1899,9 @@
       <c r="AA11" s="84"/>
       <c r="AB11" s="81"/>
       <c r="AC11" s="81"/>
-      <c r="AD11" s="98"/>
-      <c r="AE11" s="99"/>
-      <c r="AF11" s="100"/>
+      <c r="AD11" s="96"/>
+      <c r="AE11" s="97"/>
+      <c r="AF11" s="98"/>
       <c r="AG11" s="10"/>
     </row>
     <row r="12" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1937,9 +1936,9 @@
       <c r="AA12" s="84"/>
       <c r="AB12" s="81"/>
       <c r="AC12" s="81"/>
-      <c r="AD12" s="98"/>
-      <c r="AE12" s="99"/>
-      <c r="AF12" s="100"/>
+      <c r="AD12" s="96"/>
+      <c r="AE12" s="97"/>
+      <c r="AF12" s="98"/>
       <c r="AG12" s="10"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
@@ -1974,9 +1973,9 @@
       <c r="AA13" s="84"/>
       <c r="AB13" s="81"/>
       <c r="AC13" s="81"/>
-      <c r="AD13" s="98"/>
-      <c r="AE13" s="99"/>
-      <c r="AF13" s="100"/>
+      <c r="AD13" s="96"/>
+      <c r="AE13" s="97"/>
+      <c r="AF13" s="98"/>
       <c r="AG13" s="10"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
@@ -2009,9 +2008,9 @@
       <c r="AA14" s="84"/>
       <c r="AB14" s="81"/>
       <c r="AC14" s="81"/>
-      <c r="AD14" s="98"/>
-      <c r="AE14" s="99"/>
-      <c r="AF14" s="100"/>
+      <c r="AD14" s="96"/>
+      <c r="AE14" s="97"/>
+      <c r="AF14" s="98"/>
       <c r="AG14" s="10"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
@@ -2046,9 +2045,9 @@
       <c r="AA15" s="84"/>
       <c r="AB15" s="81"/>
       <c r="AC15" s="81"/>
-      <c r="AD15" s="98"/>
-      <c r="AE15" s="99"/>
-      <c r="AF15" s="100"/>
+      <c r="AD15" s="96"/>
+      <c r="AE15" s="97"/>
+      <c r="AF15" s="98"/>
       <c r="AG15" s="10"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
@@ -2085,9 +2084,9 @@
       <c r="AA16" s="84"/>
       <c r="AB16" s="81"/>
       <c r="AC16" s="81"/>
-      <c r="AD16" s="98"/>
-      <c r="AE16" s="99"/>
-      <c r="AF16" s="100"/>
+      <c r="AD16" s="96"/>
+      <c r="AE16" s="97"/>
+      <c r="AF16" s="98"/>
       <c r="AG16" s="10"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
@@ -2105,7 +2104,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="39"/>
       <c r="L17" s="83"/>
-      <c r="M17" s="117"/>
+      <c r="M17" s="115"/>
       <c r="N17" s="81"/>
       <c r="O17" s="81"/>
       <c r="P17" s="81"/>
@@ -2122,9 +2121,9 @@
       <c r="AA17" s="84"/>
       <c r="AB17" s="81"/>
       <c r="AC17" s="81"/>
-      <c r="AD17" s="98"/>
-      <c r="AE17" s="99"/>
-      <c r="AF17" s="100"/>
+      <c r="AD17" s="96"/>
+      <c r="AE17" s="97"/>
+      <c r="AF17" s="98"/>
       <c r="AG17" s="10"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
@@ -2144,7 +2143,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="39"/>
       <c r="L18" s="83"/>
-      <c r="M18" s="117"/>
+      <c r="M18" s="115"/>
       <c r="N18" s="81"/>
       <c r="O18" s="81"/>
       <c r="P18" s="81"/>
@@ -2161,9 +2160,9 @@
       <c r="AA18" s="84"/>
       <c r="AB18" s="81"/>
       <c r="AC18" s="81"/>
-      <c r="AD18" s="98"/>
-      <c r="AE18" s="99"/>
-      <c r="AF18" s="100"/>
+      <c r="AD18" s="96"/>
+      <c r="AE18" s="97"/>
+      <c r="AF18" s="98"/>
       <c r="AG18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.35">
@@ -2181,7 +2180,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="39"/>
       <c r="L19" s="83"/>
-      <c r="M19" s="117"/>
+      <c r="M19" s="115"/>
       <c r="N19" s="81"/>
       <c r="O19" s="81"/>
       <c r="P19" s="81"/>
@@ -2198,9 +2197,9 @@
       <c r="AA19" s="84"/>
       <c r="AB19" s="81"/>
       <c r="AC19" s="81"/>
-      <c r="AD19" s="98"/>
-      <c r="AE19" s="99"/>
-      <c r="AF19" s="100"/>
+      <c r="AD19" s="96"/>
+      <c r="AE19" s="97"/>
+      <c r="AF19" s="98"/>
       <c r="AG19" s="10"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
@@ -2235,9 +2234,9 @@
       <c r="AA20" s="84"/>
       <c r="AB20" s="81"/>
       <c r="AC20" s="81"/>
-      <c r="AD20" s="98"/>
-      <c r="AE20" s="99"/>
-      <c r="AF20" s="100"/>
+      <c r="AD20" s="96"/>
+      <c r="AE20" s="97"/>
+      <c r="AF20" s="98"/>
       <c r="AG20" s="10"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
@@ -2258,7 +2257,7 @@
       <c r="K21" s="39"/>
       <c r="L21" s="83"/>
       <c r="M21" s="81"/>
-      <c r="N21" s="117"/>
+      <c r="N21" s="115"/>
       <c r="O21" s="81"/>
       <c r="P21" s="81"/>
       <c r="Q21" s="81"/>
@@ -2274,9 +2273,9 @@
       <c r="AA21" s="84"/>
       <c r="AB21" s="81"/>
       <c r="AC21" s="81"/>
-      <c r="AD21" s="98"/>
-      <c r="AE21" s="99"/>
-      <c r="AF21" s="100"/>
+      <c r="AD21" s="96"/>
+      <c r="AE21" s="97"/>
+      <c r="AF21" s="98"/>
       <c r="AG21" s="10"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
@@ -2295,7 +2294,7 @@
       <c r="K22" s="39"/>
       <c r="L22" s="83"/>
       <c r="M22" s="81"/>
-      <c r="N22" s="117"/>
+      <c r="N22" s="115"/>
       <c r="O22" s="81"/>
       <c r="P22" s="81"/>
       <c r="Q22" s="81"/>
@@ -2311,9 +2310,9 @@
       <c r="AA22" s="84"/>
       <c r="AB22" s="81"/>
       <c r="AC22" s="81"/>
-      <c r="AD22" s="98"/>
-      <c r="AE22" s="99"/>
-      <c r="AF22" s="100"/>
+      <c r="AD22" s="96"/>
+      <c r="AE22" s="97"/>
+      <c r="AF22" s="98"/>
       <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
@@ -2332,7 +2331,7 @@
       <c r="K23" s="39"/>
       <c r="L23" s="83"/>
       <c r="M23" s="81"/>
-      <c r="N23" s="117"/>
+      <c r="N23" s="115"/>
       <c r="O23" s="81"/>
       <c r="P23" s="81"/>
       <c r="Q23" s="81"/>
@@ -2348,9 +2347,9 @@
       <c r="AA23" s="84"/>
       <c r="AB23" s="81"/>
       <c r="AC23" s="81"/>
-      <c r="AD23" s="98"/>
-      <c r="AE23" s="99"/>
-      <c r="AF23" s="100"/>
+      <c r="AD23" s="96"/>
+      <c r="AE23" s="97"/>
+      <c r="AF23" s="98"/>
       <c r="AG23" s="10"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
@@ -2369,7 +2368,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="83"/>
       <c r="M24" s="81"/>
-      <c r="N24" s="117"/>
+      <c r="N24" s="115"/>
       <c r="O24" s="81"/>
       <c r="P24" s="81"/>
       <c r="Q24" s="81"/>
@@ -2385,9 +2384,9 @@
       <c r="AA24" s="84"/>
       <c r="AB24" s="81"/>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="98"/>
-      <c r="AE24" s="99"/>
-      <c r="AF24" s="100"/>
+      <c r="AD24" s="96"/>
+      <c r="AE24" s="97"/>
+      <c r="AF24" s="98"/>
       <c r="AG24" s="10"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
@@ -2407,7 +2406,7 @@
       <c r="L25" s="83"/>
       <c r="M25" s="81"/>
       <c r="N25" s="81"/>
-      <c r="O25" s="117"/>
+      <c r="O25" s="115"/>
       <c r="P25" s="81"/>
       <c r="Q25" s="81"/>
       <c r="R25" s="82"/>
@@ -2422,9 +2421,9 @@
       <c r="AA25" s="84"/>
       <c r="AB25" s="81"/>
       <c r="AC25" s="81"/>
-      <c r="AD25" s="98"/>
-      <c r="AE25" s="99"/>
-      <c r="AF25" s="100"/>
+      <c r="AD25" s="96"/>
+      <c r="AE25" s="97"/>
+      <c r="AF25" s="98"/>
       <c r="AG25" s="10"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
@@ -2444,7 +2443,7 @@
       <c r="L26" s="83"/>
       <c r="M26" s="81"/>
       <c r="N26" s="81"/>
-      <c r="O26" s="117"/>
+      <c r="O26" s="115"/>
       <c r="P26" s="81"/>
       <c r="Q26" s="81"/>
       <c r="R26" s="82"/>
@@ -2459,9 +2458,9 @@
       <c r="AA26" s="84"/>
       <c r="AB26" s="81"/>
       <c r="AC26" s="81"/>
-      <c r="AD26" s="98"/>
-      <c r="AE26" s="99"/>
-      <c r="AF26" s="100"/>
+      <c r="AD26" s="96"/>
+      <c r="AE26" s="97"/>
+      <c r="AF26" s="98"/>
       <c r="AG26" s="10"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
@@ -2481,7 +2480,7 @@
       <c r="L27" s="83"/>
       <c r="M27" s="81"/>
       <c r="N27" s="81"/>
-      <c r="O27" s="117"/>
+      <c r="O27" s="115"/>
       <c r="P27" s="81"/>
       <c r="Q27" s="81"/>
       <c r="R27" s="82"/>
@@ -2496,9 +2495,9 @@
       <c r="AA27" s="84"/>
       <c r="AB27" s="81"/>
       <c r="AC27" s="81"/>
-      <c r="AD27" s="98"/>
-      <c r="AE27" s="99"/>
-      <c r="AF27" s="100"/>
+      <c r="AD27" s="96"/>
+      <c r="AE27" s="97"/>
+      <c r="AF27" s="98"/>
       <c r="AG27" s="10"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
@@ -2518,7 +2517,7 @@
       <c r="L28" s="83"/>
       <c r="M28" s="81"/>
       <c r="N28" s="81"/>
-      <c r="O28" s="117"/>
+      <c r="O28" s="115"/>
       <c r="P28" s="81"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="82"/>
@@ -2533,9 +2532,9 @@
       <c r="AA28" s="84"/>
       <c r="AB28" s="81"/>
       <c r="AC28" s="81"/>
-      <c r="AD28" s="98"/>
-      <c r="AE28" s="99"/>
-      <c r="AF28" s="100"/>
+      <c r="AD28" s="96"/>
+      <c r="AE28" s="97"/>
+      <c r="AF28" s="98"/>
       <c r="AG28" s="10"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.35">
@@ -2555,7 +2554,7 @@
       <c r="L29" s="83"/>
       <c r="M29" s="81"/>
       <c r="N29" s="81"/>
-      <c r="O29" s="117"/>
+      <c r="O29" s="115"/>
       <c r="P29" s="81"/>
       <c r="Q29" s="81"/>
       <c r="R29" s="82"/>
@@ -2570,9 +2569,9 @@
       <c r="AA29" s="84"/>
       <c r="AB29" s="81"/>
       <c r="AC29" s="81"/>
-      <c r="AD29" s="98"/>
-      <c r="AE29" s="99"/>
-      <c r="AF29" s="100"/>
+      <c r="AD29" s="96"/>
+      <c r="AE29" s="97"/>
+      <c r="AF29" s="98"/>
       <c r="AG29" s="10"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
@@ -2607,9 +2606,9 @@
       <c r="AA30" s="84"/>
       <c r="AB30" s="81"/>
       <c r="AC30" s="81"/>
-      <c r="AD30" s="98"/>
-      <c r="AE30" s="99"/>
-      <c r="AF30" s="100"/>
+      <c r="AD30" s="96"/>
+      <c r="AE30" s="97"/>
+      <c r="AF30" s="98"/>
       <c r="AG30" s="10"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
@@ -2644,8 +2643,8 @@
       <c r="AA31" s="66"/>
       <c r="AB31" s="63"/>
       <c r="AC31" s="63"/>
-      <c r="AD31" s="104"/>
-      <c r="AE31" s="105"/>
+      <c r="AD31" s="102"/>
+      <c r="AE31" s="103"/>
       <c r="AF31" s="56"/>
       <c r="AG31" s="10"/>
     </row>
@@ -2681,9 +2680,9 @@
       <c r="AA32" s="76"/>
       <c r="AB32" s="74"/>
       <c r="AC32" s="74"/>
-      <c r="AD32" s="95"/>
-      <c r="AE32" s="96"/>
-      <c r="AF32" s="97"/>
+      <c r="AD32" s="93"/>
+      <c r="AE32" s="94"/>
+      <c r="AF32" s="95"/>
       <c r="AG32" s="10"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
@@ -2718,9 +2717,9 @@
       <c r="AA33" s="84"/>
       <c r="AB33" s="81"/>
       <c r="AC33" s="81"/>
-      <c r="AD33" s="98"/>
-      <c r="AE33" s="99"/>
-      <c r="AF33" s="100"/>
+      <c r="AD33" s="96"/>
+      <c r="AE33" s="97"/>
+      <c r="AF33" s="98"/>
       <c r="AG33" s="10"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.35">
@@ -2755,9 +2754,9 @@
       <c r="AA34" s="84"/>
       <c r="AB34" s="81"/>
       <c r="AC34" s="81"/>
-      <c r="AD34" s="98"/>
-      <c r="AE34" s="99"/>
-      <c r="AF34" s="100"/>
+      <c r="AD34" s="96"/>
+      <c r="AE34" s="97"/>
+      <c r="AF34" s="98"/>
       <c r="AG34" s="10"/>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.35">
@@ -2792,9 +2791,9 @@
       <c r="AA35" s="84"/>
       <c r="AB35" s="81"/>
       <c r="AC35" s="81"/>
-      <c r="AD35" s="98"/>
-      <c r="AE35" s="99"/>
-      <c r="AF35" s="100"/>
+      <c r="AD35" s="96"/>
+      <c r="AE35" s="97"/>
+      <c r="AF35" s="98"/>
       <c r="AG35" s="10"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.35">
@@ -2831,9 +2830,9 @@
       <c r="AA36" s="84"/>
       <c r="AB36" s="81"/>
       <c r="AC36" s="81"/>
-      <c r="AD36" s="98"/>
-      <c r="AE36" s="99"/>
-      <c r="AF36" s="100"/>
+      <c r="AD36" s="96"/>
+      <c r="AE36" s="97"/>
+      <c r="AF36" s="98"/>
       <c r="AG36" s="10"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.35">
@@ -2856,7 +2855,7 @@
       <c r="O37" s="81"/>
       <c r="P37" s="81"/>
       <c r="Q37" s="81"/>
-      <c r="R37" s="118"/>
+      <c r="R37" s="116"/>
       <c r="S37" s="83"/>
       <c r="T37" s="81"/>
       <c r="U37" s="84"/>
@@ -2868,9 +2867,9 @@
       <c r="AA37" s="84"/>
       <c r="AB37" s="81"/>
       <c r="AC37" s="81"/>
-      <c r="AD37" s="98"/>
-      <c r="AE37" s="99"/>
-      <c r="AF37" s="100"/>
+      <c r="AD37" s="96"/>
+      <c r="AE37" s="97"/>
+      <c r="AF37" s="98"/>
       <c r="AG37" s="10"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.35">
@@ -2893,7 +2892,7 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
       <c r="Q38" s="61"/>
-      <c r="R38" s="119"/>
+      <c r="R38" s="117"/>
       <c r="S38" s="59"/>
       <c r="T38" s="61"/>
       <c r="U38" s="65"/>
@@ -2905,8 +2904,8 @@
       <c r="AA38" s="65"/>
       <c r="AB38" s="61"/>
       <c r="AC38" s="61"/>
-      <c r="AD38" s="106"/>
-      <c r="AE38" s="107"/>
+      <c r="AD38" s="104"/>
+      <c r="AE38" s="105"/>
       <c r="AF38" s="55"/>
       <c r="AG38" s="10"/>
     </row>
@@ -2940,8 +2939,8 @@
       <c r="AA39" s="66"/>
       <c r="AB39" s="63"/>
       <c r="AC39" s="63"/>
-      <c r="AD39" s="104"/>
-      <c r="AE39" s="105"/>
+      <c r="AD39" s="102"/>
+      <c r="AE39" s="103"/>
       <c r="AF39" s="56"/>
       <c r="AG39" s="10"/>
     </row>
@@ -2977,9 +2976,9 @@
       <c r="AA40" s="76"/>
       <c r="AB40" s="74"/>
       <c r="AC40" s="74"/>
-      <c r="AD40" s="95"/>
-      <c r="AE40" s="96"/>
-      <c r="AF40" s="97"/>
+      <c r="AD40" s="93"/>
+      <c r="AE40" s="94"/>
+      <c r="AF40" s="95"/>
       <c r="AG40" s="10"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.35">
@@ -3014,9 +3013,9 @@
       <c r="AA41" s="84"/>
       <c r="AB41" s="81"/>
       <c r="AC41" s="81"/>
-      <c r="AD41" s="98"/>
-      <c r="AE41" s="99"/>
-      <c r="AF41" s="100"/>
+      <c r="AD41" s="96"/>
+      <c r="AE41" s="97"/>
+      <c r="AF41" s="98"/>
       <c r="AG41" s="10"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.35">
@@ -3049,9 +3048,9 @@
       <c r="AA42" s="84"/>
       <c r="AB42" s="81"/>
       <c r="AC42" s="81"/>
-      <c r="AD42" s="98"/>
-      <c r="AE42" s="99"/>
-      <c r="AF42" s="100"/>
+      <c r="AD42" s="96"/>
+      <c r="AE42" s="97"/>
+      <c r="AF42" s="98"/>
       <c r="AG42" s="10"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.35">
@@ -3086,9 +3085,9 @@
       <c r="AA43" s="84"/>
       <c r="AB43" s="81"/>
       <c r="AC43" s="81"/>
-      <c r="AD43" s="98"/>
-      <c r="AE43" s="99"/>
-      <c r="AF43" s="100"/>
+      <c r="AD43" s="96"/>
+      <c r="AE43" s="97"/>
+      <c r="AF43" s="98"/>
       <c r="AG43" s="10"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.35">
@@ -3116,7 +3115,9 @@
       <c r="T44" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="U44" s="85"/>
+      <c r="U44" s="85">
+        <v>1</v>
+      </c>
       <c r="V44" s="81"/>
       <c r="W44" s="81"/>
       <c r="X44" s="81"/>
@@ -3125,9 +3126,9 @@
       <c r="AA44" s="84"/>
       <c r="AB44" s="81"/>
       <c r="AC44" s="81"/>
-      <c r="AD44" s="98"/>
-      <c r="AE44" s="99"/>
-      <c r="AF44" s="100"/>
+      <c r="AD44" s="96"/>
+      <c r="AE44" s="97"/>
+      <c r="AF44" s="98"/>
       <c r="AG44" s="10"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
@@ -3162,9 +3163,9 @@
       <c r="AA45" s="84"/>
       <c r="AB45" s="81"/>
       <c r="AC45" s="81"/>
-      <c r="AD45" s="98"/>
-      <c r="AE45" s="99"/>
-      <c r="AF45" s="100"/>
+      <c r="AD45" s="96"/>
+      <c r="AE45" s="97"/>
+      <c r="AF45" s="98"/>
       <c r="AG45" s="10"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.35">
@@ -3194,7 +3195,9 @@
       <c r="R46" s="82"/>
       <c r="S46" s="83"/>
       <c r="T46" s="81"/>
-      <c r="U46" s="85"/>
+      <c r="U46" s="115">
+        <v>1</v>
+      </c>
       <c r="V46" s="81"/>
       <c r="W46" s="81"/>
       <c r="X46" s="81"/>
@@ -3203,9 +3206,9 @@
       <c r="AA46" s="84"/>
       <c r="AB46" s="81"/>
       <c r="AC46" s="81"/>
-      <c r="AD46" s="98"/>
-      <c r="AE46" s="99"/>
-      <c r="AF46" s="100"/>
+      <c r="AD46" s="96"/>
+      <c r="AE46" s="97"/>
+      <c r="AF46" s="98"/>
       <c r="AG46" s="10"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.35">
@@ -3240,9 +3243,9 @@
       <c r="AA47" s="84"/>
       <c r="AB47" s="81"/>
       <c r="AC47" s="81"/>
-      <c r="AD47" s="98"/>
-      <c r="AE47" s="99"/>
-      <c r="AF47" s="100"/>
+      <c r="AD47" s="96"/>
+      <c r="AE47" s="97"/>
+      <c r="AF47" s="98"/>
       <c r="AG47" s="10"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.35">
@@ -3279,9 +3282,9 @@
       <c r="AA48" s="84"/>
       <c r="AB48" s="81"/>
       <c r="AC48" s="81"/>
-      <c r="AD48" s="98"/>
-      <c r="AE48" s="99"/>
-      <c r="AF48" s="100"/>
+      <c r="AD48" s="96"/>
+      <c r="AE48" s="97"/>
+      <c r="AF48" s="98"/>
       <c r="AG48" s="10"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.35">
@@ -3306,7 +3309,9 @@
       <c r="Q49" s="81"/>
       <c r="R49" s="82"/>
       <c r="S49" s="83"/>
-      <c r="T49" s="89"/>
+      <c r="T49" s="89">
+        <v>1</v>
+      </c>
       <c r="U49" s="84"/>
       <c r="V49" s="81"/>
       <c r="W49" s="81"/>
@@ -3316,9 +3321,9 @@
       <c r="AA49" s="84"/>
       <c r="AB49" s="81"/>
       <c r="AC49" s="81"/>
-      <c r="AD49" s="98"/>
-      <c r="AE49" s="99"/>
-      <c r="AF49" s="100"/>
+      <c r="AD49" s="96"/>
+      <c r="AE49" s="97"/>
+      <c r="AF49" s="98"/>
       <c r="AG49" s="10"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.35">
@@ -3347,7 +3352,9 @@
       <c r="U50" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="V50" s="90"/>
+      <c r="V50" s="115">
+        <v>1</v>
+      </c>
       <c r="W50" s="81"/>
       <c r="X50" s="81"/>
       <c r="Y50" s="82"/>
@@ -3355,9 +3362,9 @@
       <c r="AA50" s="84"/>
       <c r="AB50" s="81"/>
       <c r="AC50" s="81"/>
-      <c r="AD50" s="98"/>
-      <c r="AE50" s="99"/>
-      <c r="AF50" s="100"/>
+      <c r="AD50" s="96"/>
+      <c r="AE50" s="97"/>
+      <c r="AF50" s="98"/>
       <c r="AG50" s="10"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.35">
@@ -3392,9 +3399,9 @@
       <c r="AA51" s="84"/>
       <c r="AB51" s="81"/>
       <c r="AC51" s="81"/>
-      <c r="AD51" s="98"/>
-      <c r="AE51" s="99"/>
-      <c r="AF51" s="100"/>
+      <c r="AD51" s="96"/>
+      <c r="AE51" s="97"/>
+      <c r="AF51" s="98"/>
       <c r="AG51" s="10"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.35">
@@ -3429,8 +3436,8 @@
       <c r="AA52" s="65"/>
       <c r="AB52" s="61"/>
       <c r="AC52" s="61"/>
-      <c r="AD52" s="106"/>
-      <c r="AE52" s="107"/>
+      <c r="AD52" s="104"/>
+      <c r="AE52" s="105"/>
       <c r="AF52" s="55"/>
       <c r="AG52" s="10"/>
     </row>
@@ -3464,8 +3471,8 @@
       <c r="AA53" s="65"/>
       <c r="AB53" s="61"/>
       <c r="AC53" s="61"/>
-      <c r="AD53" s="106"/>
-      <c r="AE53" s="107"/>
+      <c r="AD53" s="104"/>
+      <c r="AE53" s="105"/>
       <c r="AF53" s="55"/>
       <c r="AG53" s="10"/>
     </row>
@@ -3499,8 +3506,8 @@
       <c r="AA54" s="66"/>
       <c r="AB54" s="63"/>
       <c r="AC54" s="63"/>
-      <c r="AD54" s="104"/>
-      <c r="AE54" s="105"/>
+      <c r="AD54" s="102"/>
+      <c r="AE54" s="103"/>
       <c r="AF54" s="56"/>
       <c r="AG54" s="10"/>
     </row>
@@ -3534,9 +3541,9 @@
       <c r="AA55" s="76"/>
       <c r="AB55" s="74"/>
       <c r="AC55" s="74"/>
-      <c r="AD55" s="95"/>
-      <c r="AE55" s="96"/>
-      <c r="AF55" s="97"/>
+      <c r="AD55" s="93"/>
+      <c r="AE55" s="94"/>
+      <c r="AF55" s="95"/>
       <c r="AG55" s="10"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.35">
@@ -3571,9 +3578,9 @@
       <c r="AA56" s="84"/>
       <c r="AB56" s="81"/>
       <c r="AC56" s="81"/>
-      <c r="AD56" s="98"/>
-      <c r="AE56" s="99"/>
-      <c r="AF56" s="100"/>
+      <c r="AD56" s="96"/>
+      <c r="AE56" s="97"/>
+      <c r="AF56" s="98"/>
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.35">
@@ -3612,9 +3619,9 @@
       <c r="AA57" s="84"/>
       <c r="AB57" s="81"/>
       <c r="AC57" s="81"/>
-      <c r="AD57" s="98"/>
-      <c r="AE57" s="99"/>
-      <c r="AF57" s="100"/>
+      <c r="AD57" s="96"/>
+      <c r="AE57" s="97"/>
+      <c r="AF57" s="98"/>
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.35">
@@ -3649,9 +3656,9 @@
       <c r="AA58" s="84"/>
       <c r="AB58" s="81"/>
       <c r="AC58" s="81"/>
-      <c r="AD58" s="98"/>
-      <c r="AE58" s="99"/>
-      <c r="AF58" s="100"/>
+      <c r="AD58" s="96"/>
+      <c r="AE58" s="97"/>
+      <c r="AF58" s="98"/>
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.35">
@@ -3684,9 +3691,9 @@
       <c r="AA59" s="84"/>
       <c r="AB59" s="81"/>
       <c r="AC59" s="81"/>
-      <c r="AD59" s="98"/>
-      <c r="AE59" s="99"/>
-      <c r="AF59" s="100"/>
+      <c r="AD59" s="96"/>
+      <c r="AE59" s="97"/>
+      <c r="AF59" s="98"/>
       <c r="AG59" s="10"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.35">
@@ -3719,8 +3726,8 @@
       <c r="AA60" s="66"/>
       <c r="AB60" s="63"/>
       <c r="AC60" s="63"/>
-      <c r="AD60" s="104"/>
-      <c r="AE60" s="105"/>
+      <c r="AD60" s="102"/>
+      <c r="AE60" s="103"/>
       <c r="AF60" s="56"/>
       <c r="AG60" s="10"/>
     </row>
@@ -3754,9 +3761,9 @@
       <c r="AA61" s="76"/>
       <c r="AB61" s="74"/>
       <c r="AC61" s="74"/>
-      <c r="AD61" s="95"/>
-      <c r="AE61" s="96"/>
-      <c r="AF61" s="97"/>
+      <c r="AD61" s="93"/>
+      <c r="AE61" s="94"/>
+      <c r="AF61" s="95"/>
       <c r="AG61" s="10"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.35">
@@ -3791,9 +3798,9 @@
       <c r="AA62" s="84"/>
       <c r="AB62" s="81"/>
       <c r="AC62" s="81"/>
-      <c r="AD62" s="98"/>
-      <c r="AE62" s="99"/>
-      <c r="AF62" s="100"/>
+      <c r="AD62" s="96"/>
+      <c r="AE62" s="97"/>
+      <c r="AF62" s="98"/>
       <c r="AG62" s="10"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.35">
@@ -3830,9 +3837,9 @@
       <c r="AA63" s="84"/>
       <c r="AB63" s="81"/>
       <c r="AC63" s="81"/>
-      <c r="AD63" s="98"/>
-      <c r="AE63" s="99"/>
-      <c r="AF63" s="100"/>
+      <c r="AD63" s="96"/>
+      <c r="AE63" s="97"/>
+      <c r="AF63" s="98"/>
       <c r="AG63" s="10"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.35">
@@ -3865,9 +3872,9 @@
       <c r="AA64" s="84"/>
       <c r="AB64" s="81"/>
       <c r="AC64" s="81"/>
-      <c r="AD64" s="98"/>
-      <c r="AE64" s="99"/>
-      <c r="AF64" s="100"/>
+      <c r="AD64" s="96"/>
+      <c r="AE64" s="97"/>
+      <c r="AF64" s="98"/>
       <c r="AG64" s="10"/>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
@@ -3906,9 +3913,9 @@
       <c r="AA65" s="84"/>
       <c r="AB65" s="81"/>
       <c r="AC65" s="81"/>
-      <c r="AD65" s="98"/>
-      <c r="AE65" s="99"/>
-      <c r="AF65" s="100"/>
+      <c r="AD65" s="96"/>
+      <c r="AE65" s="97"/>
+      <c r="AF65" s="98"/>
       <c r="AG65" s="10"/>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
@@ -3938,14 +3945,16 @@
       <c r="V66" s="81"/>
       <c r="W66" s="81"/>
       <c r="X66" s="81"/>
-      <c r="Y66" s="91"/>
+      <c r="Y66" s="90">
+        <v>1</v>
+      </c>
       <c r="Z66" s="83"/>
       <c r="AA66" s="84"/>
       <c r="AB66" s="81"/>
       <c r="AC66" s="81"/>
-      <c r="AD66" s="98"/>
-      <c r="AE66" s="99"/>
-      <c r="AF66" s="100"/>
+      <c r="AD66" s="96"/>
+      <c r="AE66" s="97"/>
+      <c r="AF66" s="98"/>
       <c r="AG66" s="10"/>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
@@ -3978,9 +3987,9 @@
       <c r="AA67" s="69"/>
       <c r="AB67" s="68"/>
       <c r="AC67" s="68"/>
-      <c r="AD67" s="101"/>
-      <c r="AE67" s="102"/>
-      <c r="AF67" s="103"/>
+      <c r="AD67" s="99"/>
+      <c r="AE67" s="100"/>
+      <c r="AF67" s="101"/>
       <c r="AG67" s="10"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
@@ -4015,9 +4024,9 @@
       <c r="AA68" s="84"/>
       <c r="AB68" s="81"/>
       <c r="AC68" s="81"/>
-      <c r="AD68" s="98"/>
-      <c r="AE68" s="99"/>
-      <c r="AF68" s="100"/>
+      <c r="AD68" s="96"/>
+      <c r="AE68" s="97"/>
+      <c r="AF68" s="98"/>
       <c r="AG68" s="10"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
@@ -4052,9 +4061,9 @@
       <c r="AA69" s="84"/>
       <c r="AB69" s="81"/>
       <c r="AC69" s="81"/>
-      <c r="AD69" s="98"/>
-      <c r="AE69" s="99"/>
-      <c r="AF69" s="100"/>
+      <c r="AD69" s="96"/>
+      <c r="AE69" s="97"/>
+      <c r="AF69" s="98"/>
       <c r="AG69" s="10"/>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
@@ -4087,8 +4096,8 @@
       <c r="AA70" s="66"/>
       <c r="AB70" s="63"/>
       <c r="AC70" s="63"/>
-      <c r="AD70" s="104"/>
-      <c r="AE70" s="105"/>
+      <c r="AD70" s="102"/>
+      <c r="AE70" s="103"/>
       <c r="AF70" s="56"/>
       <c r="AG70" s="10"/>
     </row>
@@ -4124,9 +4133,9 @@
       <c r="AA71" s="76"/>
       <c r="AB71" s="74"/>
       <c r="AC71" s="74"/>
-      <c r="AD71" s="95"/>
-      <c r="AE71" s="96"/>
-      <c r="AF71" s="97"/>
+      <c r="AD71" s="93"/>
+      <c r="AE71" s="94"/>
+      <c r="AF71" s="95"/>
       <c r="AG71" s="10"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
@@ -4161,9 +4170,9 @@
       <c r="AA72" s="84"/>
       <c r="AB72" s="81"/>
       <c r="AC72" s="81"/>
-      <c r="AD72" s="98"/>
-      <c r="AE72" s="99"/>
-      <c r="AF72" s="100"/>
+      <c r="AD72" s="96"/>
+      <c r="AE72" s="97"/>
+      <c r="AF72" s="98"/>
       <c r="AG72" s="10"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
@@ -4198,9 +4207,9 @@
       <c r="AA73" s="84"/>
       <c r="AB73" s="81"/>
       <c r="AC73" s="81"/>
-      <c r="AD73" s="98"/>
-      <c r="AE73" s="99"/>
-      <c r="AF73" s="100"/>
+      <c r="AD73" s="96"/>
+      <c r="AE73" s="97"/>
+      <c r="AF73" s="98"/>
       <c r="AG73" s="10"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
@@ -4221,7 +4230,7 @@
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="39"/>
-      <c r="L74" s="120"/>
+      <c r="L74" s="118"/>
       <c r="M74" s="81"/>
       <c r="N74" s="81"/>
       <c r="O74" s="81"/>
@@ -4239,9 +4248,9 @@
       <c r="AA74" s="84"/>
       <c r="AB74" s="81"/>
       <c r="AC74" s="81"/>
-      <c r="AD74" s="111"/>
-      <c r="AE74" s="98"/>
-      <c r="AF74" s="100"/>
+      <c r="AD74" s="109"/>
+      <c r="AE74" s="96"/>
+      <c r="AF74" s="98"/>
       <c r="AG74" s="10"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
@@ -4264,21 +4273,21 @@
       <c r="O75" s="81"/>
       <c r="P75" s="81"/>
       <c r="Q75" s="81"/>
-      <c r="R75" s="92"/>
+      <c r="R75" s="91"/>
       <c r="S75" s="83"/>
       <c r="T75" s="81"/>
       <c r="U75" s="84"/>
       <c r="V75" s="81"/>
       <c r="W75" s="81"/>
       <c r="X75" s="81"/>
-      <c r="Y75" s="92"/>
+      <c r="Y75" s="91"/>
       <c r="Z75" s="83"/>
       <c r="AA75" s="84"/>
       <c r="AB75" s="81"/>
-      <c r="AC75" s="110"/>
-      <c r="AD75" s="112"/>
-      <c r="AE75" s="99"/>
-      <c r="AF75" s="92"/>
+      <c r="AC75" s="108"/>
+      <c r="AD75" s="110"/>
+      <c r="AE75" s="97"/>
+      <c r="AF75" s="91"/>
       <c r="AG75" s="10"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
@@ -4311,9 +4320,9 @@
       <c r="AA76" s="84"/>
       <c r="AB76" s="81"/>
       <c r="AC76" s="81"/>
-      <c r="AD76" s="101"/>
-      <c r="AE76" s="98"/>
-      <c r="AF76" s="109"/>
+      <c r="AD76" s="99"/>
+      <c r="AE76" s="96"/>
+      <c r="AF76" s="107"/>
       <c r="AG76" s="10"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
@@ -4348,9 +4357,9 @@
       <c r="AA77" s="84"/>
       <c r="AB77" s="81"/>
       <c r="AC77" s="81"/>
-      <c r="AD77" s="98"/>
-      <c r="AE77" s="111"/>
-      <c r="AF77" s="109"/>
+      <c r="AD77" s="96"/>
+      <c r="AE77" s="109"/>
+      <c r="AF77" s="107"/>
       <c r="AG77" s="10"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
@@ -4369,25 +4378,25 @@
       <c r="K78" s="70"/>
       <c r="L78" s="80"/>
       <c r="M78" s="85"/>
-      <c r="N78" s="117"/>
-      <c r="O78" s="117"/>
-      <c r="P78" s="117"/>
-      <c r="Q78" s="117"/>
-      <c r="R78" s="117"/>
-      <c r="S78" s="120"/>
+      <c r="N78" s="115"/>
+      <c r="O78" s="115"/>
+      <c r="P78" s="115"/>
+      <c r="Q78" s="115"/>
+      <c r="R78" s="115"/>
+      <c r="S78" s="118"/>
       <c r="T78" s="85"/>
-      <c r="U78" s="121"/>
+      <c r="U78" s="119"/>
       <c r="V78" s="85"/>
       <c r="W78" s="85"/>
       <c r="X78" s="85"/>
-      <c r="Y78" s="93"/>
+      <c r="Y78" s="120"/>
       <c r="Z78" s="80"/>
       <c r="AA78" s="85"/>
       <c r="AB78" s="85"/>
       <c r="AC78" s="85"/>
-      <c r="AD78" s="116"/>
+      <c r="AD78" s="114"/>
       <c r="AE78" s="57"/>
-      <c r="AF78" s="92"/>
+      <c r="AF78" s="91"/>
       <c r="AG78" s="10"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
@@ -4420,9 +4429,9 @@
       <c r="AA79" s="63"/>
       <c r="AB79" s="63"/>
       <c r="AC79" s="63"/>
-      <c r="AD79" s="114"/>
-      <c r="AE79" s="104"/>
-      <c r="AF79" s="115"/>
+      <c r="AD79" s="112"/>
+      <c r="AE79" s="102"/>
+      <c r="AF79" s="113"/>
       <c r="AG79" s="10"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
@@ -4447,21 +4456,21 @@
       <c r="O80" s="74"/>
       <c r="P80" s="74"/>
       <c r="Q80" s="74"/>
-      <c r="R80" s="94"/>
+      <c r="R80" s="92"/>
       <c r="S80" s="76"/>
       <c r="T80" s="74"/>
       <c r="U80" s="74"/>
       <c r="V80" s="74"/>
       <c r="W80" s="74"/>
       <c r="X80" s="74"/>
-      <c r="Y80" s="94"/>
+      <c r="Y80" s="92"/>
       <c r="Z80" s="76"/>
       <c r="AA80" s="74"/>
       <c r="AB80" s="74"/>
       <c r="AC80" s="74"/>
-      <c r="AD80" s="101"/>
-      <c r="AE80" s="101"/>
-      <c r="AF80" s="113"/>
+      <c r="AD80" s="99"/>
+      <c r="AE80" s="99"/>
+      <c r="AF80" s="111"/>
       <c r="AG80" s="10"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
@@ -4498,9 +4507,9 @@
       <c r="AA81" s="67"/>
       <c r="AB81" s="67"/>
       <c r="AC81" s="63"/>
-      <c r="AD81" s="114"/>
-      <c r="AE81" s="114"/>
-      <c r="AF81" s="115"/>
+      <c r="AD81" s="112"/>
+      <c r="AE81" s="112"/>
+      <c r="AF81" s="113"/>
       <c r="AG81" s="10"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
@@ -4596,13 +4605,13 @@
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C89" s="108"/>
+      <c r="C89" s="106"/>
       <c r="D89" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C90" s="112"/>
+      <c r="C90" s="110"/>
       <c r="D90" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Animacion de Marceline y la roca del easter egg
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195A88F9-45D6-450D-9F74-22113D6B1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E260C64E-8F99-4AA1-8A0C-927202B2C339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="T49" sqref="T48:T49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="AI45" sqref="AI45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3115,7 +3115,7 @@
       <c r="T44" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="U44" s="85">
+      <c r="U44" s="115">
         <v>1</v>
       </c>
       <c r="V44" s="81"/>

</xml_diff>

<commit_message>
Luces puntuales y direccional para ciclo dia-noche
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E260C64E-8F99-4AA1-8A0C-927202B2C339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F0F2E-70EC-4E4A-BC15-0AD43D5C28B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -1043,7 +1043,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1074,6 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="AI45" sqref="AI45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="X69" sqref="G69:X69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1716,9 +1716,9 @@
       <c r="AA6" s="76"/>
       <c r="AB6" s="74"/>
       <c r="AC6" s="74"/>
-      <c r="AD6" s="93"/>
-      <c r="AE6" s="94"/>
-      <c r="AF6" s="95"/>
+      <c r="AD6" s="92"/>
+      <c r="AE6" s="93"/>
+      <c r="AF6" s="94"/>
       <c r="AG6" s="10"/>
     </row>
     <row r="7" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1753,9 +1753,9 @@
       <c r="AA7" s="84"/>
       <c r="AB7" s="81"/>
       <c r="AC7" s="85"/>
-      <c r="AD7" s="96"/>
-      <c r="AE7" s="97"/>
-      <c r="AF7" s="98"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="97"/>
       <c r="AG7" s="10"/>
     </row>
     <row r="8" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1790,9 +1790,9 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="68"/>
       <c r="AC8" s="79"/>
-      <c r="AD8" s="99"/>
-      <c r="AE8" s="100"/>
-      <c r="AF8" s="101"/>
+      <c r="AD8" s="98"/>
+      <c r="AE8" s="99"/>
+      <c r="AF8" s="100"/>
       <c r="AG8" s="10"/>
     </row>
     <row r="9" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1827,9 +1827,9 @@
       <c r="AA9" s="84"/>
       <c r="AB9" s="81"/>
       <c r="AC9" s="81"/>
-      <c r="AD9" s="96"/>
-      <c r="AE9" s="97"/>
-      <c r="AF9" s="98"/>
+      <c r="AD9" s="95"/>
+      <c r="AE9" s="96"/>
+      <c r="AF9" s="97"/>
       <c r="AG9" s="10"/>
     </row>
     <row r="10" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1862,9 +1862,9 @@
       <c r="AA10" s="84"/>
       <c r="AB10" s="81"/>
       <c r="AC10" s="81"/>
-      <c r="AD10" s="96"/>
-      <c r="AE10" s="97"/>
-      <c r="AF10" s="98"/>
+      <c r="AD10" s="95"/>
+      <c r="AE10" s="96"/>
+      <c r="AF10" s="97"/>
       <c r="AG10" s="10"/>
     </row>
     <row r="11" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1899,9 +1899,9 @@
       <c r="AA11" s="84"/>
       <c r="AB11" s="81"/>
       <c r="AC11" s="81"/>
-      <c r="AD11" s="96"/>
-      <c r="AE11" s="97"/>
-      <c r="AF11" s="98"/>
+      <c r="AD11" s="95"/>
+      <c r="AE11" s="96"/>
+      <c r="AF11" s="97"/>
       <c r="AG11" s="10"/>
     </row>
     <row r="12" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1936,9 +1936,9 @@
       <c r="AA12" s="84"/>
       <c r="AB12" s="81"/>
       <c r="AC12" s="81"/>
-      <c r="AD12" s="96"/>
-      <c r="AE12" s="97"/>
-      <c r="AF12" s="98"/>
+      <c r="AD12" s="95"/>
+      <c r="AE12" s="96"/>
+      <c r="AF12" s="97"/>
       <c r="AG12" s="10"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
@@ -1973,9 +1973,9 @@
       <c r="AA13" s="84"/>
       <c r="AB13" s="81"/>
       <c r="AC13" s="81"/>
-      <c r="AD13" s="96"/>
-      <c r="AE13" s="97"/>
-      <c r="AF13" s="98"/>
+      <c r="AD13" s="95"/>
+      <c r="AE13" s="96"/>
+      <c r="AF13" s="97"/>
       <c r="AG13" s="10"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
@@ -2008,9 +2008,9 @@
       <c r="AA14" s="84"/>
       <c r="AB14" s="81"/>
       <c r="AC14" s="81"/>
-      <c r="AD14" s="96"/>
-      <c r="AE14" s="97"/>
-      <c r="AF14" s="98"/>
+      <c r="AD14" s="95"/>
+      <c r="AE14" s="96"/>
+      <c r="AF14" s="97"/>
       <c r="AG14" s="10"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
@@ -2045,9 +2045,9 @@
       <c r="AA15" s="84"/>
       <c r="AB15" s="81"/>
       <c r="AC15" s="81"/>
-      <c r="AD15" s="96"/>
-      <c r="AE15" s="97"/>
-      <c r="AF15" s="98"/>
+      <c r="AD15" s="95"/>
+      <c r="AE15" s="96"/>
+      <c r="AF15" s="97"/>
       <c r="AG15" s="10"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
@@ -2084,9 +2084,9 @@
       <c r="AA16" s="84"/>
       <c r="AB16" s="81"/>
       <c r="AC16" s="81"/>
-      <c r="AD16" s="96"/>
-      <c r="AE16" s="97"/>
-      <c r="AF16" s="98"/>
+      <c r="AD16" s="95"/>
+      <c r="AE16" s="96"/>
+      <c r="AF16" s="97"/>
       <c r="AG16" s="10"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
@@ -2104,7 +2104,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="39"/>
       <c r="L17" s="83"/>
-      <c r="M17" s="115"/>
+      <c r="M17" s="114"/>
       <c r="N17" s="81"/>
       <c r="O17" s="81"/>
       <c r="P17" s="81"/>
@@ -2121,9 +2121,9 @@
       <c r="AA17" s="84"/>
       <c r="AB17" s="81"/>
       <c r="AC17" s="81"/>
-      <c r="AD17" s="96"/>
-      <c r="AE17" s="97"/>
-      <c r="AF17" s="98"/>
+      <c r="AD17" s="95"/>
+      <c r="AE17" s="96"/>
+      <c r="AF17" s="97"/>
       <c r="AG17" s="10"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
@@ -2143,7 +2143,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="39"/>
       <c r="L18" s="83"/>
-      <c r="M18" s="115"/>
+      <c r="M18" s="114"/>
       <c r="N18" s="81"/>
       <c r="O18" s="81"/>
       <c r="P18" s="81"/>
@@ -2160,9 +2160,9 @@
       <c r="AA18" s="84"/>
       <c r="AB18" s="81"/>
       <c r="AC18" s="81"/>
-      <c r="AD18" s="96"/>
-      <c r="AE18" s="97"/>
-      <c r="AF18" s="98"/>
+      <c r="AD18" s="95"/>
+      <c r="AE18" s="96"/>
+      <c r="AF18" s="97"/>
       <c r="AG18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.35">
@@ -2180,7 +2180,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="39"/>
       <c r="L19" s="83"/>
-      <c r="M19" s="115"/>
+      <c r="M19" s="114"/>
       <c r="N19" s="81"/>
       <c r="O19" s="81"/>
       <c r="P19" s="81"/>
@@ -2197,9 +2197,9 @@
       <c r="AA19" s="84"/>
       <c r="AB19" s="81"/>
       <c r="AC19" s="81"/>
-      <c r="AD19" s="96"/>
-      <c r="AE19" s="97"/>
-      <c r="AF19" s="98"/>
+      <c r="AD19" s="95"/>
+      <c r="AE19" s="96"/>
+      <c r="AF19" s="97"/>
       <c r="AG19" s="10"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
@@ -2234,9 +2234,9 @@
       <c r="AA20" s="84"/>
       <c r="AB20" s="81"/>
       <c r="AC20" s="81"/>
-      <c r="AD20" s="96"/>
-      <c r="AE20" s="97"/>
-      <c r="AF20" s="98"/>
+      <c r="AD20" s="95"/>
+      <c r="AE20" s="96"/>
+      <c r="AF20" s="97"/>
       <c r="AG20" s="10"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
@@ -2257,7 +2257,7 @@
       <c r="K21" s="39"/>
       <c r="L21" s="83"/>
       <c r="M21" s="81"/>
-      <c r="N21" s="115"/>
+      <c r="N21" s="114"/>
       <c r="O21" s="81"/>
       <c r="P21" s="81"/>
       <c r="Q21" s="81"/>
@@ -2273,9 +2273,9 @@
       <c r="AA21" s="84"/>
       <c r="AB21" s="81"/>
       <c r="AC21" s="81"/>
-      <c r="AD21" s="96"/>
-      <c r="AE21" s="97"/>
-      <c r="AF21" s="98"/>
+      <c r="AD21" s="95"/>
+      <c r="AE21" s="96"/>
+      <c r="AF21" s="97"/>
       <c r="AG21" s="10"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
@@ -2294,7 +2294,7 @@
       <c r="K22" s="39"/>
       <c r="L22" s="83"/>
       <c r="M22" s="81"/>
-      <c r="N22" s="115"/>
+      <c r="N22" s="114"/>
       <c r="O22" s="81"/>
       <c r="P22" s="81"/>
       <c r="Q22" s="81"/>
@@ -2310,9 +2310,9 @@
       <c r="AA22" s="84"/>
       <c r="AB22" s="81"/>
       <c r="AC22" s="81"/>
-      <c r="AD22" s="96"/>
-      <c r="AE22" s="97"/>
-      <c r="AF22" s="98"/>
+      <c r="AD22" s="95"/>
+      <c r="AE22" s="96"/>
+      <c r="AF22" s="97"/>
       <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
@@ -2331,7 +2331,7 @@
       <c r="K23" s="39"/>
       <c r="L23" s="83"/>
       <c r="M23" s="81"/>
-      <c r="N23" s="115"/>
+      <c r="N23" s="114"/>
       <c r="O23" s="81"/>
       <c r="P23" s="81"/>
       <c r="Q23" s="81"/>
@@ -2347,9 +2347,9 @@
       <c r="AA23" s="84"/>
       <c r="AB23" s="81"/>
       <c r="AC23" s="81"/>
-      <c r="AD23" s="96"/>
-      <c r="AE23" s="97"/>
-      <c r="AF23" s="98"/>
+      <c r="AD23" s="95"/>
+      <c r="AE23" s="96"/>
+      <c r="AF23" s="97"/>
       <c r="AG23" s="10"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
@@ -2368,7 +2368,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="83"/>
       <c r="M24" s="81"/>
-      <c r="N24" s="115"/>
+      <c r="N24" s="114"/>
       <c r="O24" s="81"/>
       <c r="P24" s="81"/>
       <c r="Q24" s="81"/>
@@ -2384,9 +2384,9 @@
       <c r="AA24" s="84"/>
       <c r="AB24" s="81"/>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="96"/>
-      <c r="AE24" s="97"/>
-      <c r="AF24" s="98"/>
+      <c r="AD24" s="95"/>
+      <c r="AE24" s="96"/>
+      <c r="AF24" s="97"/>
       <c r="AG24" s="10"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
@@ -2406,7 +2406,7 @@
       <c r="L25" s="83"/>
       <c r="M25" s="81"/>
       <c r="N25" s="81"/>
-      <c r="O25" s="115"/>
+      <c r="O25" s="114"/>
       <c r="P25" s="81"/>
       <c r="Q25" s="81"/>
       <c r="R25" s="82"/>
@@ -2421,9 +2421,9 @@
       <c r="AA25" s="84"/>
       <c r="AB25" s="81"/>
       <c r="AC25" s="81"/>
-      <c r="AD25" s="96"/>
-      <c r="AE25" s="97"/>
-      <c r="AF25" s="98"/>
+      <c r="AD25" s="95"/>
+      <c r="AE25" s="96"/>
+      <c r="AF25" s="97"/>
       <c r="AG25" s="10"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
@@ -2443,7 +2443,7 @@
       <c r="L26" s="83"/>
       <c r="M26" s="81"/>
       <c r="N26" s="81"/>
-      <c r="O26" s="115"/>
+      <c r="O26" s="114"/>
       <c r="P26" s="81"/>
       <c r="Q26" s="81"/>
       <c r="R26" s="82"/>
@@ -2458,9 +2458,9 @@
       <c r="AA26" s="84"/>
       <c r="AB26" s="81"/>
       <c r="AC26" s="81"/>
-      <c r="AD26" s="96"/>
-      <c r="AE26" s="97"/>
-      <c r="AF26" s="98"/>
+      <c r="AD26" s="95"/>
+      <c r="AE26" s="96"/>
+      <c r="AF26" s="97"/>
       <c r="AG26" s="10"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
@@ -2480,7 +2480,7 @@
       <c r="L27" s="83"/>
       <c r="M27" s="81"/>
       <c r="N27" s="81"/>
-      <c r="O27" s="115"/>
+      <c r="O27" s="114"/>
       <c r="P27" s="81"/>
       <c r="Q27" s="81"/>
       <c r="R27" s="82"/>
@@ -2495,9 +2495,9 @@
       <c r="AA27" s="84"/>
       <c r="AB27" s="81"/>
       <c r="AC27" s="81"/>
-      <c r="AD27" s="96"/>
-      <c r="AE27" s="97"/>
-      <c r="AF27" s="98"/>
+      <c r="AD27" s="95"/>
+      <c r="AE27" s="96"/>
+      <c r="AF27" s="97"/>
       <c r="AG27" s="10"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
@@ -2517,7 +2517,7 @@
       <c r="L28" s="83"/>
       <c r="M28" s="81"/>
       <c r="N28" s="81"/>
-      <c r="O28" s="115"/>
+      <c r="O28" s="114"/>
       <c r="P28" s="81"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="82"/>
@@ -2532,9 +2532,9 @@
       <c r="AA28" s="84"/>
       <c r="AB28" s="81"/>
       <c r="AC28" s="81"/>
-      <c r="AD28" s="96"/>
-      <c r="AE28" s="97"/>
-      <c r="AF28" s="98"/>
+      <c r="AD28" s="95"/>
+      <c r="AE28" s="96"/>
+      <c r="AF28" s="97"/>
       <c r="AG28" s="10"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.35">
@@ -2554,7 +2554,7 @@
       <c r="L29" s="83"/>
       <c r="M29" s="81"/>
       <c r="N29" s="81"/>
-      <c r="O29" s="115"/>
+      <c r="O29" s="114"/>
       <c r="P29" s="81"/>
       <c r="Q29" s="81"/>
       <c r="R29" s="82"/>
@@ -2569,9 +2569,9 @@
       <c r="AA29" s="84"/>
       <c r="AB29" s="81"/>
       <c r="AC29" s="81"/>
-      <c r="AD29" s="96"/>
-      <c r="AE29" s="97"/>
-      <c r="AF29" s="98"/>
+      <c r="AD29" s="95"/>
+      <c r="AE29" s="96"/>
+      <c r="AF29" s="97"/>
       <c r="AG29" s="10"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
@@ -2606,9 +2606,9 @@
       <c r="AA30" s="84"/>
       <c r="AB30" s="81"/>
       <c r="AC30" s="81"/>
-      <c r="AD30" s="96"/>
-      <c r="AE30" s="97"/>
-      <c r="AF30" s="98"/>
+      <c r="AD30" s="95"/>
+      <c r="AE30" s="96"/>
+      <c r="AF30" s="97"/>
       <c r="AG30" s="10"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
@@ -2643,8 +2643,8 @@
       <c r="AA31" s="66"/>
       <c r="AB31" s="63"/>
       <c r="AC31" s="63"/>
-      <c r="AD31" s="102"/>
-      <c r="AE31" s="103"/>
+      <c r="AD31" s="101"/>
+      <c r="AE31" s="102"/>
       <c r="AF31" s="56"/>
       <c r="AG31" s="10"/>
     </row>
@@ -2680,9 +2680,9 @@
       <c r="AA32" s="76"/>
       <c r="AB32" s="74"/>
       <c r="AC32" s="74"/>
-      <c r="AD32" s="93"/>
-      <c r="AE32" s="94"/>
-      <c r="AF32" s="95"/>
+      <c r="AD32" s="92"/>
+      <c r="AE32" s="93"/>
+      <c r="AF32" s="94"/>
       <c r="AG32" s="10"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
@@ -2717,9 +2717,9 @@
       <c r="AA33" s="84"/>
       <c r="AB33" s="81"/>
       <c r="AC33" s="81"/>
-      <c r="AD33" s="96"/>
-      <c r="AE33" s="97"/>
-      <c r="AF33" s="98"/>
+      <c r="AD33" s="95"/>
+      <c r="AE33" s="96"/>
+      <c r="AF33" s="97"/>
       <c r="AG33" s="10"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.35">
@@ -2754,9 +2754,9 @@
       <c r="AA34" s="84"/>
       <c r="AB34" s="81"/>
       <c r="AC34" s="81"/>
-      <c r="AD34" s="96"/>
-      <c r="AE34" s="97"/>
-      <c r="AF34" s="98"/>
+      <c r="AD34" s="95"/>
+      <c r="AE34" s="96"/>
+      <c r="AF34" s="97"/>
       <c r="AG34" s="10"/>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.35">
@@ -2791,9 +2791,9 @@
       <c r="AA35" s="84"/>
       <c r="AB35" s="81"/>
       <c r="AC35" s="81"/>
-      <c r="AD35" s="96"/>
-      <c r="AE35" s="97"/>
-      <c r="AF35" s="98"/>
+      <c r="AD35" s="95"/>
+      <c r="AE35" s="96"/>
+      <c r="AF35" s="97"/>
       <c r="AG35" s="10"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.35">
@@ -2830,9 +2830,9 @@
       <c r="AA36" s="84"/>
       <c r="AB36" s="81"/>
       <c r="AC36" s="81"/>
-      <c r="AD36" s="96"/>
-      <c r="AE36" s="97"/>
-      <c r="AF36" s="98"/>
+      <c r="AD36" s="95"/>
+      <c r="AE36" s="96"/>
+      <c r="AF36" s="97"/>
       <c r="AG36" s="10"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.35">
@@ -2855,7 +2855,7 @@
       <c r="O37" s="81"/>
       <c r="P37" s="81"/>
       <c r="Q37" s="81"/>
-      <c r="R37" s="116"/>
+      <c r="R37" s="115"/>
       <c r="S37" s="83"/>
       <c r="T37" s="81"/>
       <c r="U37" s="84"/>
@@ -2867,9 +2867,9 @@
       <c r="AA37" s="84"/>
       <c r="AB37" s="81"/>
       <c r="AC37" s="81"/>
-      <c r="AD37" s="96"/>
-      <c r="AE37" s="97"/>
-      <c r="AF37" s="98"/>
+      <c r="AD37" s="95"/>
+      <c r="AE37" s="96"/>
+      <c r="AF37" s="97"/>
       <c r="AG37" s="10"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.35">
@@ -2892,7 +2892,7 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
       <c r="Q38" s="61"/>
-      <c r="R38" s="117"/>
+      <c r="R38" s="116"/>
       <c r="S38" s="59"/>
       <c r="T38" s="61"/>
       <c r="U38" s="65"/>
@@ -2904,8 +2904,8 @@
       <c r="AA38" s="65"/>
       <c r="AB38" s="61"/>
       <c r="AC38" s="61"/>
-      <c r="AD38" s="104"/>
-      <c r="AE38" s="105"/>
+      <c r="AD38" s="103"/>
+      <c r="AE38" s="104"/>
       <c r="AF38" s="55"/>
       <c r="AG38" s="10"/>
     </row>
@@ -2939,8 +2939,8 @@
       <c r="AA39" s="66"/>
       <c r="AB39" s="63"/>
       <c r="AC39" s="63"/>
-      <c r="AD39" s="102"/>
-      <c r="AE39" s="103"/>
+      <c r="AD39" s="101"/>
+      <c r="AE39" s="102"/>
       <c r="AF39" s="56"/>
       <c r="AG39" s="10"/>
     </row>
@@ -2976,9 +2976,9 @@
       <c r="AA40" s="76"/>
       <c r="AB40" s="74"/>
       <c r="AC40" s="74"/>
-      <c r="AD40" s="93"/>
-      <c r="AE40" s="94"/>
-      <c r="AF40" s="95"/>
+      <c r="AD40" s="92"/>
+      <c r="AE40" s="93"/>
+      <c r="AF40" s="94"/>
       <c r="AG40" s="10"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.35">
@@ -3013,9 +3013,9 @@
       <c r="AA41" s="84"/>
       <c r="AB41" s="81"/>
       <c r="AC41" s="81"/>
-      <c r="AD41" s="96"/>
-      <c r="AE41" s="97"/>
-      <c r="AF41" s="98"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="96"/>
+      <c r="AF41" s="97"/>
       <c r="AG41" s="10"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.35">
@@ -3048,9 +3048,9 @@
       <c r="AA42" s="84"/>
       <c r="AB42" s="81"/>
       <c r="AC42" s="81"/>
-      <c r="AD42" s="96"/>
-      <c r="AE42" s="97"/>
-      <c r="AF42" s="98"/>
+      <c r="AD42" s="95"/>
+      <c r="AE42" s="96"/>
+      <c r="AF42" s="97"/>
       <c r="AG42" s="10"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.35">
@@ -3085,9 +3085,9 @@
       <c r="AA43" s="84"/>
       <c r="AB43" s="81"/>
       <c r="AC43" s="81"/>
-      <c r="AD43" s="96"/>
-      <c r="AE43" s="97"/>
-      <c r="AF43" s="98"/>
+      <c r="AD43" s="95"/>
+      <c r="AE43" s="96"/>
+      <c r="AF43" s="97"/>
       <c r="AG43" s="10"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.35">
@@ -3115,7 +3115,7 @@
       <c r="T44" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="U44" s="115">
+      <c r="U44" s="114">
         <v>1</v>
       </c>
       <c r="V44" s="81"/>
@@ -3126,9 +3126,9 @@
       <c r="AA44" s="84"/>
       <c r="AB44" s="81"/>
       <c r="AC44" s="81"/>
-      <c r="AD44" s="96"/>
-      <c r="AE44" s="97"/>
-      <c r="AF44" s="98"/>
+      <c r="AD44" s="95"/>
+      <c r="AE44" s="96"/>
+      <c r="AF44" s="97"/>
       <c r="AG44" s="10"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
@@ -3163,9 +3163,9 @@
       <c r="AA45" s="84"/>
       <c r="AB45" s="81"/>
       <c r="AC45" s="81"/>
-      <c r="AD45" s="96"/>
-      <c r="AE45" s="97"/>
-      <c r="AF45" s="98"/>
+      <c r="AD45" s="95"/>
+      <c r="AE45" s="96"/>
+      <c r="AF45" s="97"/>
       <c r="AG45" s="10"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.35">
@@ -3195,7 +3195,7 @@
       <c r="R46" s="82"/>
       <c r="S46" s="83"/>
       <c r="T46" s="81"/>
-      <c r="U46" s="115">
+      <c r="U46" s="114">
         <v>1</v>
       </c>
       <c r="V46" s="81"/>
@@ -3206,9 +3206,9 @@
       <c r="AA46" s="84"/>
       <c r="AB46" s="81"/>
       <c r="AC46" s="81"/>
-      <c r="AD46" s="96"/>
-      <c r="AE46" s="97"/>
-      <c r="AF46" s="98"/>
+      <c r="AD46" s="95"/>
+      <c r="AE46" s="96"/>
+      <c r="AF46" s="97"/>
       <c r="AG46" s="10"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.35">
@@ -3243,9 +3243,9 @@
       <c r="AA47" s="84"/>
       <c r="AB47" s="81"/>
       <c r="AC47" s="81"/>
-      <c r="AD47" s="96"/>
-      <c r="AE47" s="97"/>
-      <c r="AF47" s="98"/>
+      <c r="AD47" s="95"/>
+      <c r="AE47" s="96"/>
+      <c r="AF47" s="97"/>
       <c r="AG47" s="10"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.35">
@@ -3282,9 +3282,9 @@
       <c r="AA48" s="84"/>
       <c r="AB48" s="81"/>
       <c r="AC48" s="81"/>
-      <c r="AD48" s="96"/>
-      <c r="AE48" s="97"/>
-      <c r="AF48" s="98"/>
+      <c r="AD48" s="95"/>
+      <c r="AE48" s="96"/>
+      <c r="AF48" s="97"/>
       <c r="AG48" s="10"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.35">
@@ -3321,9 +3321,9 @@
       <c r="AA49" s="84"/>
       <c r="AB49" s="81"/>
       <c r="AC49" s="81"/>
-      <c r="AD49" s="96"/>
-      <c r="AE49" s="97"/>
-      <c r="AF49" s="98"/>
+      <c r="AD49" s="95"/>
+      <c r="AE49" s="96"/>
+      <c r="AF49" s="97"/>
       <c r="AG49" s="10"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.35">
@@ -3352,7 +3352,7 @@
       <c r="U50" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="V50" s="115">
+      <c r="V50" s="114">
         <v>1</v>
       </c>
       <c r="W50" s="81"/>
@@ -3362,9 +3362,9 @@
       <c r="AA50" s="84"/>
       <c r="AB50" s="81"/>
       <c r="AC50" s="81"/>
-      <c r="AD50" s="96"/>
-      <c r="AE50" s="97"/>
-      <c r="AF50" s="98"/>
+      <c r="AD50" s="95"/>
+      <c r="AE50" s="96"/>
+      <c r="AF50" s="97"/>
       <c r="AG50" s="10"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.35">
@@ -3399,9 +3399,9 @@
       <c r="AA51" s="84"/>
       <c r="AB51" s="81"/>
       <c r="AC51" s="81"/>
-      <c r="AD51" s="96"/>
-      <c r="AE51" s="97"/>
-      <c r="AF51" s="98"/>
+      <c r="AD51" s="95"/>
+      <c r="AE51" s="96"/>
+      <c r="AF51" s="97"/>
       <c r="AG51" s="10"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.35">
@@ -3436,8 +3436,8 @@
       <c r="AA52" s="65"/>
       <c r="AB52" s="61"/>
       <c r="AC52" s="61"/>
-      <c r="AD52" s="104"/>
-      <c r="AE52" s="105"/>
+      <c r="AD52" s="103"/>
+      <c r="AE52" s="104"/>
       <c r="AF52" s="55"/>
       <c r="AG52" s="10"/>
     </row>
@@ -3471,8 +3471,8 @@
       <c r="AA53" s="65"/>
       <c r="AB53" s="61"/>
       <c r="AC53" s="61"/>
-      <c r="AD53" s="104"/>
-      <c r="AE53" s="105"/>
+      <c r="AD53" s="103"/>
+      <c r="AE53" s="104"/>
       <c r="AF53" s="55"/>
       <c r="AG53" s="10"/>
     </row>
@@ -3506,8 +3506,8 @@
       <c r="AA54" s="66"/>
       <c r="AB54" s="63"/>
       <c r="AC54" s="63"/>
-      <c r="AD54" s="102"/>
-      <c r="AE54" s="103"/>
+      <c r="AD54" s="101"/>
+      <c r="AE54" s="102"/>
       <c r="AF54" s="56"/>
       <c r="AG54" s="10"/>
     </row>
@@ -3541,9 +3541,9 @@
       <c r="AA55" s="76"/>
       <c r="AB55" s="74"/>
       <c r="AC55" s="74"/>
-      <c r="AD55" s="93"/>
-      <c r="AE55" s="94"/>
-      <c r="AF55" s="95"/>
+      <c r="AD55" s="92"/>
+      <c r="AE55" s="93"/>
+      <c r="AF55" s="94"/>
       <c r="AG55" s="10"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.35">
@@ -3578,9 +3578,9 @@
       <c r="AA56" s="84"/>
       <c r="AB56" s="81"/>
       <c r="AC56" s="81"/>
-      <c r="AD56" s="96"/>
-      <c r="AE56" s="97"/>
-      <c r="AF56" s="98"/>
+      <c r="AD56" s="95"/>
+      <c r="AE56" s="96"/>
+      <c r="AF56" s="97"/>
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.35">
@@ -3619,9 +3619,9 @@
       <c r="AA57" s="84"/>
       <c r="AB57" s="81"/>
       <c r="AC57" s="81"/>
-      <c r="AD57" s="96"/>
-      <c r="AE57" s="97"/>
-      <c r="AF57" s="98"/>
+      <c r="AD57" s="95"/>
+      <c r="AE57" s="96"/>
+      <c r="AF57" s="97"/>
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.35">
@@ -3656,9 +3656,9 @@
       <c r="AA58" s="84"/>
       <c r="AB58" s="81"/>
       <c r="AC58" s="81"/>
-      <c r="AD58" s="96"/>
-      <c r="AE58" s="97"/>
-      <c r="AF58" s="98"/>
+      <c r="AD58" s="95"/>
+      <c r="AE58" s="96"/>
+      <c r="AF58" s="97"/>
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.35">
@@ -3691,9 +3691,9 @@
       <c r="AA59" s="84"/>
       <c r="AB59" s="81"/>
       <c r="AC59" s="81"/>
-      <c r="AD59" s="96"/>
-      <c r="AE59" s="97"/>
-      <c r="AF59" s="98"/>
+      <c r="AD59" s="95"/>
+      <c r="AE59" s="96"/>
+      <c r="AF59" s="97"/>
       <c r="AG59" s="10"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.35">
@@ -3726,8 +3726,8 @@
       <c r="AA60" s="66"/>
       <c r="AB60" s="63"/>
       <c r="AC60" s="63"/>
-      <c r="AD60" s="102"/>
-      <c r="AE60" s="103"/>
+      <c r="AD60" s="101"/>
+      <c r="AE60" s="102"/>
       <c r="AF60" s="56"/>
       <c r="AG60" s="10"/>
     </row>
@@ -3761,9 +3761,9 @@
       <c r="AA61" s="76"/>
       <c r="AB61" s="74"/>
       <c r="AC61" s="74"/>
-      <c r="AD61" s="93"/>
-      <c r="AE61" s="94"/>
-      <c r="AF61" s="95"/>
+      <c r="AD61" s="92"/>
+      <c r="AE61" s="93"/>
+      <c r="AF61" s="94"/>
       <c r="AG61" s="10"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.35">
@@ -3798,9 +3798,9 @@
       <c r="AA62" s="84"/>
       <c r="AB62" s="81"/>
       <c r="AC62" s="81"/>
-      <c r="AD62" s="96"/>
-      <c r="AE62" s="97"/>
-      <c r="AF62" s="98"/>
+      <c r="AD62" s="95"/>
+      <c r="AE62" s="96"/>
+      <c r="AF62" s="97"/>
       <c r="AG62" s="10"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.35">
@@ -3829,7 +3829,7 @@
       <c r="U63" s="84"/>
       <c r="V63" s="81"/>
       <c r="W63" s="81"/>
-      <c r="X63" s="87">
+      <c r="X63" s="114">
         <v>1</v>
       </c>
       <c r="Y63" s="82"/>
@@ -3837,9 +3837,9 @@
       <c r="AA63" s="84"/>
       <c r="AB63" s="81"/>
       <c r="AC63" s="81"/>
-      <c r="AD63" s="96"/>
-      <c r="AE63" s="97"/>
-      <c r="AF63" s="98"/>
+      <c r="AD63" s="95"/>
+      <c r="AE63" s="96"/>
+      <c r="AF63" s="97"/>
       <c r="AG63" s="10"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.35">
@@ -3872,9 +3872,9 @@
       <c r="AA64" s="84"/>
       <c r="AB64" s="81"/>
       <c r="AC64" s="81"/>
-      <c r="AD64" s="96"/>
-      <c r="AE64" s="97"/>
-      <c r="AF64" s="98"/>
+      <c r="AD64" s="95"/>
+      <c r="AE64" s="96"/>
+      <c r="AF64" s="97"/>
       <c r="AG64" s="10"/>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
@@ -3913,9 +3913,9 @@
       <c r="AA65" s="84"/>
       <c r="AB65" s="81"/>
       <c r="AC65" s="81"/>
-      <c r="AD65" s="96"/>
-      <c r="AE65" s="97"/>
-      <c r="AF65" s="98"/>
+      <c r="AD65" s="95"/>
+      <c r="AE65" s="96"/>
+      <c r="AF65" s="97"/>
       <c r="AG65" s="10"/>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
@@ -3945,16 +3945,16 @@
       <c r="V66" s="81"/>
       <c r="W66" s="81"/>
       <c r="X66" s="81"/>
-      <c r="Y66" s="90">
+      <c r="Y66" s="120">
         <v>1</v>
       </c>
       <c r="Z66" s="83"/>
       <c r="AA66" s="84"/>
       <c r="AB66" s="81"/>
       <c r="AC66" s="81"/>
-      <c r="AD66" s="96"/>
-      <c r="AE66" s="97"/>
-      <c r="AF66" s="98"/>
+      <c r="AD66" s="95"/>
+      <c r="AE66" s="96"/>
+      <c r="AF66" s="97"/>
       <c r="AG66" s="10"/>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
@@ -3987,9 +3987,9 @@
       <c r="AA67" s="69"/>
       <c r="AB67" s="68"/>
       <c r="AC67" s="68"/>
-      <c r="AD67" s="99"/>
-      <c r="AE67" s="100"/>
-      <c r="AF67" s="101"/>
+      <c r="AD67" s="98"/>
+      <c r="AE67" s="99"/>
+      <c r="AF67" s="100"/>
       <c r="AG67" s="10"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
@@ -4024,9 +4024,9 @@
       <c r="AA68" s="84"/>
       <c r="AB68" s="81"/>
       <c r="AC68" s="81"/>
-      <c r="AD68" s="96"/>
-      <c r="AE68" s="97"/>
-      <c r="AF68" s="98"/>
+      <c r="AD68" s="95"/>
+      <c r="AE68" s="96"/>
+      <c r="AF68" s="97"/>
       <c r="AG68" s="10"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
@@ -4061,9 +4061,9 @@
       <c r="AA69" s="84"/>
       <c r="AB69" s="81"/>
       <c r="AC69" s="81"/>
-      <c r="AD69" s="96"/>
-      <c r="AE69" s="97"/>
-      <c r="AF69" s="98"/>
+      <c r="AD69" s="95"/>
+      <c r="AE69" s="96"/>
+      <c r="AF69" s="97"/>
       <c r="AG69" s="10"/>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
@@ -4096,8 +4096,8 @@
       <c r="AA70" s="66"/>
       <c r="AB70" s="63"/>
       <c r="AC70" s="63"/>
-      <c r="AD70" s="102"/>
-      <c r="AE70" s="103"/>
+      <c r="AD70" s="101"/>
+      <c r="AE70" s="102"/>
       <c r="AF70" s="56"/>
       <c r="AG70" s="10"/>
     </row>
@@ -4133,9 +4133,9 @@
       <c r="AA71" s="76"/>
       <c r="AB71" s="74"/>
       <c r="AC71" s="74"/>
-      <c r="AD71" s="93"/>
-      <c r="AE71" s="94"/>
-      <c r="AF71" s="95"/>
+      <c r="AD71" s="92"/>
+      <c r="AE71" s="93"/>
+      <c r="AF71" s="94"/>
       <c r="AG71" s="10"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
@@ -4170,9 +4170,9 @@
       <c r="AA72" s="84"/>
       <c r="AB72" s="81"/>
       <c r="AC72" s="81"/>
-      <c r="AD72" s="96"/>
-      <c r="AE72" s="97"/>
-      <c r="AF72" s="98"/>
+      <c r="AD72" s="95"/>
+      <c r="AE72" s="96"/>
+      <c r="AF72" s="97"/>
       <c r="AG72" s="10"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
@@ -4207,9 +4207,9 @@
       <c r="AA73" s="84"/>
       <c r="AB73" s="81"/>
       <c r="AC73" s="81"/>
-      <c r="AD73" s="96"/>
-      <c r="AE73" s="97"/>
-      <c r="AF73" s="98"/>
+      <c r="AD73" s="95"/>
+      <c r="AE73" s="96"/>
+      <c r="AF73" s="97"/>
       <c r="AG73" s="10"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
@@ -4230,7 +4230,7 @@
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="39"/>
-      <c r="L74" s="118"/>
+      <c r="L74" s="117"/>
       <c r="M74" s="81"/>
       <c r="N74" s="81"/>
       <c r="O74" s="81"/>
@@ -4248,9 +4248,9 @@
       <c r="AA74" s="84"/>
       <c r="AB74" s="81"/>
       <c r="AC74" s="81"/>
-      <c r="AD74" s="109"/>
-      <c r="AE74" s="96"/>
-      <c r="AF74" s="98"/>
+      <c r="AD74" s="108"/>
+      <c r="AE74" s="95"/>
+      <c r="AF74" s="97"/>
       <c r="AG74" s="10"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
@@ -4273,21 +4273,21 @@
       <c r="O75" s="81"/>
       <c r="P75" s="81"/>
       <c r="Q75" s="81"/>
-      <c r="R75" s="91"/>
+      <c r="R75" s="90"/>
       <c r="S75" s="83"/>
       <c r="T75" s="81"/>
       <c r="U75" s="84"/>
       <c r="V75" s="81"/>
       <c r="W75" s="81"/>
       <c r="X75" s="81"/>
-      <c r="Y75" s="91"/>
+      <c r="Y75" s="90"/>
       <c r="Z75" s="83"/>
       <c r="AA75" s="84"/>
       <c r="AB75" s="81"/>
-      <c r="AC75" s="108"/>
-      <c r="AD75" s="110"/>
-      <c r="AE75" s="97"/>
-      <c r="AF75" s="91"/>
+      <c r="AC75" s="107"/>
+      <c r="AD75" s="109"/>
+      <c r="AE75" s="96"/>
+      <c r="AF75" s="90"/>
       <c r="AG75" s="10"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
@@ -4320,9 +4320,9 @@
       <c r="AA76" s="84"/>
       <c r="AB76" s="81"/>
       <c r="AC76" s="81"/>
-      <c r="AD76" s="99"/>
-      <c r="AE76" s="96"/>
-      <c r="AF76" s="107"/>
+      <c r="AD76" s="98"/>
+      <c r="AE76" s="95"/>
+      <c r="AF76" s="106"/>
       <c r="AG76" s="10"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
@@ -4357,9 +4357,9 @@
       <c r="AA77" s="84"/>
       <c r="AB77" s="81"/>
       <c r="AC77" s="81"/>
-      <c r="AD77" s="96"/>
-      <c r="AE77" s="109"/>
-      <c r="AF77" s="107"/>
+      <c r="AD77" s="95"/>
+      <c r="AE77" s="108"/>
+      <c r="AF77" s="106"/>
       <c r="AG77" s="10"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
@@ -4378,25 +4378,25 @@
       <c r="K78" s="70"/>
       <c r="L78" s="80"/>
       <c r="M78" s="85"/>
-      <c r="N78" s="115"/>
-      <c r="O78" s="115"/>
-      <c r="P78" s="115"/>
-      <c r="Q78" s="115"/>
-      <c r="R78" s="115"/>
-      <c r="S78" s="118"/>
+      <c r="N78" s="114"/>
+      <c r="O78" s="114"/>
+      <c r="P78" s="114"/>
+      <c r="Q78" s="114"/>
+      <c r="R78" s="114"/>
+      <c r="S78" s="117"/>
       <c r="T78" s="85"/>
-      <c r="U78" s="119"/>
+      <c r="U78" s="118"/>
       <c r="V78" s="85"/>
       <c r="W78" s="85"/>
       <c r="X78" s="85"/>
-      <c r="Y78" s="120"/>
-      <c r="Z78" s="80"/>
-      <c r="AA78" s="85"/>
+      <c r="Y78" s="119"/>
+      <c r="Z78" s="117"/>
+      <c r="AA78" s="114"/>
       <c r="AB78" s="85"/>
       <c r="AC78" s="85"/>
-      <c r="AD78" s="114"/>
+      <c r="AD78" s="113"/>
       <c r="AE78" s="57"/>
-      <c r="AF78" s="91"/>
+      <c r="AF78" s="90"/>
       <c r="AG78" s="10"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
@@ -4429,9 +4429,9 @@
       <c r="AA79" s="63"/>
       <c r="AB79" s="63"/>
       <c r="AC79" s="63"/>
-      <c r="AD79" s="112"/>
-      <c r="AE79" s="102"/>
-      <c r="AF79" s="113"/>
+      <c r="AD79" s="111"/>
+      <c r="AE79" s="101"/>
+      <c r="AF79" s="112"/>
       <c r="AG79" s="10"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
@@ -4456,21 +4456,21 @@
       <c r="O80" s="74"/>
       <c r="P80" s="74"/>
       <c r="Q80" s="74"/>
-      <c r="R80" s="92"/>
+      <c r="R80" s="91"/>
       <c r="S80" s="76"/>
       <c r="T80" s="74"/>
       <c r="U80" s="74"/>
       <c r="V80" s="74"/>
       <c r="W80" s="74"/>
       <c r="X80" s="74"/>
-      <c r="Y80" s="92"/>
+      <c r="Y80" s="91"/>
       <c r="Z80" s="76"/>
       <c r="AA80" s="74"/>
       <c r="AB80" s="74"/>
       <c r="AC80" s="74"/>
-      <c r="AD80" s="99"/>
-      <c r="AE80" s="99"/>
-      <c r="AF80" s="111"/>
+      <c r="AD80" s="98"/>
+      <c r="AE80" s="98"/>
+      <c r="AF80" s="110"/>
       <c r="AG80" s="10"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
@@ -4507,9 +4507,9 @@
       <c r="AA81" s="67"/>
       <c r="AB81" s="67"/>
       <c r="AC81" s="63"/>
-      <c r="AD81" s="112"/>
-      <c r="AE81" s="112"/>
-      <c r="AF81" s="113"/>
+      <c r="AD81" s="111"/>
+      <c r="AE81" s="111"/>
+      <c r="AF81" s="112"/>
       <c r="AG81" s="10"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
@@ -4605,13 +4605,13 @@
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C89" s="106"/>
+      <c r="C89" s="105"/>
       <c r="D89" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C90" s="110"/>
+      <c r="C90" s="109"/>
       <c r="D90" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Camaras al piso, areras y libre
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F0F2E-70EC-4E4A-BC15-0AD43D5C28B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2054E84-4CF0-4E0F-B338-96F3BCB494FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="X69" sqref="G69:X69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="V76" sqref="V76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3612,7 +3612,7 @@
       <c r="T57" s="81"/>
       <c r="U57" s="84"/>
       <c r="V57" s="81"/>
-      <c r="W57" s="87"/>
+      <c r="W57" s="114"/>
       <c r="X57" s="81"/>
       <c r="Y57" s="82"/>
       <c r="Z57" s="83"/>
@@ -3649,7 +3649,7 @@
       <c r="T58" s="81"/>
       <c r="U58" s="84"/>
       <c r="V58" s="81"/>
-      <c r="W58" s="87"/>
+      <c r="W58" s="114"/>
       <c r="X58" s="81"/>
       <c r="Y58" s="82"/>
       <c r="Z58" s="83"/>
@@ -4392,7 +4392,7 @@
       <c r="Y78" s="119"/>
       <c r="Z78" s="117"/>
       <c r="AA78" s="114"/>
-      <c r="AB78" s="85"/>
+      <c r="AB78" s="114"/>
       <c r="AC78" s="85"/>
       <c r="AD78" s="113"/>
       <c r="AE78" s="57"/>

</xml_diff>

<commit_message>
Show de luces y decoracion del piso
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2054E84-4CF0-4E0F-B338-96F3BCB494FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A568D-B46F-4E43-80D3-4C985F20E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="V76" sqref="V76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4055,7 +4055,7 @@
       <c r="U69" s="84"/>
       <c r="V69" s="81"/>
       <c r="W69" s="81"/>
-      <c r="X69" s="87"/>
+      <c r="X69" s="114"/>
       <c r="Y69" s="82"/>
       <c r="Z69" s="83"/>
       <c r="AA69" s="84"/>

</xml_diff>

<commit_message>
Guardado de camaras, arreglando luces puntuales
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A568D-B46F-4E43-80D3-4C985F20E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3601DD8-6166-47CE-B0A9-8196CA863B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
@@ -204,12 +204,6 @@
     <t>- Movimiento en las nubes</t>
   </si>
   <si>
-    <t>- Movimiento en los postes de entrada</t>
-  </si>
-  <si>
-    <t>- Movimiento en una de las rocas</t>
-  </si>
-  <si>
     <t>- Musica para la pista de baile</t>
   </si>
   <si>
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>- Movimiento en los postes de entrada (Muñecos de nieve)</t>
+  </si>
+  <si>
+    <t>- Movimiento en una de las rocas (Se paso a compleja)</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1039,7 +1039,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1390,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V52" sqref="V52"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="Q34" sqref="G33:Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1716,9 +1715,9 @@
       <c r="AA6" s="76"/>
       <c r="AB6" s="74"/>
       <c r="AC6" s="74"/>
-      <c r="AD6" s="92"/>
-      <c r="AE6" s="93"/>
-      <c r="AF6" s="94"/>
+      <c r="AD6" s="91"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="93"/>
       <c r="AG6" s="10"/>
     </row>
     <row r="7" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1753,9 +1752,9 @@
       <c r="AA7" s="84"/>
       <c r="AB7" s="81"/>
       <c r="AC7" s="85"/>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="96"/>
-      <c r="AF7" s="97"/>
+      <c r="AD7" s="94"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="96"/>
       <c r="AG7" s="10"/>
     </row>
     <row r="8" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1765,7 +1764,7 @@
       <c r="D8" s="46"/>
       <c r="E8" s="14"/>
       <c r="F8" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="4"/>
@@ -1790,9 +1789,9 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="68"/>
       <c r="AC8" s="79"/>
-      <c r="AD8" s="98"/>
-      <c r="AE8" s="99"/>
-      <c r="AF8" s="100"/>
+      <c r="AD8" s="97"/>
+      <c r="AE8" s="98"/>
+      <c r="AF8" s="99"/>
       <c r="AG8" s="10"/>
     </row>
     <row r="9" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1802,7 +1801,7 @@
       <c r="D9" s="46"/>
       <c r="E9" s="14"/>
       <c r="F9" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="4"/>
@@ -1827,9 +1826,9 @@
       <c r="AA9" s="84"/>
       <c r="AB9" s="81"/>
       <c r="AC9" s="81"/>
-      <c r="AD9" s="95"/>
-      <c r="AE9" s="96"/>
-      <c r="AF9" s="97"/>
+      <c r="AD9" s="94"/>
+      <c r="AE9" s="95"/>
+      <c r="AF9" s="96"/>
       <c r="AG9" s="10"/>
     </row>
     <row r="10" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1862,9 +1861,9 @@
       <c r="AA10" s="84"/>
       <c r="AB10" s="81"/>
       <c r="AC10" s="81"/>
-      <c r="AD10" s="95"/>
-      <c r="AE10" s="96"/>
-      <c r="AF10" s="97"/>
+      <c r="AD10" s="94"/>
+      <c r="AE10" s="95"/>
+      <c r="AF10" s="96"/>
       <c r="AG10" s="10"/>
     </row>
     <row r="11" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1899,9 +1898,9 @@
       <c r="AA11" s="84"/>
       <c r="AB11" s="81"/>
       <c r="AC11" s="81"/>
-      <c r="AD11" s="95"/>
-      <c r="AE11" s="96"/>
-      <c r="AF11" s="97"/>
+      <c r="AD11" s="94"/>
+      <c r="AE11" s="95"/>
+      <c r="AF11" s="96"/>
       <c r="AG11" s="10"/>
     </row>
     <row r="12" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1936,9 +1935,9 @@
       <c r="AA12" s="84"/>
       <c r="AB12" s="81"/>
       <c r="AC12" s="81"/>
-      <c r="AD12" s="95"/>
-      <c r="AE12" s="96"/>
-      <c r="AF12" s="97"/>
+      <c r="AD12" s="94"/>
+      <c r="AE12" s="95"/>
+      <c r="AF12" s="96"/>
       <c r="AG12" s="10"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
@@ -1973,9 +1972,9 @@
       <c r="AA13" s="84"/>
       <c r="AB13" s="81"/>
       <c r="AC13" s="81"/>
-      <c r="AD13" s="95"/>
-      <c r="AE13" s="96"/>
-      <c r="AF13" s="97"/>
+      <c r="AD13" s="94"/>
+      <c r="AE13" s="95"/>
+      <c r="AF13" s="96"/>
       <c r="AG13" s="10"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
@@ -2008,9 +2007,9 @@
       <c r="AA14" s="84"/>
       <c r="AB14" s="81"/>
       <c r="AC14" s="81"/>
-      <c r="AD14" s="95"/>
-      <c r="AE14" s="96"/>
-      <c r="AF14" s="97"/>
+      <c r="AD14" s="94"/>
+      <c r="AE14" s="95"/>
+      <c r="AF14" s="96"/>
       <c r="AG14" s="10"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
@@ -2045,9 +2044,9 @@
       <c r="AA15" s="84"/>
       <c r="AB15" s="81"/>
       <c r="AC15" s="81"/>
-      <c r="AD15" s="95"/>
-      <c r="AE15" s="96"/>
-      <c r="AF15" s="97"/>
+      <c r="AD15" s="94"/>
+      <c r="AE15" s="95"/>
+      <c r="AF15" s="96"/>
       <c r="AG15" s="10"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
@@ -2064,7 +2063,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="86">
+      <c r="L16" s="116">
         <v>1</v>
       </c>
       <c r="M16" s="81"/>
@@ -2084,9 +2083,9 @@
       <c r="AA16" s="84"/>
       <c r="AB16" s="81"/>
       <c r="AC16" s="81"/>
-      <c r="AD16" s="95"/>
-      <c r="AE16" s="96"/>
-      <c r="AF16" s="97"/>
+      <c r="AD16" s="94"/>
+      <c r="AE16" s="95"/>
+      <c r="AF16" s="96"/>
       <c r="AG16" s="10"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
@@ -2104,7 +2103,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="39"/>
       <c r="L17" s="83"/>
-      <c r="M17" s="114"/>
+      <c r="M17" s="113"/>
       <c r="N17" s="81"/>
       <c r="O17" s="81"/>
       <c r="P17" s="81"/>
@@ -2121,9 +2120,9 @@
       <c r="AA17" s="84"/>
       <c r="AB17" s="81"/>
       <c r="AC17" s="81"/>
-      <c r="AD17" s="95"/>
-      <c r="AE17" s="96"/>
-      <c r="AF17" s="97"/>
+      <c r="AD17" s="94"/>
+      <c r="AE17" s="95"/>
+      <c r="AF17" s="96"/>
       <c r="AG17" s="10"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
@@ -2143,7 +2142,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="39"/>
       <c r="L18" s="83"/>
-      <c r="M18" s="114"/>
+      <c r="M18" s="113"/>
       <c r="N18" s="81"/>
       <c r="O18" s="81"/>
       <c r="P18" s="81"/>
@@ -2160,9 +2159,9 @@
       <c r="AA18" s="84"/>
       <c r="AB18" s="81"/>
       <c r="AC18" s="81"/>
-      <c r="AD18" s="95"/>
-      <c r="AE18" s="96"/>
-      <c r="AF18" s="97"/>
+      <c r="AD18" s="94"/>
+      <c r="AE18" s="95"/>
+      <c r="AF18" s="96"/>
       <c r="AG18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.35">
@@ -2180,7 +2179,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="39"/>
       <c r="L19" s="83"/>
-      <c r="M19" s="114"/>
+      <c r="M19" s="113"/>
       <c r="N19" s="81"/>
       <c r="O19" s="81"/>
       <c r="P19" s="81"/>
@@ -2197,9 +2196,9 @@
       <c r="AA19" s="84"/>
       <c r="AB19" s="81"/>
       <c r="AC19" s="81"/>
-      <c r="AD19" s="95"/>
-      <c r="AE19" s="96"/>
-      <c r="AF19" s="97"/>
+      <c r="AD19" s="94"/>
+      <c r="AE19" s="95"/>
+      <c r="AF19" s="96"/>
       <c r="AG19" s="10"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
@@ -2234,9 +2233,9 @@
       <c r="AA20" s="84"/>
       <c r="AB20" s="81"/>
       <c r="AC20" s="81"/>
-      <c r="AD20" s="95"/>
-      <c r="AE20" s="96"/>
-      <c r="AF20" s="97"/>
+      <c r="AD20" s="94"/>
+      <c r="AE20" s="95"/>
+      <c r="AF20" s="96"/>
       <c r="AG20" s="10"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
@@ -2250,14 +2249,14 @@
         <v>23</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="39"/>
       <c r="L21" s="83"/>
       <c r="M21" s="81"/>
-      <c r="N21" s="114"/>
+      <c r="N21" s="113"/>
       <c r="O21" s="81"/>
       <c r="P21" s="81"/>
       <c r="Q21" s="81"/>
@@ -2273,9 +2272,9 @@
       <c r="AA21" s="84"/>
       <c r="AB21" s="81"/>
       <c r="AC21" s="81"/>
-      <c r="AD21" s="95"/>
-      <c r="AE21" s="96"/>
-      <c r="AF21" s="97"/>
+      <c r="AD21" s="94"/>
+      <c r="AE21" s="95"/>
+      <c r="AF21" s="96"/>
       <c r="AG21" s="10"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
@@ -2294,7 +2293,7 @@
       <c r="K22" s="39"/>
       <c r="L22" s="83"/>
       <c r="M22" s="81"/>
-      <c r="N22" s="114"/>
+      <c r="N22" s="113"/>
       <c r="O22" s="81"/>
       <c r="P22" s="81"/>
       <c r="Q22" s="81"/>
@@ -2310,9 +2309,9 @@
       <c r="AA22" s="84"/>
       <c r="AB22" s="81"/>
       <c r="AC22" s="81"/>
-      <c r="AD22" s="95"/>
-      <c r="AE22" s="96"/>
-      <c r="AF22" s="97"/>
+      <c r="AD22" s="94"/>
+      <c r="AE22" s="95"/>
+      <c r="AF22" s="96"/>
       <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
@@ -2331,7 +2330,7 @@
       <c r="K23" s="39"/>
       <c r="L23" s="83"/>
       <c r="M23" s="81"/>
-      <c r="N23" s="114"/>
+      <c r="N23" s="113"/>
       <c r="O23" s="81"/>
       <c r="P23" s="81"/>
       <c r="Q23" s="81"/>
@@ -2347,9 +2346,9 @@
       <c r="AA23" s="84"/>
       <c r="AB23" s="81"/>
       <c r="AC23" s="81"/>
-      <c r="AD23" s="95"/>
-      <c r="AE23" s="96"/>
-      <c r="AF23" s="97"/>
+      <c r="AD23" s="94"/>
+      <c r="AE23" s="95"/>
+      <c r="AF23" s="96"/>
       <c r="AG23" s="10"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
@@ -2368,7 +2367,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="83"/>
       <c r="M24" s="81"/>
-      <c r="N24" s="114"/>
+      <c r="N24" s="113"/>
       <c r="O24" s="81"/>
       <c r="P24" s="81"/>
       <c r="Q24" s="81"/>
@@ -2384,9 +2383,9 @@
       <c r="AA24" s="84"/>
       <c r="AB24" s="81"/>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="95"/>
-      <c r="AE24" s="96"/>
-      <c r="AF24" s="97"/>
+      <c r="AD24" s="94"/>
+      <c r="AE24" s="95"/>
+      <c r="AF24" s="96"/>
       <c r="AG24" s="10"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
@@ -2406,7 +2405,7 @@
       <c r="L25" s="83"/>
       <c r="M25" s="81"/>
       <c r="N25" s="81"/>
-      <c r="O25" s="114"/>
+      <c r="O25" s="113"/>
       <c r="P25" s="81"/>
       <c r="Q25" s="81"/>
       <c r="R25" s="82"/>
@@ -2421,9 +2420,9 @@
       <c r="AA25" s="84"/>
       <c r="AB25" s="81"/>
       <c r="AC25" s="81"/>
-      <c r="AD25" s="95"/>
-      <c r="AE25" s="96"/>
-      <c r="AF25" s="97"/>
+      <c r="AD25" s="94"/>
+      <c r="AE25" s="95"/>
+      <c r="AF25" s="96"/>
       <c r="AG25" s="10"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
@@ -2443,7 +2442,7 @@
       <c r="L26" s="83"/>
       <c r="M26" s="81"/>
       <c r="N26" s="81"/>
-      <c r="O26" s="114"/>
+      <c r="O26" s="113"/>
       <c r="P26" s="81"/>
       <c r="Q26" s="81"/>
       <c r="R26" s="82"/>
@@ -2458,9 +2457,9 @@
       <c r="AA26" s="84"/>
       <c r="AB26" s="81"/>
       <c r="AC26" s="81"/>
-      <c r="AD26" s="95"/>
-      <c r="AE26" s="96"/>
-      <c r="AF26" s="97"/>
+      <c r="AD26" s="94"/>
+      <c r="AE26" s="95"/>
+      <c r="AF26" s="96"/>
       <c r="AG26" s="10"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
@@ -2480,7 +2479,7 @@
       <c r="L27" s="83"/>
       <c r="M27" s="81"/>
       <c r="N27" s="81"/>
-      <c r="O27" s="114"/>
+      <c r="O27" s="113"/>
       <c r="P27" s="81"/>
       <c r="Q27" s="81"/>
       <c r="R27" s="82"/>
@@ -2495,9 +2494,9 @@
       <c r="AA27" s="84"/>
       <c r="AB27" s="81"/>
       <c r="AC27" s="81"/>
-      <c r="AD27" s="95"/>
-      <c r="AE27" s="96"/>
-      <c r="AF27" s="97"/>
+      <c r="AD27" s="94"/>
+      <c r="AE27" s="95"/>
+      <c r="AF27" s="96"/>
       <c r="AG27" s="10"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
@@ -2517,7 +2516,7 @@
       <c r="L28" s="83"/>
       <c r="M28" s="81"/>
       <c r="N28" s="81"/>
-      <c r="O28" s="114"/>
+      <c r="O28" s="113"/>
       <c r="P28" s="81"/>
       <c r="Q28" s="81"/>
       <c r="R28" s="82"/>
@@ -2532,9 +2531,9 @@
       <c r="AA28" s="84"/>
       <c r="AB28" s="81"/>
       <c r="AC28" s="81"/>
-      <c r="AD28" s="95"/>
-      <c r="AE28" s="96"/>
-      <c r="AF28" s="97"/>
+      <c r="AD28" s="94"/>
+      <c r="AE28" s="95"/>
+      <c r="AF28" s="96"/>
       <c r="AG28" s="10"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.35">
@@ -2554,7 +2553,7 @@
       <c r="L29" s="83"/>
       <c r="M29" s="81"/>
       <c r="N29" s="81"/>
-      <c r="O29" s="114"/>
+      <c r="O29" s="113"/>
       <c r="P29" s="81"/>
       <c r="Q29" s="81"/>
       <c r="R29" s="82"/>
@@ -2569,9 +2568,9 @@
       <c r="AA29" s="84"/>
       <c r="AB29" s="81"/>
       <c r="AC29" s="81"/>
-      <c r="AD29" s="95"/>
-      <c r="AE29" s="96"/>
-      <c r="AF29" s="97"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="95"/>
+      <c r="AF29" s="96"/>
       <c r="AG29" s="10"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
@@ -2606,9 +2605,9 @@
       <c r="AA30" s="84"/>
       <c r="AB30" s="81"/>
       <c r="AC30" s="81"/>
-      <c r="AD30" s="95"/>
-      <c r="AE30" s="96"/>
-      <c r="AF30" s="97"/>
+      <c r="AD30" s="94"/>
+      <c r="AE30" s="95"/>
+      <c r="AF30" s="96"/>
       <c r="AG30" s="10"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
@@ -2643,8 +2642,8 @@
       <c r="AA31" s="66"/>
       <c r="AB31" s="63"/>
       <c r="AC31" s="63"/>
-      <c r="AD31" s="101"/>
-      <c r="AE31" s="102"/>
+      <c r="AD31" s="100"/>
+      <c r="AE31" s="101"/>
       <c r="AF31" s="56"/>
       <c r="AG31" s="10"/>
     </row>
@@ -2680,9 +2679,9 @@
       <c r="AA32" s="76"/>
       <c r="AB32" s="74"/>
       <c r="AC32" s="74"/>
-      <c r="AD32" s="92"/>
-      <c r="AE32" s="93"/>
-      <c r="AF32" s="94"/>
+      <c r="AD32" s="91"/>
+      <c r="AE32" s="92"/>
+      <c r="AF32" s="93"/>
       <c r="AG32" s="10"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
@@ -2704,7 +2703,7 @@
       <c r="N33" s="81"/>
       <c r="O33" s="81"/>
       <c r="P33" s="81"/>
-      <c r="Q33" s="87"/>
+      <c r="Q33" s="86"/>
       <c r="R33" s="82"/>
       <c r="S33" s="83"/>
       <c r="T33" s="81"/>
@@ -2717,9 +2716,9 @@
       <c r="AA33" s="84"/>
       <c r="AB33" s="81"/>
       <c r="AC33" s="81"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="96"/>
-      <c r="AF33" s="97"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="95"/>
+      <c r="AF33" s="96"/>
       <c r="AG33" s="10"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.35">
@@ -2741,7 +2740,7 @@
       <c r="N34" s="81"/>
       <c r="O34" s="81"/>
       <c r="P34" s="81"/>
-      <c r="Q34" s="87"/>
+      <c r="Q34" s="86"/>
       <c r="R34" s="82"/>
       <c r="S34" s="83"/>
       <c r="T34" s="81"/>
@@ -2754,9 +2753,9 @@
       <c r="AA34" s="84"/>
       <c r="AB34" s="81"/>
       <c r="AC34" s="81"/>
-      <c r="AD34" s="95"/>
-      <c r="AE34" s="96"/>
-      <c r="AF34" s="97"/>
+      <c r="AD34" s="94"/>
+      <c r="AE34" s="95"/>
+      <c r="AF34" s="96"/>
       <c r="AG34" s="10"/>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.35">
@@ -2768,7 +2767,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="16"/>
       <c r="H35" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="6"/>
@@ -2791,9 +2790,9 @@
       <c r="AA35" s="84"/>
       <c r="AB35" s="81"/>
       <c r="AC35" s="81"/>
-      <c r="AD35" s="95"/>
-      <c r="AE35" s="96"/>
-      <c r="AF35" s="97"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="95"/>
+      <c r="AF35" s="96"/>
       <c r="AG35" s="10"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.35">
@@ -2830,9 +2829,9 @@
       <c r="AA36" s="84"/>
       <c r="AB36" s="81"/>
       <c r="AC36" s="81"/>
-      <c r="AD36" s="95"/>
-      <c r="AE36" s="96"/>
-      <c r="AF36" s="97"/>
+      <c r="AD36" s="94"/>
+      <c r="AE36" s="95"/>
+      <c r="AF36" s="96"/>
       <c r="AG36" s="10"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.35">
@@ -2855,7 +2854,7 @@
       <c r="O37" s="81"/>
       <c r="P37" s="81"/>
       <c r="Q37" s="81"/>
-      <c r="R37" s="115"/>
+      <c r="R37" s="114"/>
       <c r="S37" s="83"/>
       <c r="T37" s="81"/>
       <c r="U37" s="84"/>
@@ -2867,9 +2866,9 @@
       <c r="AA37" s="84"/>
       <c r="AB37" s="81"/>
       <c r="AC37" s="81"/>
-      <c r="AD37" s="95"/>
-      <c r="AE37" s="96"/>
-      <c r="AF37" s="97"/>
+      <c r="AD37" s="94"/>
+      <c r="AE37" s="95"/>
+      <c r="AF37" s="96"/>
       <c r="AG37" s="10"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.35">
@@ -2892,7 +2891,7 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
       <c r="Q38" s="61"/>
-      <c r="R38" s="116"/>
+      <c r="R38" s="115"/>
       <c r="S38" s="59"/>
       <c r="T38" s="61"/>
       <c r="U38" s="65"/>
@@ -2904,8 +2903,8 @@
       <c r="AA38" s="65"/>
       <c r="AB38" s="61"/>
       <c r="AC38" s="61"/>
-      <c r="AD38" s="103"/>
-      <c r="AE38" s="104"/>
+      <c r="AD38" s="102"/>
+      <c r="AE38" s="103"/>
       <c r="AF38" s="55"/>
       <c r="AG38" s="10"/>
     </row>
@@ -2939,8 +2938,8 @@
       <c r="AA39" s="66"/>
       <c r="AB39" s="63"/>
       <c r="AC39" s="63"/>
-      <c r="AD39" s="101"/>
-      <c r="AE39" s="102"/>
+      <c r="AD39" s="100"/>
+      <c r="AE39" s="101"/>
       <c r="AF39" s="56"/>
       <c r="AG39" s="10"/>
     </row>
@@ -2976,9 +2975,9 @@
       <c r="AA40" s="76"/>
       <c r="AB40" s="74"/>
       <c r="AC40" s="74"/>
-      <c r="AD40" s="92"/>
-      <c r="AE40" s="93"/>
-      <c r="AF40" s="94"/>
+      <c r="AD40" s="91"/>
+      <c r="AE40" s="92"/>
+      <c r="AF40" s="93"/>
       <c r="AG40" s="10"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.35">
@@ -3002,7 +3001,7 @@
       <c r="P41" s="81"/>
       <c r="Q41" s="81"/>
       <c r="R41" s="82"/>
-      <c r="S41" s="88"/>
+      <c r="S41" s="87"/>
       <c r="T41" s="81"/>
       <c r="U41" s="84"/>
       <c r="V41" s="81"/>
@@ -3013,9 +3012,9 @@
       <c r="AA41" s="84"/>
       <c r="AB41" s="81"/>
       <c r="AC41" s="81"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="96"/>
-      <c r="AF41" s="97"/>
+      <c r="AD41" s="94"/>
+      <c r="AE41" s="95"/>
+      <c r="AF41" s="96"/>
       <c r="AG41" s="10"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.35">
@@ -3048,9 +3047,9 @@
       <c r="AA42" s="84"/>
       <c r="AB42" s="81"/>
       <c r="AC42" s="81"/>
-      <c r="AD42" s="95"/>
-      <c r="AE42" s="96"/>
-      <c r="AF42" s="97"/>
+      <c r="AD42" s="94"/>
+      <c r="AE42" s="95"/>
+      <c r="AF42" s="96"/>
       <c r="AG42" s="10"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.35">
@@ -3085,9 +3084,9 @@
       <c r="AA43" s="84"/>
       <c r="AB43" s="81"/>
       <c r="AC43" s="81"/>
-      <c r="AD43" s="95"/>
-      <c r="AE43" s="96"/>
-      <c r="AF43" s="97"/>
+      <c r="AD43" s="94"/>
+      <c r="AE43" s="95"/>
+      <c r="AF43" s="96"/>
       <c r="AG43" s="10"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.35">
@@ -3097,7 +3096,7 @@
       <c r="D44" s="46"/>
       <c r="E44" s="14"/>
       <c r="F44" s="24" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="4"/>
@@ -3113,9 +3112,9 @@
       <c r="R44" s="82"/>
       <c r="S44" s="83"/>
       <c r="T44" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="U44" s="114">
+        <v>76</v>
+      </c>
+      <c r="U44" s="113">
         <v>1</v>
       </c>
       <c r="V44" s="81"/>
@@ -3126,9 +3125,9 @@
       <c r="AA44" s="84"/>
       <c r="AB44" s="81"/>
       <c r="AC44" s="81"/>
-      <c r="AD44" s="95"/>
-      <c r="AE44" s="96"/>
-      <c r="AF44" s="97"/>
+      <c r="AD44" s="94"/>
+      <c r="AE44" s="95"/>
+      <c r="AF44" s="96"/>
       <c r="AG44" s="10"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
@@ -3138,7 +3137,7 @@
       <c r="D45" s="46"/>
       <c r="E45" s="14"/>
       <c r="F45" s="24" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="4"/>
@@ -3163,9 +3162,9 @@
       <c r="AA45" s="84"/>
       <c r="AB45" s="81"/>
       <c r="AC45" s="81"/>
-      <c r="AD45" s="95"/>
-      <c r="AE45" s="96"/>
-      <c r="AF45" s="97"/>
+      <c r="AD45" s="94"/>
+      <c r="AE45" s="95"/>
+      <c r="AF45" s="96"/>
       <c r="AG45" s="10"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.35">
@@ -3177,11 +3176,11 @@
       <c r="D46" s="46"/>
       <c r="E46" s="28"/>
       <c r="F46" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="6"/>
@@ -3195,7 +3194,7 @@
       <c r="R46" s="82"/>
       <c r="S46" s="83"/>
       <c r="T46" s="81"/>
-      <c r="U46" s="114">
+      <c r="U46" s="113">
         <v>1</v>
       </c>
       <c r="V46" s="81"/>
@@ -3206,9 +3205,9 @@
       <c r="AA46" s="84"/>
       <c r="AB46" s="81"/>
       <c r="AC46" s="81"/>
-      <c r="AD46" s="95"/>
-      <c r="AE46" s="96"/>
-      <c r="AF46" s="97"/>
+      <c r="AD46" s="94"/>
+      <c r="AE46" s="95"/>
+      <c r="AF46" s="96"/>
       <c r="AG46" s="10"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.35">
@@ -3243,9 +3242,9 @@
       <c r="AA47" s="84"/>
       <c r="AB47" s="81"/>
       <c r="AC47" s="81"/>
-      <c r="AD47" s="95"/>
-      <c r="AE47" s="96"/>
-      <c r="AF47" s="97"/>
+      <c r="AD47" s="94"/>
+      <c r="AE47" s="95"/>
+      <c r="AF47" s="96"/>
       <c r="AG47" s="10"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.35">
@@ -3270,9 +3269,9 @@
       <c r="Q48" s="81"/>
       <c r="R48" s="82"/>
       <c r="S48" s="83" t="s">
-        <v>78</v>
-      </c>
-      <c r="T48" s="89"/>
+        <v>76</v>
+      </c>
+      <c r="T48" s="88"/>
       <c r="U48" s="84"/>
       <c r="V48" s="81"/>
       <c r="W48" s="81"/>
@@ -3282,9 +3281,9 @@
       <c r="AA48" s="84"/>
       <c r="AB48" s="81"/>
       <c r="AC48" s="81"/>
-      <c r="AD48" s="95"/>
-      <c r="AE48" s="96"/>
-      <c r="AF48" s="97"/>
+      <c r="AD48" s="94"/>
+      <c r="AE48" s="95"/>
+      <c r="AF48" s="96"/>
       <c r="AG48" s="10"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.35">
@@ -3309,7 +3308,7 @@
       <c r="Q49" s="81"/>
       <c r="R49" s="82"/>
       <c r="S49" s="83"/>
-      <c r="T49" s="89">
+      <c r="T49" s="88">
         <v>1</v>
       </c>
       <c r="U49" s="84"/>
@@ -3321,9 +3320,9 @@
       <c r="AA49" s="84"/>
       <c r="AB49" s="81"/>
       <c r="AC49" s="81"/>
-      <c r="AD49" s="95"/>
-      <c r="AE49" s="96"/>
-      <c r="AF49" s="97"/>
+      <c r="AD49" s="94"/>
+      <c r="AE49" s="95"/>
+      <c r="AF49" s="96"/>
       <c r="AG49" s="10"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.35">
@@ -3350,9 +3349,9 @@
       <c r="S50" s="83"/>
       <c r="T50" s="81"/>
       <c r="U50" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="V50" s="114">
+        <v>76</v>
+      </c>
+      <c r="V50" s="113">
         <v>1</v>
       </c>
       <c r="W50" s="81"/>
@@ -3362,9 +3361,9 @@
       <c r="AA50" s="84"/>
       <c r="AB50" s="81"/>
       <c r="AC50" s="81"/>
-      <c r="AD50" s="95"/>
-      <c r="AE50" s="96"/>
-      <c r="AF50" s="97"/>
+      <c r="AD50" s="94"/>
+      <c r="AE50" s="95"/>
+      <c r="AF50" s="96"/>
       <c r="AG50" s="10"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.35">
@@ -3399,9 +3398,9 @@
       <c r="AA51" s="84"/>
       <c r="AB51" s="81"/>
       <c r="AC51" s="81"/>
-      <c r="AD51" s="95"/>
-      <c r="AE51" s="96"/>
-      <c r="AF51" s="97"/>
+      <c r="AD51" s="94"/>
+      <c r="AE51" s="95"/>
+      <c r="AF51" s="96"/>
       <c r="AG51" s="10"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.35">
@@ -3436,8 +3435,8 @@
       <c r="AA52" s="65"/>
       <c r="AB52" s="61"/>
       <c r="AC52" s="61"/>
-      <c r="AD52" s="103"/>
-      <c r="AE52" s="104"/>
+      <c r="AD52" s="102"/>
+      <c r="AE52" s="103"/>
       <c r="AF52" s="55"/>
       <c r="AG52" s="10"/>
     </row>
@@ -3471,8 +3470,8 @@
       <c r="AA53" s="65"/>
       <c r="AB53" s="61"/>
       <c r="AC53" s="61"/>
-      <c r="AD53" s="103"/>
-      <c r="AE53" s="104"/>
+      <c r="AD53" s="102"/>
+      <c r="AE53" s="103"/>
       <c r="AF53" s="55"/>
       <c r="AG53" s="10"/>
     </row>
@@ -3506,8 +3505,8 @@
       <c r="AA54" s="66"/>
       <c r="AB54" s="63"/>
       <c r="AC54" s="63"/>
-      <c r="AD54" s="101"/>
-      <c r="AE54" s="102"/>
+      <c r="AD54" s="100"/>
+      <c r="AE54" s="101"/>
       <c r="AF54" s="56"/>
       <c r="AG54" s="10"/>
     </row>
@@ -3541,9 +3540,9 @@
       <c r="AA55" s="76"/>
       <c r="AB55" s="74"/>
       <c r="AC55" s="74"/>
-      <c r="AD55" s="92"/>
-      <c r="AE55" s="93"/>
-      <c r="AF55" s="94"/>
+      <c r="AD55" s="91"/>
+      <c r="AE55" s="92"/>
+      <c r="AF55" s="93"/>
       <c r="AG55" s="10"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.35">
@@ -3578,9 +3577,9 @@
       <c r="AA56" s="84"/>
       <c r="AB56" s="81"/>
       <c r="AC56" s="81"/>
-      <c r="AD56" s="95"/>
-      <c r="AE56" s="96"/>
-      <c r="AF56" s="97"/>
+      <c r="AD56" s="94"/>
+      <c r="AE56" s="95"/>
+      <c r="AF56" s="96"/>
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.35">
@@ -3596,7 +3595,7 @@
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="6"/>
@@ -3612,16 +3611,16 @@
       <c r="T57" s="81"/>
       <c r="U57" s="84"/>
       <c r="V57" s="81"/>
-      <c r="W57" s="114"/>
+      <c r="W57" s="113"/>
       <c r="X57" s="81"/>
       <c r="Y57" s="82"/>
       <c r="Z57" s="83"/>
       <c r="AA57" s="84"/>
       <c r="AB57" s="81"/>
       <c r="AC57" s="81"/>
-      <c r="AD57" s="95"/>
-      <c r="AE57" s="96"/>
-      <c r="AF57" s="97"/>
+      <c r="AD57" s="94"/>
+      <c r="AE57" s="95"/>
+      <c r="AF57" s="96"/>
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.35">
@@ -3649,16 +3648,16 @@
       <c r="T58" s="81"/>
       <c r="U58" s="84"/>
       <c r="V58" s="81"/>
-      <c r="W58" s="114"/>
+      <c r="W58" s="113"/>
       <c r="X58" s="81"/>
       <c r="Y58" s="82"/>
       <c r="Z58" s="83"/>
       <c r="AA58" s="84"/>
       <c r="AB58" s="81"/>
       <c r="AC58" s="81"/>
-      <c r="AD58" s="95"/>
-      <c r="AE58" s="96"/>
-      <c r="AF58" s="97"/>
+      <c r="AD58" s="94"/>
+      <c r="AE58" s="95"/>
+      <c r="AF58" s="96"/>
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.35">
@@ -3691,9 +3690,9 @@
       <c r="AA59" s="84"/>
       <c r="AB59" s="81"/>
       <c r="AC59" s="81"/>
-      <c r="AD59" s="95"/>
-      <c r="AE59" s="96"/>
-      <c r="AF59" s="97"/>
+      <c r="AD59" s="94"/>
+      <c r="AE59" s="95"/>
+      <c r="AF59" s="96"/>
       <c r="AG59" s="10"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.35">
@@ -3726,8 +3725,8 @@
       <c r="AA60" s="66"/>
       <c r="AB60" s="63"/>
       <c r="AC60" s="63"/>
-      <c r="AD60" s="101"/>
-      <c r="AE60" s="102"/>
+      <c r="AD60" s="100"/>
+      <c r="AE60" s="101"/>
       <c r="AF60" s="56"/>
       <c r="AG60" s="10"/>
     </row>
@@ -3761,9 +3760,9 @@
       <c r="AA61" s="76"/>
       <c r="AB61" s="74"/>
       <c r="AC61" s="74"/>
-      <c r="AD61" s="92"/>
-      <c r="AE61" s="93"/>
-      <c r="AF61" s="94"/>
+      <c r="AD61" s="91"/>
+      <c r="AE61" s="92"/>
+      <c r="AF61" s="93"/>
       <c r="AG61" s="10"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.35">
@@ -3798,9 +3797,9 @@
       <c r="AA62" s="84"/>
       <c r="AB62" s="81"/>
       <c r="AC62" s="81"/>
-      <c r="AD62" s="95"/>
-      <c r="AE62" s="96"/>
-      <c r="AF62" s="97"/>
+      <c r="AD62" s="94"/>
+      <c r="AE62" s="95"/>
+      <c r="AF62" s="96"/>
       <c r="AG62" s="10"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.35">
@@ -3829,7 +3828,7 @@
       <c r="U63" s="84"/>
       <c r="V63" s="81"/>
       <c r="W63" s="81"/>
-      <c r="X63" s="114">
+      <c r="X63" s="113">
         <v>1</v>
       </c>
       <c r="Y63" s="82"/>
@@ -3837,9 +3836,9 @@
       <c r="AA63" s="84"/>
       <c r="AB63" s="81"/>
       <c r="AC63" s="81"/>
-      <c r="AD63" s="95"/>
-      <c r="AE63" s="96"/>
-      <c r="AF63" s="97"/>
+      <c r="AD63" s="94"/>
+      <c r="AE63" s="95"/>
+      <c r="AF63" s="96"/>
       <c r="AG63" s="10"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.35">
@@ -3872,9 +3871,9 @@
       <c r="AA64" s="84"/>
       <c r="AB64" s="81"/>
       <c r="AC64" s="81"/>
-      <c r="AD64" s="95"/>
-      <c r="AE64" s="96"/>
-      <c r="AF64" s="97"/>
+      <c r="AD64" s="94"/>
+      <c r="AE64" s="95"/>
+      <c r="AF64" s="96"/>
       <c r="AG64" s="10"/>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
@@ -3890,7 +3889,7 @@
       <c r="F65" s="15"/>
       <c r="G65" s="16"/>
       <c r="H65" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="6"/>
@@ -3913,9 +3912,9 @@
       <c r="AA65" s="84"/>
       <c r="AB65" s="81"/>
       <c r="AC65" s="81"/>
-      <c r="AD65" s="95"/>
-      <c r="AE65" s="96"/>
-      <c r="AF65" s="97"/>
+      <c r="AD65" s="94"/>
+      <c r="AE65" s="95"/>
+      <c r="AF65" s="96"/>
       <c r="AG65" s="10"/>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
@@ -3945,16 +3944,16 @@
       <c r="V66" s="81"/>
       <c r="W66" s="81"/>
       <c r="X66" s="81"/>
-      <c r="Y66" s="120">
+      <c r="Y66" s="119">
         <v>1</v>
       </c>
       <c r="Z66" s="83"/>
       <c r="AA66" s="84"/>
       <c r="AB66" s="81"/>
       <c r="AC66" s="81"/>
-      <c r="AD66" s="95"/>
-      <c r="AE66" s="96"/>
-      <c r="AF66" s="97"/>
+      <c r="AD66" s="94"/>
+      <c r="AE66" s="95"/>
+      <c r="AF66" s="96"/>
       <c r="AG66" s="10"/>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
@@ -3987,9 +3986,9 @@
       <c r="AA67" s="69"/>
       <c r="AB67" s="68"/>
       <c r="AC67" s="68"/>
-      <c r="AD67" s="98"/>
-      <c r="AE67" s="99"/>
-      <c r="AF67" s="100"/>
+      <c r="AD67" s="97"/>
+      <c r="AE67" s="98"/>
+      <c r="AF67" s="99"/>
       <c r="AG67" s="10"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
@@ -4024,9 +4023,9 @@
       <c r="AA68" s="84"/>
       <c r="AB68" s="81"/>
       <c r="AC68" s="81"/>
-      <c r="AD68" s="95"/>
-      <c r="AE68" s="96"/>
-      <c r="AF68" s="97"/>
+      <c r="AD68" s="94"/>
+      <c r="AE68" s="95"/>
+      <c r="AF68" s="96"/>
       <c r="AG68" s="10"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
@@ -4055,15 +4054,15 @@
       <c r="U69" s="84"/>
       <c r="V69" s="81"/>
       <c r="W69" s="81"/>
-      <c r="X69" s="114"/>
+      <c r="X69" s="113"/>
       <c r="Y69" s="82"/>
       <c r="Z69" s="83"/>
       <c r="AA69" s="84"/>
       <c r="AB69" s="81"/>
       <c r="AC69" s="81"/>
-      <c r="AD69" s="95"/>
-      <c r="AE69" s="96"/>
-      <c r="AF69" s="97"/>
+      <c r="AD69" s="94"/>
+      <c r="AE69" s="95"/>
+      <c r="AF69" s="96"/>
       <c r="AG69" s="10"/>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
@@ -4096,8 +4095,8 @@
       <c r="AA70" s="66"/>
       <c r="AB70" s="63"/>
       <c r="AC70" s="63"/>
-      <c r="AD70" s="101"/>
-      <c r="AE70" s="102"/>
+      <c r="AD70" s="100"/>
+      <c r="AE70" s="101"/>
       <c r="AF70" s="56"/>
       <c r="AG70" s="10"/>
     </row>
@@ -4107,7 +4106,7 @@
       <c r="C71" s="42"/>
       <c r="D71" s="43"/>
       <c r="E71" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F71" s="15"/>
       <c r="G71" s="16"/>
@@ -4133,9 +4132,9 @@
       <c r="AA71" s="76"/>
       <c r="AB71" s="74"/>
       <c r="AC71" s="74"/>
-      <c r="AD71" s="92"/>
-      <c r="AE71" s="93"/>
-      <c r="AF71" s="94"/>
+      <c r="AD71" s="91"/>
+      <c r="AE71" s="92"/>
+      <c r="AF71" s="93"/>
       <c r="AG71" s="10"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
@@ -4145,7 +4144,7 @@
       <c r="D72" s="46"/>
       <c r="E72" s="14"/>
       <c r="F72" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G72" s="16"/>
       <c r="H72" s="4"/>
@@ -4170,9 +4169,9 @@
       <c r="AA72" s="84"/>
       <c r="AB72" s="81"/>
       <c r="AC72" s="81"/>
-      <c r="AD72" s="95"/>
-      <c r="AE72" s="96"/>
-      <c r="AF72" s="97"/>
+      <c r="AD72" s="94"/>
+      <c r="AE72" s="95"/>
+      <c r="AF72" s="96"/>
       <c r="AG72" s="10"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
@@ -4181,7 +4180,7 @@
       <c r="C73" s="45"/>
       <c r="D73" s="46"/>
       <c r="E73" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="16"/>
@@ -4207,9 +4206,9 @@
       <c r="AA73" s="84"/>
       <c r="AB73" s="81"/>
       <c r="AC73" s="81"/>
-      <c r="AD73" s="95"/>
-      <c r="AE73" s="96"/>
-      <c r="AF73" s="97"/>
+      <c r="AD73" s="94"/>
+      <c r="AE73" s="95"/>
+      <c r="AF73" s="96"/>
       <c r="AG73" s="10"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
@@ -4221,16 +4220,16 @@
       <c r="D74" s="46"/>
       <c r="E74" s="14"/>
       <c r="F74" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G74" s="16"/>
       <c r="H74" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="39"/>
-      <c r="L74" s="117"/>
+      <c r="L74" s="116"/>
       <c r="M74" s="81"/>
       <c r="N74" s="81"/>
       <c r="O74" s="81"/>
@@ -4248,9 +4247,9 @@
       <c r="AA74" s="84"/>
       <c r="AB74" s="81"/>
       <c r="AC74" s="81"/>
-      <c r="AD74" s="108"/>
-      <c r="AE74" s="95"/>
-      <c r="AF74" s="97"/>
+      <c r="AD74" s="107"/>
+      <c r="AE74" s="94"/>
+      <c r="AF74" s="96"/>
       <c r="AG74" s="10"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
@@ -4260,7 +4259,7 @@
       <c r="D75" s="46"/>
       <c r="E75" s="14"/>
       <c r="F75" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G75" s="16"/>
       <c r="H75" s="4"/>
@@ -4273,21 +4272,21 @@
       <c r="O75" s="81"/>
       <c r="P75" s="81"/>
       <c r="Q75" s="81"/>
-      <c r="R75" s="90"/>
+      <c r="R75" s="89"/>
       <c r="S75" s="83"/>
       <c r="T75" s="81"/>
       <c r="U75" s="84"/>
       <c r="V75" s="81"/>
       <c r="W75" s="81"/>
       <c r="X75" s="81"/>
-      <c r="Y75" s="90"/>
+      <c r="Y75" s="89"/>
       <c r="Z75" s="83"/>
       <c r="AA75" s="84"/>
       <c r="AB75" s="81"/>
-      <c r="AC75" s="107"/>
-      <c r="AD75" s="109"/>
-      <c r="AE75" s="96"/>
-      <c r="AF75" s="90"/>
+      <c r="AC75" s="106"/>
+      <c r="AD75" s="108"/>
+      <c r="AE75" s="95"/>
+      <c r="AF75" s="89"/>
       <c r="AG75" s="10"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
@@ -4320,9 +4319,9 @@
       <c r="AA76" s="84"/>
       <c r="AB76" s="81"/>
       <c r="AC76" s="81"/>
-      <c r="AD76" s="98"/>
-      <c r="AE76" s="95"/>
-      <c r="AF76" s="106"/>
+      <c r="AD76" s="97"/>
+      <c r="AE76" s="94"/>
+      <c r="AF76" s="105"/>
       <c r="AG76" s="10"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
@@ -4331,7 +4330,7 @@
       <c r="C77" s="45"/>
       <c r="D77" s="46"/>
       <c r="E77" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F77" s="24"/>
       <c r="G77" s="16"/>
@@ -4357,9 +4356,9 @@
       <c r="AA77" s="84"/>
       <c r="AB77" s="81"/>
       <c r="AC77" s="81"/>
-      <c r="AD77" s="95"/>
-      <c r="AE77" s="108"/>
-      <c r="AF77" s="106"/>
+      <c r="AD77" s="94"/>
+      <c r="AE77" s="107"/>
+      <c r="AF77" s="105"/>
       <c r="AG77" s="10"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
@@ -4369,7 +4368,7 @@
       <c r="D78" s="46"/>
       <c r="E78" s="28"/>
       <c r="F78" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G78" s="14"/>
       <c r="H78" s="4"/>
@@ -4378,25 +4377,25 @@
       <c r="K78" s="70"/>
       <c r="L78" s="80"/>
       <c r="M78" s="85"/>
-      <c r="N78" s="114"/>
-      <c r="O78" s="114"/>
-      <c r="P78" s="114"/>
-      <c r="Q78" s="114"/>
-      <c r="R78" s="114"/>
-      <c r="S78" s="117"/>
+      <c r="N78" s="113"/>
+      <c r="O78" s="113"/>
+      <c r="P78" s="113"/>
+      <c r="Q78" s="113"/>
+      <c r="R78" s="113"/>
+      <c r="S78" s="116"/>
       <c r="T78" s="85"/>
-      <c r="U78" s="118"/>
+      <c r="U78" s="117"/>
       <c r="V78" s="85"/>
       <c r="W78" s="85"/>
       <c r="X78" s="85"/>
-      <c r="Y78" s="119"/>
-      <c r="Z78" s="117"/>
-      <c r="AA78" s="114"/>
-      <c r="AB78" s="114"/>
+      <c r="Y78" s="118"/>
+      <c r="Z78" s="116"/>
+      <c r="AA78" s="113"/>
+      <c r="AB78" s="113"/>
       <c r="AC78" s="85"/>
-      <c r="AD78" s="113"/>
+      <c r="AD78" s="112"/>
       <c r="AE78" s="57"/>
-      <c r="AF78" s="90"/>
+      <c r="AF78" s="89"/>
       <c r="AG78" s="10"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
@@ -4429,9 +4428,9 @@
       <c r="AA79" s="63"/>
       <c r="AB79" s="63"/>
       <c r="AC79" s="63"/>
-      <c r="AD79" s="111"/>
-      <c r="AE79" s="101"/>
-      <c r="AF79" s="112"/>
+      <c r="AD79" s="110"/>
+      <c r="AE79" s="100"/>
+      <c r="AF79" s="111"/>
       <c r="AG79" s="10"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
@@ -4442,7 +4441,7 @@
       </c>
       <c r="D80" s="43"/>
       <c r="E80" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="13"/>
@@ -4456,21 +4455,21 @@
       <c r="O80" s="74"/>
       <c r="P80" s="74"/>
       <c r="Q80" s="74"/>
-      <c r="R80" s="91"/>
+      <c r="R80" s="90"/>
       <c r="S80" s="76"/>
       <c r="T80" s="74"/>
       <c r="U80" s="74"/>
       <c r="V80" s="74"/>
       <c r="W80" s="74"/>
       <c r="X80" s="74"/>
-      <c r="Y80" s="91"/>
+      <c r="Y80" s="90"/>
       <c r="Z80" s="76"/>
       <c r="AA80" s="74"/>
       <c r="AB80" s="74"/>
       <c r="AC80" s="74"/>
-      <c r="AD80" s="98"/>
-      <c r="AE80" s="98"/>
-      <c r="AF80" s="110"/>
+      <c r="AD80" s="97"/>
+      <c r="AE80" s="97"/>
+      <c r="AF80" s="109"/>
       <c r="AG80" s="10"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
@@ -4480,11 +4479,11 @@
       <c r="D81" s="48"/>
       <c r="E81" s="17"/>
       <c r="F81" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G81" s="19"/>
       <c r="H81" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I81" s="8"/>
       <c r="J81" s="9"/>
@@ -4507,9 +4506,9 @@
       <c r="AA81" s="67"/>
       <c r="AB81" s="67"/>
       <c r="AC81" s="63"/>
-      <c r="AD81" s="111"/>
-      <c r="AE81" s="111"/>
-      <c r="AF81" s="112"/>
+      <c r="AD81" s="110"/>
+      <c r="AE81" s="110"/>
+      <c r="AF81" s="111"/>
       <c r="AG81" s="10"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
@@ -4584,41 +4583,41 @@
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C87" s="57"/>
       <c r="D87" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C88" s="58"/>
       <c r="D88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C89" s="105"/>
+      <c r="C89" s="104"/>
       <c r="D89" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C90" s="109"/>
+      <c r="C90" s="108"/>
       <c r="D90" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entrega final de laboratorio
</commit_message>
<xml_diff>
--- a/Documentos/Diagrama_de_Gantt.xlsx
+++ b/Documentos/Diagrama_de_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNAM\CompuGrafica\PROYECTO-FINAL-LAB\Versiones\Pachanga-Time\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3601DD8-6166-47CE-B0A9-8196CA863B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B40056-704E-42B2-AB81-3713C016BEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{CD2DF5CE-EA37-41C2-90D3-98A5F8E8DB04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -914,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1017,7 +1017,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1039,9 +1038,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1065,7 +1061,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1073,6 +1068,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5964B6-8B39-4F3E-95F0-A3E27A75FB75}">
   <dimension ref="A2:AX92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="Q34" sqref="G33:Q34"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1697,27 +1695,27 @@
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="38"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="75"/>
-      <c r="S6" s="73"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="76"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
-      <c r="X6" s="74"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="73"/>
-      <c r="AA6" s="76"/>
-      <c r="AB6" s="74"/>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="91"/>
-      <c r="AE6" s="92"/>
-      <c r="AF6" s="93"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="73"/>
+      <c r="Y6" s="74"/>
+      <c r="Z6" s="72"/>
+      <c r="AA6" s="75"/>
+      <c r="AB6" s="73"/>
+      <c r="AC6" s="73"/>
+      <c r="AD6" s="87"/>
+      <c r="AE6" s="88"/>
+      <c r="AF6" s="89"/>
       <c r="AG6" s="10"/>
     </row>
     <row r="7" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1734,27 +1732,27 @@
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
       <c r="K7" s="39"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="83"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="82"/>
-      <c r="Z7" s="83"/>
-      <c r="AA7" s="84"/>
-      <c r="AB7" s="81"/>
-      <c r="AC7" s="85"/>
-      <c r="AD7" s="94"/>
-      <c r="AE7" s="95"/>
-      <c r="AF7" s="96"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="82"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="90"/>
+      <c r="AE7" s="91"/>
+      <c r="AF7" s="92"/>
       <c r="AG7" s="10"/>
     </row>
     <row r="8" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1771,27 +1769,27 @@
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
       <c r="K8" s="39"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="78"/>
-      <c r="Z8" s="77"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="68"/>
-      <c r="AC8" s="79"/>
-      <c r="AD8" s="97"/>
-      <c r="AE8" s="98"/>
-      <c r="AF8" s="99"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="77"/>
+      <c r="Z8" s="76"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="78"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="94"/>
+      <c r="AF8" s="95"/>
       <c r="AG8" s="10"/>
     </row>
     <row r="9" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1808,27 +1806,27 @@
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
       <c r="K9" s="39"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="83"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="84"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="83"/>
-      <c r="AA9" s="84"/>
-      <c r="AB9" s="81"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="94"/>
-      <c r="AE9" s="95"/>
-      <c r="AF9" s="96"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="84"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="82"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="82"/>
+      <c r="AA9" s="83"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
+      <c r="AD9" s="90"/>
+      <c r="AE9" s="91"/>
+      <c r="AF9" s="92"/>
       <c r="AG9" s="10"/>
     </row>
     <row r="10" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1843,27 +1841,27 @@
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="83"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="84"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="82"/>
-      <c r="Z10" s="83"/>
-      <c r="AA10" s="84"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="81"/>
-      <c r="AD10" s="94"/>
-      <c r="AE10" s="95"/>
-      <c r="AF10" s="96"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="80"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="80"/>
+      <c r="W10" s="80"/>
+      <c r="X10" s="80"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="83"/>
+      <c r="AB10" s="80"/>
+      <c r="AC10" s="80"/>
+      <c r="AD10" s="90"/>
+      <c r="AE10" s="91"/>
+      <c r="AF10" s="92"/>
       <c r="AG10" s="10"/>
     </row>
     <row r="11" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1880,27 +1878,27 @@
       <c r="I11" s="5"/>
       <c r="J11" s="6"/>
       <c r="K11" s="39"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="82"/>
-      <c r="S11" s="83"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="84"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
-      <c r="Y11" s="82"/>
-      <c r="Z11" s="83"/>
-      <c r="AA11" s="84"/>
-      <c r="AB11" s="81"/>
-      <c r="AC11" s="81"/>
-      <c r="AD11" s="94"/>
-      <c r="AE11" s="95"/>
-      <c r="AF11" s="96"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="82"/>
+      <c r="T11" s="80"/>
+      <c r="U11" s="83"/>
+      <c r="V11" s="80"/>
+      <c r="W11" s="80"/>
+      <c r="X11" s="80"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="83"/>
+      <c r="AB11" s="80"/>
+      <c r="AC11" s="80"/>
+      <c r="AD11" s="90"/>
+      <c r="AE11" s="91"/>
+      <c r="AF11" s="92"/>
       <c r="AG11" s="10"/>
     </row>
     <row r="12" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1917,27 +1915,27 @@
       <c r="I12" s="5"/>
       <c r="J12" s="6"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="82"/>
-      <c r="S12" s="83"/>
-      <c r="T12" s="81"/>
-      <c r="U12" s="84"/>
-      <c r="V12" s="81"/>
-      <c r="W12" s="81"/>
-      <c r="X12" s="81"/>
-      <c r="Y12" s="82"/>
-      <c r="Z12" s="83"/>
-      <c r="AA12" s="84"/>
-      <c r="AB12" s="81"/>
-      <c r="AC12" s="81"/>
-      <c r="AD12" s="94"/>
-      <c r="AE12" s="95"/>
-      <c r="AF12" s="96"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="83"/>
+      <c r="V12" s="80"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="83"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
+      <c r="AD12" s="90"/>
+      <c r="AE12" s="91"/>
+      <c r="AF12" s="92"/>
       <c r="AG12" s="10"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
@@ -1954,27 +1952,27 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="39"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="83"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="82"/>
-      <c r="Z13" s="83"/>
-      <c r="AA13" s="84"/>
-      <c r="AB13" s="81"/>
-      <c r="AC13" s="81"/>
-      <c r="AD13" s="94"/>
-      <c r="AE13" s="95"/>
-      <c r="AF13" s="96"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="84"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="82"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="83"/>
+      <c r="V13" s="80"/>
+      <c r="W13" s="80"/>
+      <c r="X13" s="80"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="82"/>
+      <c r="AA13" s="83"/>
+      <c r="AB13" s="80"/>
+      <c r="AC13" s="80"/>
+      <c r="AD13" s="90"/>
+      <c r="AE13" s="91"/>
+      <c r="AF13" s="92"/>
       <c r="AG13" s="10"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
@@ -1989,27 +1987,27 @@
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="81"/>
-      <c r="U14" s="84"/>
-      <c r="V14" s="81"/>
-      <c r="W14" s="81"/>
-      <c r="X14" s="81"/>
-      <c r="Y14" s="82"/>
-      <c r="Z14" s="83"/>
-      <c r="AA14" s="84"/>
-      <c r="AB14" s="81"/>
-      <c r="AC14" s="81"/>
-      <c r="AD14" s="94"/>
-      <c r="AE14" s="95"/>
-      <c r="AF14" s="96"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="81"/>
+      <c r="S14" s="82"/>
+      <c r="T14" s="80"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="80"/>
+      <c r="W14" s="80"/>
+      <c r="X14" s="80"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="82"/>
+      <c r="AA14" s="83"/>
+      <c r="AB14" s="80"/>
+      <c r="AC14" s="80"/>
+      <c r="AD14" s="90"/>
+      <c r="AE14" s="91"/>
+      <c r="AF14" s="92"/>
       <c r="AG14" s="10"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
@@ -2026,27 +2024,27 @@
       <c r="I15" s="5"/>
       <c r="J15" s="6"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="84"/>
-      <c r="V15" s="81"/>
-      <c r="W15" s="81"/>
-      <c r="X15" s="81"/>
-      <c r="Y15" s="82"/>
-      <c r="Z15" s="83"/>
-      <c r="AA15" s="84"/>
-      <c r="AB15" s="81"/>
-      <c r="AC15" s="81"/>
-      <c r="AD15" s="94"/>
-      <c r="AE15" s="95"/>
-      <c r="AF15" s="96"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="81"/>
+      <c r="S15" s="82"/>
+      <c r="T15" s="80"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="80"/>
+      <c r="W15" s="80"/>
+      <c r="X15" s="80"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="82"/>
+      <c r="AA15" s="83"/>
+      <c r="AB15" s="80"/>
+      <c r="AC15" s="80"/>
+      <c r="AD15" s="90"/>
+      <c r="AE15" s="91"/>
+      <c r="AF15" s="92"/>
       <c r="AG15" s="10"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
@@ -2063,29 +2061,29 @@
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="116">
+      <c r="L16" s="111">
         <v>1</v>
       </c>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="83"/>
-      <c r="T16" s="81"/>
-      <c r="U16" s="84"/>
-      <c r="V16" s="81"/>
-      <c r="W16" s="81"/>
-      <c r="X16" s="81"/>
-      <c r="Y16" s="82"/>
-      <c r="Z16" s="83"/>
-      <c r="AA16" s="84"/>
-      <c r="AB16" s="81"/>
-      <c r="AC16" s="81"/>
-      <c r="AD16" s="94"/>
-      <c r="AE16" s="95"/>
-      <c r="AF16" s="96"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
+      <c r="S16" s="82"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="83"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="83"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="90"/>
+      <c r="AE16" s="91"/>
+      <c r="AF16" s="92"/>
       <c r="AG16" s="10"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
@@ -2102,27 +2100,27 @@
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
       <c r="K17" s="39"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="113"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="83"/>
-      <c r="T17" s="81"/>
-      <c r="U17" s="84"/>
-      <c r="V17" s="81"/>
-      <c r="W17" s="81"/>
-      <c r="X17" s="81"/>
-      <c r="Y17" s="82"/>
-      <c r="Z17" s="83"/>
-      <c r="AA17" s="84"/>
-      <c r="AB17" s="81"/>
-      <c r="AC17" s="81"/>
-      <c r="AD17" s="94"/>
-      <c r="AE17" s="95"/>
-      <c r="AF17" s="96"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="80"/>
+      <c r="U17" s="83"/>
+      <c r="V17" s="80"/>
+      <c r="W17" s="80"/>
+      <c r="X17" s="80"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="83"/>
+      <c r="AB17" s="80"/>
+      <c r="AC17" s="80"/>
+      <c r="AD17" s="90"/>
+      <c r="AE17" s="91"/>
+      <c r="AF17" s="92"/>
       <c r="AG17" s="10"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
@@ -2141,27 +2139,27 @@
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="113"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="83"/>
-      <c r="T18" s="81"/>
-      <c r="U18" s="84"/>
-      <c r="V18" s="81"/>
-      <c r="W18" s="81"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="83"/>
-      <c r="AA18" s="84"/>
-      <c r="AB18" s="81"/>
-      <c r="AC18" s="81"/>
-      <c r="AD18" s="94"/>
-      <c r="AE18" s="95"/>
-      <c r="AF18" s="96"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="81"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="80"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="80"/>
+      <c r="W18" s="80"/>
+      <c r="X18" s="80"/>
+      <c r="Y18" s="81"/>
+      <c r="Z18" s="82"/>
+      <c r="AA18" s="83"/>
+      <c r="AB18" s="80"/>
+      <c r="AC18" s="80"/>
+      <c r="AD18" s="90"/>
+      <c r="AE18" s="91"/>
+      <c r="AF18" s="92"/>
       <c r="AG18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.35">
@@ -2178,27 +2176,27 @@
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="82"/>
-      <c r="S19" s="83"/>
-      <c r="T19" s="81"/>
-      <c r="U19" s="84"/>
-      <c r="V19" s="81"/>
-      <c r="W19" s="81"/>
-      <c r="X19" s="81"/>
-      <c r="Y19" s="82"/>
-      <c r="Z19" s="83"/>
-      <c r="AA19" s="84"/>
-      <c r="AB19" s="81"/>
-      <c r="AC19" s="81"/>
-      <c r="AD19" s="94"/>
-      <c r="AE19" s="95"/>
-      <c r="AF19" s="96"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="81"/>
+      <c r="S19" s="82"/>
+      <c r="T19" s="80"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="80"/>
+      <c r="W19" s="80"/>
+      <c r="X19" s="80"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="82"/>
+      <c r="AA19" s="83"/>
+      <c r="AB19" s="80"/>
+      <c r="AC19" s="80"/>
+      <c r="AD19" s="90"/>
+      <c r="AE19" s="91"/>
+      <c r="AF19" s="92"/>
       <c r="AG19" s="10"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
@@ -2215,27 +2213,27 @@
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
       <c r="K20" s="39"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="83"/>
-      <c r="T20" s="81"/>
-      <c r="U20" s="84"/>
-      <c r="V20" s="81"/>
-      <c r="W20" s="81"/>
-      <c r="X20" s="81"/>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="84"/>
-      <c r="AB20" s="81"/>
-      <c r="AC20" s="81"/>
-      <c r="AD20" s="94"/>
-      <c r="AE20" s="95"/>
-      <c r="AF20" s="96"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="81"/>
+      <c r="S20" s="82"/>
+      <c r="T20" s="80"/>
+      <c r="U20" s="83"/>
+      <c r="V20" s="80"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="80"/>
+      <c r="Y20" s="81"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="83"/>
+      <c r="AB20" s="80"/>
+      <c r="AC20" s="80"/>
+      <c r="AD20" s="90"/>
+      <c r="AE20" s="91"/>
+      <c r="AF20" s="92"/>
       <c r="AG20" s="10"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
@@ -2254,27 +2252,27 @@
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="39"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="113"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="82"/>
-      <c r="S21" s="83"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="84"/>
-      <c r="V21" s="81"/>
-      <c r="W21" s="81"/>
-      <c r="X21" s="81"/>
-      <c r="Y21" s="82"/>
-      <c r="Z21" s="83"/>
-      <c r="AA21" s="84"/>
-      <c r="AB21" s="81"/>
-      <c r="AC21" s="81"/>
-      <c r="AD21" s="94"/>
-      <c r="AE21" s="95"/>
-      <c r="AF21" s="96"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="81"/>
+      <c r="S21" s="82"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="83"/>
+      <c r="V21" s="80"/>
+      <c r="W21" s="80"/>
+      <c r="X21" s="80"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="82"/>
+      <c r="AA21" s="83"/>
+      <c r="AB21" s="80"/>
+      <c r="AC21" s="80"/>
+      <c r="AD21" s="90"/>
+      <c r="AE21" s="91"/>
+      <c r="AF21" s="92"/>
       <c r="AG21" s="10"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
@@ -2291,27 +2289,27 @@
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
       <c r="K22" s="39"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="113"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="82"/>
-      <c r="S22" s="83"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="84"/>
-      <c r="V22" s="81"/>
-      <c r="W22" s="81"/>
-      <c r="X22" s="81"/>
-      <c r="Y22" s="82"/>
-      <c r="Z22" s="83"/>
-      <c r="AA22" s="84"/>
-      <c r="AB22" s="81"/>
-      <c r="AC22" s="81"/>
-      <c r="AD22" s="94"/>
-      <c r="AE22" s="95"/>
-      <c r="AF22" s="96"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="108"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="81"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="80"/>
+      <c r="W22" s="80"/>
+      <c r="X22" s="80"/>
+      <c r="Y22" s="81"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="83"/>
+      <c r="AB22" s="80"/>
+      <c r="AC22" s="80"/>
+      <c r="AD22" s="90"/>
+      <c r="AE22" s="91"/>
+      <c r="AF22" s="92"/>
       <c r="AG22" s="10"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
@@ -2328,27 +2326,27 @@
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="113"/>
-      <c r="O23" s="81"/>
-      <c r="P23" s="81"/>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="81"/>
-      <c r="U23" s="84"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
-      <c r="X23" s="81"/>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="83"/>
-      <c r="AA23" s="84"/>
-      <c r="AB23" s="81"/>
-      <c r="AC23" s="81"/>
-      <c r="AD23" s="94"/>
-      <c r="AE23" s="95"/>
-      <c r="AF23" s="96"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="81"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="80"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="80"/>
+      <c r="W23" s="80"/>
+      <c r="X23" s="80"/>
+      <c r="Y23" s="81"/>
+      <c r="Z23" s="82"/>
+      <c r="AA23" s="83"/>
+      <c r="AB23" s="80"/>
+      <c r="AC23" s="80"/>
+      <c r="AD23" s="90"/>
+      <c r="AE23" s="91"/>
+      <c r="AF23" s="92"/>
       <c r="AG23" s="10"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
@@ -2365,27 +2363,27 @@
       <c r="I24" s="5"/>
       <c r="J24" s="6"/>
       <c r="K24" s="39"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="113"/>
-      <c r="O24" s="81"/>
-      <c r="P24" s="81"/>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="82"/>
-      <c r="S24" s="83"/>
-      <c r="T24" s="81"/>
-      <c r="U24" s="84"/>
-      <c r="V24" s="81"/>
-      <c r="W24" s="81"/>
-      <c r="X24" s="81"/>
-      <c r="Y24" s="82"/>
-      <c r="Z24" s="83"/>
-      <c r="AA24" s="84"/>
-      <c r="AB24" s="81"/>
-      <c r="AC24" s="81"/>
-      <c r="AD24" s="94"/>
-      <c r="AE24" s="95"/>
-      <c r="AF24" s="96"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="108"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="82"/>
+      <c r="T24" s="80"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="80"/>
+      <c r="W24" s="80"/>
+      <c r="X24" s="80"/>
+      <c r="Y24" s="81"/>
+      <c r="Z24" s="82"/>
+      <c r="AA24" s="83"/>
+      <c r="AB24" s="80"/>
+      <c r="AC24" s="80"/>
+      <c r="AD24" s="90"/>
+      <c r="AE24" s="91"/>
+      <c r="AF24" s="92"/>
       <c r="AG24" s="10"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
@@ -2402,27 +2400,27 @@
       <c r="I25" s="5"/>
       <c r="J25" s="6"/>
       <c r="K25" s="39"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="81"/>
-      <c r="O25" s="113"/>
-      <c r="P25" s="81"/>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="81"/>
-      <c r="U25" s="84"/>
-      <c r="V25" s="81"/>
-      <c r="W25" s="81"/>
-      <c r="X25" s="81"/>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="83"/>
-      <c r="AA25" s="84"/>
-      <c r="AB25" s="81"/>
-      <c r="AC25" s="81"/>
-      <c r="AD25" s="94"/>
-      <c r="AE25" s="95"/>
-      <c r="AF25" s="96"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="80"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="82"/>
+      <c r="T25" s="80"/>
+      <c r="U25" s="83"/>
+      <c r="V25" s="80"/>
+      <c r="W25" s="80"/>
+      <c r="X25" s="80"/>
+      <c r="Y25" s="81"/>
+      <c r="Z25" s="82"/>
+      <c r="AA25" s="83"/>
+      <c r="AB25" s="80"/>
+      <c r="AC25" s="80"/>
+      <c r="AD25" s="90"/>
+      <c r="AE25" s="91"/>
+      <c r="AF25" s="92"/>
       <c r="AG25" s="10"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
@@ -2439,27 +2437,27 @@
       <c r="I26" s="5"/>
       <c r="J26" s="6"/>
       <c r="K26" s="39"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="81"/>
-      <c r="O26" s="113"/>
-      <c r="P26" s="81"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="82"/>
-      <c r="S26" s="83"/>
-      <c r="T26" s="81"/>
-      <c r="U26" s="84"/>
-      <c r="V26" s="81"/>
-      <c r="W26" s="81"/>
-      <c r="X26" s="81"/>
-      <c r="Y26" s="82"/>
-      <c r="Z26" s="83"/>
-      <c r="AA26" s="84"/>
-      <c r="AB26" s="81"/>
-      <c r="AC26" s="81"/>
-      <c r="AD26" s="94"/>
-      <c r="AE26" s="95"/>
-      <c r="AF26" s="96"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="81"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="80"/>
+      <c r="U26" s="83"/>
+      <c r="V26" s="80"/>
+      <c r="W26" s="80"/>
+      <c r="X26" s="80"/>
+      <c r="Y26" s="81"/>
+      <c r="Z26" s="82"/>
+      <c r="AA26" s="83"/>
+      <c r="AB26" s="80"/>
+      <c r="AC26" s="80"/>
+      <c r="AD26" s="90"/>
+      <c r="AE26" s="91"/>
+      <c r="AF26" s="92"/>
       <c r="AG26" s="10"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
@@ -2476,27 +2474,27 @@
       <c r="I27" s="5"/>
       <c r="J27" s="6"/>
       <c r="K27" s="39"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="81"/>
-      <c r="N27" s="81"/>
-      <c r="O27" s="113"/>
-      <c r="P27" s="81"/>
-      <c r="Q27" s="81"/>
-      <c r="R27" s="82"/>
-      <c r="S27" s="83"/>
-      <c r="T27" s="81"/>
-      <c r="U27" s="84"/>
-      <c r="V27" s="81"/>
-      <c r="W27" s="81"/>
-      <c r="X27" s="81"/>
-      <c r="Y27" s="82"/>
-      <c r="Z27" s="83"/>
-      <c r="AA27" s="84"/>
-      <c r="AB27" s="81"/>
-      <c r="AC27" s="81"/>
-      <c r="AD27" s="94"/>
-      <c r="AE27" s="95"/>
-      <c r="AF27" s="96"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="108"/>
+      <c r="P27" s="80"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="81"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="80"/>
+      <c r="U27" s="83"/>
+      <c r="V27" s="80"/>
+      <c r="W27" s="80"/>
+      <c r="X27" s="80"/>
+      <c r="Y27" s="81"/>
+      <c r="Z27" s="82"/>
+      <c r="AA27" s="83"/>
+      <c r="AB27" s="80"/>
+      <c r="AC27" s="80"/>
+      <c r="AD27" s="90"/>
+      <c r="AE27" s="91"/>
+      <c r="AF27" s="92"/>
       <c r="AG27" s="10"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
@@ -2513,27 +2511,27 @@
       <c r="I28" s="5"/>
       <c r="J28" s="6"/>
       <c r="K28" s="39"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="113"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="81"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="83"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="84"/>
-      <c r="V28" s="81"/>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="82"/>
-      <c r="Z28" s="83"/>
-      <c r="AA28" s="84"/>
-      <c r="AB28" s="81"/>
-      <c r="AC28" s="81"/>
-      <c r="AD28" s="94"/>
-      <c r="AE28" s="95"/>
-      <c r="AF28" s="96"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="80"/>
+      <c r="Q28" s="80"/>
+      <c r="R28" s="81"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="80"/>
+      <c r="U28" s="83"/>
+      <c r="V28" s="80"/>
+      <c r="W28" s="80"/>
+      <c r="X28" s="80"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="82"/>
+      <c r="AA28" s="83"/>
+      <c r="AB28" s="80"/>
+      <c r="AC28" s="80"/>
+      <c r="AD28" s="90"/>
+      <c r="AE28" s="91"/>
+      <c r="AF28" s="92"/>
       <c r="AG28" s="10"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.35">
@@ -2550,27 +2548,27 @@
       <c r="I29" s="5"/>
       <c r="J29" s="6"/>
       <c r="K29" s="39"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="113"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="83"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="84"/>
-      <c r="V29" s="81"/>
-      <c r="W29" s="81"/>
-      <c r="X29" s="81"/>
-      <c r="Y29" s="82"/>
-      <c r="Z29" s="83"/>
-      <c r="AA29" s="84"/>
-      <c r="AB29" s="81"/>
-      <c r="AC29" s="81"/>
-      <c r="AD29" s="94"/>
-      <c r="AE29" s="95"/>
-      <c r="AF29" s="96"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="80"/>
+      <c r="U29" s="83"/>
+      <c r="V29" s="80"/>
+      <c r="W29" s="80"/>
+      <c r="X29" s="80"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="82"/>
+      <c r="AA29" s="83"/>
+      <c r="AB29" s="80"/>
+      <c r="AC29" s="80"/>
+      <c r="AD29" s="90"/>
+      <c r="AE29" s="91"/>
+      <c r="AF29" s="92"/>
       <c r="AG29" s="10"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
@@ -2587,27 +2585,27 @@
       <c r="I30" s="5"/>
       <c r="J30" s="6"/>
       <c r="K30" s="39"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="83"/>
-      <c r="T30" s="81"/>
-      <c r="U30" s="84"/>
-      <c r="V30" s="81"/>
-      <c r="W30" s="81"/>
-      <c r="X30" s="81"/>
-      <c r="Y30" s="82"/>
-      <c r="Z30" s="83"/>
-      <c r="AA30" s="84"/>
-      <c r="AB30" s="81"/>
-      <c r="AC30" s="81"/>
-      <c r="AD30" s="94"/>
-      <c r="AE30" s="95"/>
-      <c r="AF30" s="96"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="80"/>
+      <c r="Q30" s="80"/>
+      <c r="R30" s="81"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="80"/>
+      <c r="U30" s="83"/>
+      <c r="V30" s="80"/>
+      <c r="W30" s="80"/>
+      <c r="X30" s="80"/>
+      <c r="Y30" s="81"/>
+      <c r="Z30" s="82"/>
+      <c r="AA30" s="83"/>
+      <c r="AB30" s="80"/>
+      <c r="AC30" s="80"/>
+      <c r="AD30" s="90"/>
+      <c r="AE30" s="91"/>
+      <c r="AF30" s="92"/>
       <c r="AG30" s="10"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
@@ -2628,22 +2626,22 @@
       <c r="M31" s="63"/>
       <c r="N31" s="63"/>
       <c r="O31" s="63"/>
-      <c r="P31" s="64"/>
+      <c r="P31" s="117"/>
       <c r="Q31" s="63"/>
       <c r="R31" s="54"/>
       <c r="S31" s="60"/>
       <c r="T31" s="63"/>
-      <c r="U31" s="66"/>
+      <c r="U31" s="65"/>
       <c r="V31" s="63"/>
       <c r="W31" s="63"/>
       <c r="X31" s="63"/>
       <c r="Y31" s="54"/>
       <c r="Z31" s="60"/>
-      <c r="AA31" s="66"/>
+      <c r="AA31" s="65"/>
       <c r="AB31" s="63"/>
       <c r="AC31" s="63"/>
-      <c r="AD31" s="100"/>
-      <c r="AE31" s="101"/>
+      <c r="AD31" s="96"/>
+      <c r="AE31" s="97"/>
       <c r="AF31" s="56"/>
       <c r="AG31" s="10"/>
     </row>
@@ -2661,27 +2659,27 @@
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="39"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="73"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="76"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="74"/>
-      <c r="X32" s="74"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="73"/>
-      <c r="AA32" s="76"/>
-      <c r="AB32" s="74"/>
-      <c r="AC32" s="74"/>
-      <c r="AD32" s="91"/>
-      <c r="AE32" s="92"/>
-      <c r="AF32" s="93"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="74"/>
+      <c r="S32" s="72"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="75"/>
+      <c r="V32" s="73"/>
+      <c r="W32" s="73"/>
+      <c r="X32" s="73"/>
+      <c r="Y32" s="74"/>
+      <c r="Z32" s="72"/>
+      <c r="AA32" s="75"/>
+      <c r="AB32" s="73"/>
+      <c r="AC32" s="73"/>
+      <c r="AD32" s="87"/>
+      <c r="AE32" s="88"/>
+      <c r="AF32" s="89"/>
       <c r="AG32" s="10"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
@@ -2698,27 +2696,27 @@
       <c r="I33" s="5"/>
       <c r="J33" s="6"/>
       <c r="K33" s="39"/>
-      <c r="L33" s="83"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="86"/>
-      <c r="R33" s="82"/>
-      <c r="S33" s="83"/>
-      <c r="T33" s="81"/>
-      <c r="U33" s="84"/>
-      <c r="V33" s="81"/>
-      <c r="W33" s="81"/>
-      <c r="X33" s="81"/>
-      <c r="Y33" s="82"/>
-      <c r="Z33" s="83"/>
-      <c r="AA33" s="84"/>
-      <c r="AB33" s="81"/>
-      <c r="AC33" s="81"/>
-      <c r="AD33" s="94"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="96"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="81"/>
+      <c r="S33" s="82"/>
+      <c r="T33" s="80"/>
+      <c r="U33" s="83"/>
+      <c r="V33" s="80"/>
+      <c r="W33" s="80"/>
+      <c r="X33" s="80"/>
+      <c r="Y33" s="81"/>
+      <c r="Z33" s="82"/>
+      <c r="AA33" s="83"/>
+      <c r="AB33" s="80"/>
+      <c r="AC33" s="80"/>
+      <c r="AD33" s="90"/>
+      <c r="AE33" s="91"/>
+      <c r="AF33" s="92"/>
       <c r="AG33" s="10"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.35">
@@ -2735,27 +2733,27 @@
       <c r="I34" s="5"/>
       <c r="J34" s="6"/>
       <c r="K34" s="39"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="86"/>
-      <c r="R34" s="82"/>
-      <c r="S34" s="83"/>
-      <c r="T34" s="81"/>
-      <c r="U34" s="84"/>
-      <c r="V34" s="81"/>
-      <c r="W34" s="81"/>
-      <c r="X34" s="81"/>
-      <c r="Y34" s="82"/>
-      <c r="Z34" s="83"/>
-      <c r="AA34" s="84"/>
-      <c r="AB34" s="81"/>
-      <c r="AC34" s="81"/>
-      <c r="AD34" s="94"/>
-      <c r="AE34" s="95"/>
-      <c r="AF34" s="96"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="82"/>
+      <c r="T34" s="80"/>
+      <c r="U34" s="83"/>
+      <c r="V34" s="80"/>
+      <c r="W34" s="80"/>
+      <c r="X34" s="80"/>
+      <c r="Y34" s="81"/>
+      <c r="Z34" s="82"/>
+      <c r="AA34" s="83"/>
+      <c r="AB34" s="80"/>
+      <c r="AC34" s="80"/>
+      <c r="AD34" s="90"/>
+      <c r="AE34" s="91"/>
+      <c r="AF34" s="92"/>
       <c r="AG34" s="10"/>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.35">
@@ -2772,27 +2770,27 @@
       <c r="I35" s="5"/>
       <c r="J35" s="6"/>
       <c r="K35" s="39"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="82"/>
-      <c r="S35" s="83"/>
-      <c r="T35" s="81"/>
-      <c r="U35" s="84"/>
-      <c r="V35" s="81"/>
-      <c r="W35" s="81"/>
-      <c r="X35" s="81"/>
-      <c r="Y35" s="82"/>
-      <c r="Z35" s="83"/>
-      <c r="AA35" s="84"/>
-      <c r="AB35" s="81"/>
-      <c r="AC35" s="81"/>
-      <c r="AD35" s="94"/>
-      <c r="AE35" s="95"/>
-      <c r="AF35" s="96"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="81"/>
+      <c r="S35" s="82"/>
+      <c r="T35" s="80"/>
+      <c r="U35" s="83"/>
+      <c r="V35" s="80"/>
+      <c r="W35" s="80"/>
+      <c r="X35" s="80"/>
+      <c r="Y35" s="81"/>
+      <c r="Z35" s="82"/>
+      <c r="AA35" s="83"/>
+      <c r="AB35" s="80"/>
+      <c r="AC35" s="80"/>
+      <c r="AD35" s="90"/>
+      <c r="AE35" s="91"/>
+      <c r="AF35" s="92"/>
       <c r="AG35" s="10"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.35">
@@ -2811,27 +2809,27 @@
       <c r="I36" s="5"/>
       <c r="J36" s="6"/>
       <c r="K36" s="39"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="81"/>
-      <c r="N36" s="81"/>
-      <c r="O36" s="81"/>
-      <c r="P36" s="81"/>
-      <c r="Q36" s="81"/>
-      <c r="R36" s="82"/>
-      <c r="S36" s="83"/>
-      <c r="T36" s="81"/>
-      <c r="U36" s="84"/>
-      <c r="V36" s="81"/>
-      <c r="W36" s="81"/>
-      <c r="X36" s="81"/>
-      <c r="Y36" s="82"/>
-      <c r="Z36" s="83"/>
-      <c r="AA36" s="84"/>
-      <c r="AB36" s="81"/>
-      <c r="AC36" s="81"/>
-      <c r="AD36" s="94"/>
-      <c r="AE36" s="95"/>
-      <c r="AF36" s="96"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="80"/>
+      <c r="Q36" s="80"/>
+      <c r="R36" s="81"/>
+      <c r="S36" s="82"/>
+      <c r="T36" s="80"/>
+      <c r="U36" s="83"/>
+      <c r="V36" s="80"/>
+      <c r="W36" s="80"/>
+      <c r="X36" s="80"/>
+      <c r="Y36" s="81"/>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="83"/>
+      <c r="AB36" s="80"/>
+      <c r="AC36" s="80"/>
+      <c r="AD36" s="90"/>
+      <c r="AE36" s="91"/>
+      <c r="AF36" s="92"/>
       <c r="AG36" s="10"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.35">
@@ -2848,27 +2846,27 @@
       <c r="I37" s="5"/>
       <c r="J37" s="6"/>
       <c r="K37" s="39"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="81"/>
-      <c r="N37" s="81"/>
-      <c r="O37" s="81"/>
-      <c r="P37" s="81"/>
-      <c r="Q37" s="81"/>
-      <c r="R37" s="114"/>
-      <c r="S37" s="83"/>
-      <c r="T37" s="81"/>
-      <c r="U37" s="84"/>
-      <c r="V37" s="81"/>
-      <c r="W37" s="81"/>
-      <c r="X37" s="81"/>
-      <c r="Y37" s="82"/>
-      <c r="Z37" s="83"/>
-      <c r="AA37" s="84"/>
-      <c r="AB37" s="81"/>
-      <c r="AC37" s="81"/>
-      <c r="AD37" s="94"/>
-      <c r="AE37" s="95"/>
-      <c r="AF37" s="96"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="80"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="80"/>
+      <c r="Q37" s="80"/>
+      <c r="R37" s="109"/>
+      <c r="S37" s="82"/>
+      <c r="T37" s="80"/>
+      <c r="U37" s="83"/>
+      <c r="V37" s="80"/>
+      <c r="W37" s="80"/>
+      <c r="X37" s="80"/>
+      <c r="Y37" s="81"/>
+      <c r="Z37" s="82"/>
+      <c r="AA37" s="83"/>
+      <c r="AB37" s="80"/>
+      <c r="AC37" s="80"/>
+      <c r="AD37" s="90"/>
+      <c r="AE37" s="91"/>
+      <c r="AF37" s="92"/>
       <c r="AG37" s="10"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.35">
@@ -2891,20 +2889,20 @@
       <c r="O38" s="61"/>
       <c r="P38" s="61"/>
       <c r="Q38" s="61"/>
-      <c r="R38" s="115"/>
+      <c r="R38" s="110"/>
       <c r="S38" s="59"/>
       <c r="T38" s="61"/>
-      <c r="U38" s="65"/>
+      <c r="U38" s="64"/>
       <c r="V38" s="61"/>
       <c r="W38" s="61"/>
       <c r="X38" s="61"/>
       <c r="Y38" s="53"/>
       <c r="Z38" s="59"/>
-      <c r="AA38" s="65"/>
+      <c r="AA38" s="64"/>
       <c r="AB38" s="61"/>
       <c r="AC38" s="61"/>
-      <c r="AD38" s="102"/>
-      <c r="AE38" s="103"/>
+      <c r="AD38" s="98"/>
+      <c r="AE38" s="99"/>
       <c r="AF38" s="55"/>
       <c r="AG38" s="10"/>
     </row>
@@ -2929,17 +2927,17 @@
       <c r="R39" s="54"/>
       <c r="S39" s="60"/>
       <c r="T39" s="63"/>
-      <c r="U39" s="66"/>
+      <c r="U39" s="65"/>
       <c r="V39" s="63"/>
       <c r="W39" s="63"/>
       <c r="X39" s="63"/>
       <c r="Y39" s="54"/>
       <c r="Z39" s="60"/>
-      <c r="AA39" s="66"/>
+      <c r="AA39" s="65"/>
       <c r="AB39" s="63"/>
       <c r="AC39" s="63"/>
-      <c r="AD39" s="100"/>
-      <c r="AE39" s="101"/>
+      <c r="AD39" s="96"/>
+      <c r="AE39" s="97"/>
       <c r="AF39" s="56"/>
       <c r="AG39" s="10"/>
     </row>
@@ -2957,27 +2955,27 @@
       <c r="I40" s="2"/>
       <c r="J40" s="3"/>
       <c r="K40" s="39"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="74"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="75"/>
-      <c r="S40" s="73"/>
-      <c r="T40" s="74"/>
-      <c r="U40" s="76"/>
-      <c r="V40" s="74"/>
-      <c r="W40" s="74"/>
-      <c r="X40" s="74"/>
-      <c r="Y40" s="75"/>
-      <c r="Z40" s="73"/>
-      <c r="AA40" s="76"/>
-      <c r="AB40" s="74"/>
-      <c r="AC40" s="74"/>
-      <c r="AD40" s="91"/>
-      <c r="AE40" s="92"/>
-      <c r="AF40" s="93"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
+      <c r="Q40" s="73"/>
+      <c r="R40" s="74"/>
+      <c r="S40" s="72"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="75"/>
+      <c r="V40" s="73"/>
+      <c r="W40" s="73"/>
+      <c r="X40" s="73"/>
+      <c r="Y40" s="74"/>
+      <c r="Z40" s="72"/>
+      <c r="AA40" s="75"/>
+      <c r="AB40" s="73"/>
+      <c r="AC40" s="73"/>
+      <c r="AD40" s="87"/>
+      <c r="AE40" s="88"/>
+      <c r="AF40" s="89"/>
       <c r="AG40" s="10"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.35">
@@ -2994,27 +2992,27 @@
       <c r="I41" s="5"/>
       <c r="J41" s="6"/>
       <c r="K41" s="39"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="81"/>
-      <c r="N41" s="81"/>
-      <c r="O41" s="81"/>
-      <c r="P41" s="81"/>
-      <c r="Q41" s="81"/>
-      <c r="R41" s="82"/>
-      <c r="S41" s="87"/>
-      <c r="T41" s="81"/>
-      <c r="U41" s="84"/>
-      <c r="V41" s="81"/>
-      <c r="W41" s="81"/>
-      <c r="X41" s="81"/>
-      <c r="Y41" s="82"/>
-      <c r="Z41" s="83"/>
-      <c r="AA41" s="84"/>
-      <c r="AB41" s="81"/>
-      <c r="AC41" s="81"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="95"/>
-      <c r="AF41" s="96"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="80"/>
+      <c r="O41" s="80"/>
+      <c r="P41" s="80"/>
+      <c r="Q41" s="80"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="111"/>
+      <c r="T41" s="80"/>
+      <c r="U41" s="83"/>
+      <c r="V41" s="80"/>
+      <c r="W41" s="80"/>
+      <c r="X41" s="80"/>
+      <c r="Y41" s="81"/>
+      <c r="Z41" s="82"/>
+      <c r="AA41" s="83"/>
+      <c r="AB41" s="80"/>
+      <c r="AC41" s="80"/>
+      <c r="AD41" s="90"/>
+      <c r="AE41" s="91"/>
+      <c r="AF41" s="92"/>
       <c r="AG41" s="10"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.35">
@@ -3029,27 +3027,27 @@
       <c r="I42" s="5"/>
       <c r="J42" s="6"/>
       <c r="K42" s="39"/>
-      <c r="L42" s="83"/>
-      <c r="M42" s="81"/>
-      <c r="N42" s="81"/>
-      <c r="O42" s="81"/>
-      <c r="P42" s="81"/>
-      <c r="Q42" s="81"/>
-      <c r="R42" s="82"/>
-      <c r="S42" s="83"/>
-      <c r="T42" s="81"/>
-      <c r="U42" s="84"/>
-      <c r="V42" s="81"/>
-      <c r="W42" s="81"/>
-      <c r="X42" s="81"/>
-      <c r="Y42" s="82"/>
-      <c r="Z42" s="83"/>
-      <c r="AA42" s="84"/>
-      <c r="AB42" s="81"/>
-      <c r="AC42" s="81"/>
-      <c r="AD42" s="94"/>
-      <c r="AE42" s="95"/>
-      <c r="AF42" s="96"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="80"/>
+      <c r="N42" s="80"/>
+      <c r="O42" s="80"/>
+      <c r="P42" s="80"/>
+      <c r="Q42" s="80"/>
+      <c r="R42" s="81"/>
+      <c r="S42" s="82"/>
+      <c r="T42" s="80"/>
+      <c r="U42" s="83"/>
+      <c r="V42" s="80"/>
+      <c r="W42" s="80"/>
+      <c r="X42" s="80"/>
+      <c r="Y42" s="81"/>
+      <c r="Z42" s="82"/>
+      <c r="AA42" s="83"/>
+      <c r="AB42" s="80"/>
+      <c r="AC42" s="80"/>
+      <c r="AD42" s="90"/>
+      <c r="AE42" s="91"/>
+      <c r="AF42" s="92"/>
       <c r="AG42" s="10"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.35">
@@ -3066,27 +3064,27 @@
       <c r="I43" s="5"/>
       <c r="J43" s="6"/>
       <c r="K43" s="39"/>
-      <c r="L43" s="83"/>
-      <c r="M43" s="81"/>
-      <c r="N43" s="81"/>
-      <c r="O43" s="81"/>
-      <c r="P43" s="81"/>
-      <c r="Q43" s="81"/>
-      <c r="R43" s="82"/>
-      <c r="S43" s="83"/>
-      <c r="T43" s="81"/>
-      <c r="U43" s="84"/>
-      <c r="V43" s="81"/>
-      <c r="W43" s="81"/>
-      <c r="X43" s="81"/>
-      <c r="Y43" s="82"/>
-      <c r="Z43" s="83"/>
-      <c r="AA43" s="84"/>
-      <c r="AB43" s="81"/>
-      <c r="AC43" s="81"/>
-      <c r="AD43" s="94"/>
-      <c r="AE43" s="95"/>
-      <c r="AF43" s="96"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
+      <c r="Q43" s="80"/>
+      <c r="R43" s="81"/>
+      <c r="S43" s="82"/>
+      <c r="T43" s="80"/>
+      <c r="U43" s="83"/>
+      <c r="V43" s="80"/>
+      <c r="W43" s="80"/>
+      <c r="X43" s="80"/>
+      <c r="Y43" s="81"/>
+      <c r="Z43" s="82"/>
+      <c r="AA43" s="83"/>
+      <c r="AB43" s="80"/>
+      <c r="AC43" s="80"/>
+      <c r="AD43" s="90"/>
+      <c r="AE43" s="91"/>
+      <c r="AF43" s="92"/>
       <c r="AG43" s="10"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.35">
@@ -3103,31 +3101,31 @@
       <c r="I44" s="5"/>
       <c r="J44" s="6"/>
       <c r="K44" s="39"/>
-      <c r="L44" s="83"/>
-      <c r="M44" s="81"/>
-      <c r="N44" s="81"/>
-      <c r="O44" s="81"/>
-      <c r="P44" s="81"/>
-      <c r="Q44" s="81"/>
-      <c r="R44" s="82"/>
-      <c r="S44" s="83"/>
-      <c r="T44" s="81" t="s">
+      <c r="L44" s="82"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="80"/>
+      <c r="O44" s="80"/>
+      <c r="P44" s="80"/>
+      <c r="Q44" s="80"/>
+      <c r="R44" s="81"/>
+      <c r="S44" s="82"/>
+      <c r="T44" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="U44" s="113">
+      <c r="U44" s="108">
         <v>1</v>
       </c>
-      <c r="V44" s="81"/>
-      <c r="W44" s="81"/>
-      <c r="X44" s="81"/>
-      <c r="Y44" s="82"/>
-      <c r="Z44" s="83"/>
-      <c r="AA44" s="84"/>
-      <c r="AB44" s="81"/>
-      <c r="AC44" s="81"/>
-      <c r="AD44" s="94"/>
-      <c r="AE44" s="95"/>
-      <c r="AF44" s="96"/>
+      <c r="V44" s="80"/>
+      <c r="W44" s="80"/>
+      <c r="X44" s="80"/>
+      <c r="Y44" s="81"/>
+      <c r="Z44" s="82"/>
+      <c r="AA44" s="83"/>
+      <c r="AB44" s="80"/>
+      <c r="AC44" s="80"/>
+      <c r="AD44" s="90"/>
+      <c r="AE44" s="91"/>
+      <c r="AF44" s="92"/>
       <c r="AG44" s="10"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
@@ -3144,27 +3142,27 @@
       <c r="I45" s="5"/>
       <c r="J45" s="6"/>
       <c r="K45" s="39"/>
-      <c r="L45" s="83"/>
-      <c r="M45" s="81"/>
-      <c r="N45" s="81"/>
-      <c r="O45" s="81"/>
-      <c r="P45" s="81"/>
-      <c r="Q45" s="81"/>
-      <c r="R45" s="82"/>
-      <c r="S45" s="83"/>
-      <c r="T45" s="81"/>
-      <c r="U45" s="85"/>
-      <c r="V45" s="81"/>
-      <c r="W45" s="81"/>
-      <c r="X45" s="81"/>
-      <c r="Y45" s="82"/>
-      <c r="Z45" s="83"/>
-      <c r="AA45" s="84"/>
-      <c r="AB45" s="81"/>
-      <c r="AC45" s="81"/>
-      <c r="AD45" s="94"/>
-      <c r="AE45" s="95"/>
-      <c r="AF45" s="96"/>
+      <c r="L45" s="82"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="81"/>
+      <c r="S45" s="82"/>
+      <c r="T45" s="80"/>
+      <c r="U45" s="108"/>
+      <c r="V45" s="80"/>
+      <c r="W45" s="80"/>
+      <c r="X45" s="80"/>
+      <c r="Y45" s="81"/>
+      <c r="Z45" s="82"/>
+      <c r="AA45" s="83"/>
+      <c r="AB45" s="80"/>
+      <c r="AC45" s="80"/>
+      <c r="AD45" s="90"/>
+      <c r="AE45" s="91"/>
+      <c r="AF45" s="92"/>
       <c r="AG45" s="10"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.35">
@@ -3185,29 +3183,29 @@
       <c r="I46" s="5"/>
       <c r="J46" s="6"/>
       <c r="K46" s="39"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="81"/>
-      <c r="N46" s="81"/>
-      <c r="O46" s="81"/>
-      <c r="P46" s="81"/>
-      <c r="Q46" s="81"/>
-      <c r="R46" s="82"/>
-      <c r="S46" s="83"/>
-      <c r="T46" s="81"/>
-      <c r="U46" s="113">
+      <c r="L46" s="82"/>
+      <c r="M46" s="80"/>
+      <c r="N46" s="80"/>
+      <c r="O46" s="80"/>
+      <c r="P46" s="80"/>
+      <c r="Q46" s="80"/>
+      <c r="R46" s="81"/>
+      <c r="S46" s="82"/>
+      <c r="T46" s="80"/>
+      <c r="U46" s="108">
         <v>1</v>
       </c>
-      <c r="V46" s="81"/>
-      <c r="W46" s="81"/>
-      <c r="X46" s="81"/>
-      <c r="Y46" s="82"/>
-      <c r="Z46" s="83"/>
-      <c r="AA46" s="84"/>
-      <c r="AB46" s="81"/>
-      <c r="AC46" s="81"/>
-      <c r="AD46" s="94"/>
-      <c r="AE46" s="95"/>
-      <c r="AF46" s="96"/>
+      <c r="V46" s="80"/>
+      <c r="W46" s="80"/>
+      <c r="X46" s="80"/>
+      <c r="Y46" s="81"/>
+      <c r="Z46" s="82"/>
+      <c r="AA46" s="83"/>
+      <c r="AB46" s="80"/>
+      <c r="AC46" s="80"/>
+      <c r="AD46" s="90"/>
+      <c r="AE46" s="91"/>
+      <c r="AF46" s="92"/>
       <c r="AG46" s="10"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.35">
@@ -3224,27 +3222,27 @@
       <c r="I47" s="5"/>
       <c r="J47" s="6"/>
       <c r="K47" s="39"/>
-      <c r="L47" s="83"/>
-      <c r="M47" s="81"/>
-      <c r="N47" s="81"/>
-      <c r="O47" s="81"/>
-      <c r="P47" s="81"/>
-      <c r="Q47" s="81"/>
-      <c r="R47" s="82"/>
-      <c r="S47" s="83"/>
-      <c r="T47" s="81"/>
-      <c r="U47" s="84"/>
-      <c r="V47" s="81"/>
-      <c r="W47" s="81"/>
-      <c r="X47" s="81"/>
-      <c r="Y47" s="82"/>
-      <c r="Z47" s="83"/>
-      <c r="AA47" s="84"/>
-      <c r="AB47" s="81"/>
-      <c r="AC47" s="81"/>
-      <c r="AD47" s="94"/>
-      <c r="AE47" s="95"/>
-      <c r="AF47" s="96"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="80"/>
+      <c r="N47" s="80"/>
+      <c r="O47" s="80"/>
+      <c r="P47" s="80"/>
+      <c r="Q47" s="80"/>
+      <c r="R47" s="81"/>
+      <c r="S47" s="82"/>
+      <c r="T47" s="80"/>
+      <c r="U47" s="83"/>
+      <c r="V47" s="80"/>
+      <c r="W47" s="80"/>
+      <c r="X47" s="80"/>
+      <c r="Y47" s="81"/>
+      <c r="Z47" s="82"/>
+      <c r="AA47" s="83"/>
+      <c r="AB47" s="80"/>
+      <c r="AC47" s="80"/>
+      <c r="AD47" s="90"/>
+      <c r="AE47" s="91"/>
+      <c r="AF47" s="92"/>
       <c r="AG47" s="10"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.35">
@@ -3261,29 +3259,29 @@
       <c r="I48" s="5"/>
       <c r="J48" s="6"/>
       <c r="K48" s="39"/>
-      <c r="L48" s="83"/>
-      <c r="M48" s="81"/>
-      <c r="N48" s="81"/>
-      <c r="O48" s="81"/>
-      <c r="P48" s="81"/>
-      <c r="Q48" s="81"/>
-      <c r="R48" s="82"/>
-      <c r="S48" s="83" t="s">
+      <c r="L48" s="82"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="80"/>
+      <c r="O48" s="80"/>
+      <c r="P48" s="80"/>
+      <c r="Q48" s="80"/>
+      <c r="R48" s="81"/>
+      <c r="S48" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="T48" s="88"/>
-      <c r="U48" s="84"/>
-      <c r="V48" s="81"/>
-      <c r="W48" s="81"/>
-      <c r="X48" s="81"/>
-      <c r="Y48" s="82"/>
-      <c r="Z48" s="83"/>
-      <c r="AA48" s="84"/>
-      <c r="AB48" s="81"/>
-      <c r="AC48" s="81"/>
-      <c r="AD48" s="94"/>
-      <c r="AE48" s="95"/>
-      <c r="AF48" s="96"/>
+      <c r="T48" s="113"/>
+      <c r="U48" s="83"/>
+      <c r="V48" s="80"/>
+      <c r="W48" s="80"/>
+      <c r="X48" s="80"/>
+      <c r="Y48" s="81"/>
+      <c r="Z48" s="82"/>
+      <c r="AA48" s="83"/>
+      <c r="AB48" s="80"/>
+      <c r="AC48" s="80"/>
+      <c r="AD48" s="90"/>
+      <c r="AE48" s="91"/>
+      <c r="AF48" s="92"/>
       <c r="AG48" s="10"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.35">
@@ -3300,29 +3298,29 @@
       <c r="I49" s="5"/>
       <c r="J49" s="6"/>
       <c r="K49" s="39"/>
-      <c r="L49" s="83"/>
-      <c r="M49" s="81"/>
-      <c r="N49" s="81"/>
-      <c r="O49" s="81"/>
-      <c r="P49" s="81"/>
-      <c r="Q49" s="81"/>
-      <c r="R49" s="82"/>
-      <c r="S49" s="83"/>
-      <c r="T49" s="88">
+      <c r="L49" s="82"/>
+      <c r="M49" s="80"/>
+      <c r="N49" s="80"/>
+      <c r="O49" s="80"/>
+      <c r="P49" s="80"/>
+      <c r="Q49" s="80"/>
+      <c r="R49" s="81"/>
+      <c r="S49" s="82"/>
+      <c r="T49" s="113">
         <v>1</v>
       </c>
-      <c r="U49" s="84"/>
-      <c r="V49" s="81"/>
-      <c r="W49" s="81"/>
-      <c r="X49" s="81"/>
-      <c r="Y49" s="82"/>
-      <c r="Z49" s="83"/>
-      <c r="AA49" s="84"/>
-      <c r="AB49" s="81"/>
-      <c r="AC49" s="81"/>
-      <c r="AD49" s="94"/>
-      <c r="AE49" s="95"/>
-      <c r="AF49" s="96"/>
+      <c r="U49" s="83"/>
+      <c r="V49" s="80"/>
+      <c r="W49" s="80"/>
+      <c r="X49" s="80"/>
+      <c r="Y49" s="81"/>
+      <c r="Z49" s="82"/>
+      <c r="AA49" s="83"/>
+      <c r="AB49" s="80"/>
+      <c r="AC49" s="80"/>
+      <c r="AD49" s="90"/>
+      <c r="AE49" s="91"/>
+      <c r="AF49" s="92"/>
       <c r="AG49" s="10"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.35">
@@ -3339,31 +3337,31 @@
       <c r="I50" s="5"/>
       <c r="J50" s="6"/>
       <c r="K50" s="39"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="81"/>
-      <c r="N50" s="81"/>
-      <c r="O50" s="81"/>
-      <c r="P50" s="81"/>
-      <c r="Q50" s="81"/>
-      <c r="R50" s="82"/>
-      <c r="S50" s="83"/>
-      <c r="T50" s="81"/>
-      <c r="U50" s="84" t="s">
+      <c r="L50" s="82"/>
+      <c r="M50" s="80"/>
+      <c r="N50" s="80"/>
+      <c r="O50" s="80"/>
+      <c r="P50" s="80"/>
+      <c r="Q50" s="80"/>
+      <c r="R50" s="81"/>
+      <c r="S50" s="82"/>
+      <c r="T50" s="80"/>
+      <c r="U50" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="V50" s="113">
+      <c r="V50" s="108">
         <v>1</v>
       </c>
-      <c r="W50" s="81"/>
-      <c r="X50" s="81"/>
-      <c r="Y50" s="82"/>
-      <c r="Z50" s="83"/>
-      <c r="AA50" s="84"/>
-      <c r="AB50" s="81"/>
-      <c r="AC50" s="81"/>
-      <c r="AD50" s="94"/>
-      <c r="AE50" s="95"/>
-      <c r="AF50" s="96"/>
+      <c r="W50" s="80"/>
+      <c r="X50" s="80"/>
+      <c r="Y50" s="81"/>
+      <c r="Z50" s="82"/>
+      <c r="AA50" s="83"/>
+      <c r="AB50" s="80"/>
+      <c r="AC50" s="80"/>
+      <c r="AD50" s="90"/>
+      <c r="AE50" s="91"/>
+      <c r="AF50" s="92"/>
       <c r="AG50" s="10"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.35">
@@ -3380,27 +3378,27 @@
       <c r="I51" s="5"/>
       <c r="J51" s="6"/>
       <c r="K51" s="39"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="81"/>
-      <c r="N51" s="81"/>
-      <c r="O51" s="81"/>
-      <c r="P51" s="81"/>
-      <c r="Q51" s="81"/>
-      <c r="R51" s="82"/>
-      <c r="S51" s="83"/>
-      <c r="T51" s="81"/>
-      <c r="U51" s="84"/>
-      <c r="V51" s="81"/>
-      <c r="W51" s="81"/>
-      <c r="X51" s="81"/>
-      <c r="Y51" s="82"/>
-      <c r="Z51" s="83"/>
-      <c r="AA51" s="84"/>
-      <c r="AB51" s="81"/>
-      <c r="AC51" s="81"/>
-      <c r="AD51" s="94"/>
-      <c r="AE51" s="95"/>
-      <c r="AF51" s="96"/>
+      <c r="L51" s="82"/>
+      <c r="M51" s="80"/>
+      <c r="N51" s="80"/>
+      <c r="O51" s="80"/>
+      <c r="P51" s="80"/>
+      <c r="Q51" s="80"/>
+      <c r="R51" s="81"/>
+      <c r="S51" s="82"/>
+      <c r="T51" s="80"/>
+      <c r="U51" s="83"/>
+      <c r="V51" s="80"/>
+      <c r="W51" s="80"/>
+      <c r="X51" s="80"/>
+      <c r="Y51" s="81"/>
+      <c r="Z51" s="82"/>
+      <c r="AA51" s="83"/>
+      <c r="AB51" s="80"/>
+      <c r="AC51" s="80"/>
+      <c r="AD51" s="90"/>
+      <c r="AE51" s="91"/>
+      <c r="AF51" s="92"/>
       <c r="AG51" s="10"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.35">
@@ -3426,17 +3424,17 @@
       <c r="R52" s="53"/>
       <c r="S52" s="59"/>
       <c r="T52" s="61"/>
-      <c r="U52" s="65"/>
+      <c r="U52" s="64"/>
       <c r="V52" s="62"/>
       <c r="W52" s="61"/>
       <c r="X52" s="61"/>
       <c r="Y52" s="53"/>
       <c r="Z52" s="59"/>
-      <c r="AA52" s="65"/>
+      <c r="AA52" s="64"/>
       <c r="AB52" s="61"/>
       <c r="AC52" s="61"/>
-      <c r="AD52" s="102"/>
-      <c r="AE52" s="103"/>
+      <c r="AD52" s="98"/>
+      <c r="AE52" s="99"/>
       <c r="AF52" s="55"/>
       <c r="AG52" s="10"/>
     </row>
@@ -3461,17 +3459,17 @@
       <c r="R53" s="53"/>
       <c r="S53" s="59"/>
       <c r="T53" s="61"/>
-      <c r="U53" s="65"/>
+      <c r="U53" s="64"/>
       <c r="V53" s="61"/>
       <c r="W53" s="61"/>
       <c r="X53" s="61"/>
       <c r="Y53" s="53"/>
       <c r="Z53" s="59"/>
-      <c r="AA53" s="65"/>
+      <c r="AA53" s="64"/>
       <c r="AB53" s="61"/>
       <c r="AC53" s="61"/>
-      <c r="AD53" s="102"/>
-      <c r="AE53" s="103"/>
+      <c r="AD53" s="98"/>
+      <c r="AE53" s="99"/>
       <c r="AF53" s="55"/>
       <c r="AG53" s="10"/>
     </row>
@@ -3496,17 +3494,17 @@
       <c r="R54" s="54"/>
       <c r="S54" s="60"/>
       <c r="T54" s="63"/>
-      <c r="U54" s="66"/>
+      <c r="U54" s="65"/>
       <c r="V54" s="63"/>
       <c r="W54" s="63"/>
       <c r="X54" s="63"/>
       <c r="Y54" s="54"/>
       <c r="Z54" s="60"/>
-      <c r="AA54" s="66"/>
+      <c r="AA54" s="65"/>
       <c r="AB54" s="63"/>
       <c r="AC54" s="63"/>
-      <c r="AD54" s="100"/>
-      <c r="AE54" s="101"/>
+      <c r="AD54" s="96"/>
+      <c r="AE54" s="97"/>
       <c r="AF54" s="56"/>
       <c r="AG54" s="10"/>
     </row>
@@ -3522,27 +3520,27 @@
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
       <c r="K55" s="38"/>
-      <c r="L55" s="73"/>
-      <c r="M55" s="74"/>
-      <c r="N55" s="74"/>
-      <c r="O55" s="74"/>
-      <c r="P55" s="74"/>
-      <c r="Q55" s="74"/>
-      <c r="R55" s="75"/>
-      <c r="S55" s="73"/>
-      <c r="T55" s="74"/>
-      <c r="U55" s="76"/>
-      <c r="V55" s="74"/>
-      <c r="W55" s="74"/>
-      <c r="X55" s="74"/>
-      <c r="Y55" s="75"/>
-      <c r="Z55" s="73"/>
-      <c r="AA55" s="76"/>
-      <c r="AB55" s="74"/>
-      <c r="AC55" s="74"/>
-      <c r="AD55" s="91"/>
-      <c r="AE55" s="92"/>
-      <c r="AF55" s="93"/>
+      <c r="L55" s="72"/>
+      <c r="M55" s="73"/>
+      <c r="N55" s="73"/>
+      <c r="O55" s="73"/>
+      <c r="P55" s="73"/>
+      <c r="Q55" s="73"/>
+      <c r="R55" s="74"/>
+      <c r="S55" s="72"/>
+      <c r="T55" s="73"/>
+      <c r="U55" s="75"/>
+      <c r="V55" s="73"/>
+      <c r="W55" s="73"/>
+      <c r="X55" s="73"/>
+      <c r="Y55" s="74"/>
+      <c r="Z55" s="72"/>
+      <c r="AA55" s="75"/>
+      <c r="AB55" s="73"/>
+      <c r="AC55" s="73"/>
+      <c r="AD55" s="87"/>
+      <c r="AE55" s="88"/>
+      <c r="AF55" s="89"/>
       <c r="AG55" s="10"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.35">
@@ -3559,27 +3557,27 @@
       <c r="I56" s="5"/>
       <c r="J56" s="6"/>
       <c r="K56" s="39"/>
-      <c r="L56" s="83"/>
-      <c r="M56" s="81"/>
-      <c r="N56" s="81"/>
-      <c r="O56" s="81"/>
-      <c r="P56" s="81"/>
-      <c r="Q56" s="81"/>
-      <c r="R56" s="82"/>
-      <c r="S56" s="83"/>
-      <c r="T56" s="81"/>
-      <c r="U56" s="84"/>
-      <c r="V56" s="81"/>
-      <c r="W56" s="81"/>
-      <c r="X56" s="81"/>
-      <c r="Y56" s="82"/>
-      <c r="Z56" s="83"/>
-      <c r="AA56" s="84"/>
-      <c r="AB56" s="81"/>
-      <c r="AC56" s="81"/>
-      <c r="AD56" s="94"/>
-      <c r="AE56" s="95"/>
-      <c r="AF56" s="96"/>
+      <c r="L56" s="82"/>
+      <c r="M56" s="80"/>
+      <c r="N56" s="80"/>
+      <c r="O56" s="80"/>
+      <c r="P56" s="80"/>
+      <c r="Q56" s="80"/>
+      <c r="R56" s="81"/>
+      <c r="S56" s="82"/>
+      <c r="T56" s="80"/>
+      <c r="U56" s="83"/>
+      <c r="V56" s="80"/>
+      <c r="W56" s="80"/>
+      <c r="X56" s="80"/>
+      <c r="Y56" s="81"/>
+      <c r="Z56" s="82"/>
+      <c r="AA56" s="83"/>
+      <c r="AB56" s="80"/>
+      <c r="AC56" s="80"/>
+      <c r="AD56" s="90"/>
+      <c r="AE56" s="91"/>
+      <c r="AF56" s="92"/>
       <c r="AG56" s="10"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.35">
@@ -3600,27 +3598,27 @@
       <c r="I57" s="5"/>
       <c r="J57" s="6"/>
       <c r="K57" s="39"/>
-      <c r="L57" s="83"/>
-      <c r="M57" s="81"/>
-      <c r="N57" s="81"/>
-      <c r="O57" s="81"/>
-      <c r="P57" s="81"/>
-      <c r="Q57" s="81"/>
-      <c r="R57" s="82"/>
-      <c r="S57" s="83"/>
-      <c r="T57" s="81"/>
-      <c r="U57" s="84"/>
-      <c r="V57" s="81"/>
-      <c r="W57" s="113"/>
-      <c r="X57" s="81"/>
-      <c r="Y57" s="82"/>
-      <c r="Z57" s="83"/>
-      <c r="AA57" s="84"/>
-      <c r="AB57" s="81"/>
-      <c r="AC57" s="81"/>
-      <c r="AD57" s="94"/>
-      <c r="AE57" s="95"/>
-      <c r="AF57" s="96"/>
+      <c r="L57" s="82"/>
+      <c r="M57" s="80"/>
+      <c r="N57" s="80"/>
+      <c r="O57" s="80"/>
+      <c r="P57" s="80"/>
+      <c r="Q57" s="80"/>
+      <c r="R57" s="81"/>
+      <c r="S57" s="82"/>
+      <c r="T57" s="80"/>
+      <c r="U57" s="83"/>
+      <c r="V57" s="80"/>
+      <c r="W57" s="108"/>
+      <c r="X57" s="80"/>
+      <c r="Y57" s="81"/>
+      <c r="Z57" s="82"/>
+      <c r="AA57" s="83"/>
+      <c r="AB57" s="80"/>
+      <c r="AC57" s="80"/>
+      <c r="AD57" s="90"/>
+      <c r="AE57" s="91"/>
+      <c r="AF57" s="92"/>
       <c r="AG57" s="10"/>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.35">
@@ -3637,27 +3635,27 @@
       <c r="I58" s="5"/>
       <c r="J58" s="6"/>
       <c r="K58" s="39"/>
-      <c r="L58" s="83"/>
-      <c r="M58" s="81"/>
-      <c r="N58" s="81"/>
-      <c r="O58" s="81"/>
-      <c r="P58" s="81"/>
-      <c r="Q58" s="81"/>
-      <c r="R58" s="82"/>
-      <c r="S58" s="83"/>
-      <c r="T58" s="81"/>
-      <c r="U58" s="84"/>
-      <c r="V58" s="81"/>
-      <c r="W58" s="113"/>
-      <c r="X58" s="81"/>
-      <c r="Y58" s="82"/>
-      <c r="Z58" s="83"/>
-      <c r="AA58" s="84"/>
-      <c r="AB58" s="81"/>
-      <c r="AC58" s="81"/>
-      <c r="AD58" s="94"/>
-      <c r="AE58" s="95"/>
-      <c r="AF58" s="96"/>
+      <c r="L58" s="82"/>
+      <c r="M58" s="80"/>
+      <c r="N58" s="80"/>
+      <c r="O58" s="80"/>
+      <c r="P58" s="80"/>
+      <c r="Q58" s="80"/>
+      <c r="R58" s="81"/>
+      <c r="S58" s="82"/>
+      <c r="T58" s="80"/>
+      <c r="U58" s="83"/>
+      <c r="V58" s="80"/>
+      <c r="W58" s="108"/>
+      <c r="X58" s="80"/>
+      <c r="Y58" s="81"/>
+      <c r="Z58" s="82"/>
+      <c r="AA58" s="83"/>
+      <c r="AB58" s="80"/>
+      <c r="AC58" s="80"/>
+      <c r="AD58" s="90"/>
+      <c r="AE58" s="91"/>
+      <c r="AF58" s="92"/>
       <c r="AG58" s="10"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.35">
@@ -3672,27 +3670,27 @@
       <c r="I59" s="5"/>
       <c r="J59" s="6"/>
       <c r="K59" s="39"/>
-      <c r="L59" s="83"/>
-      <c r="M59" s="81"/>
-      <c r="N59" s="81"/>
-      <c r="O59" s="81"/>
-      <c r="P59" s="81"/>
-      <c r="Q59" s="81"/>
-      <c r="R59" s="82"/>
-      <c r="S59" s="83"/>
-      <c r="T59" s="81"/>
-      <c r="U59" s="84"/>
-      <c r="V59" s="81"/>
-      <c r="W59" s="81"/>
-      <c r="X59" s="81"/>
-      <c r="Y59" s="82"/>
-      <c r="Z59" s="83"/>
-      <c r="AA59" s="84"/>
-      <c r="AB59" s="81"/>
-      <c r="AC59" s="81"/>
-      <c r="AD59" s="94"/>
-      <c r="AE59" s="95"/>
-      <c r="AF59" s="96"/>
+      <c r="L59" s="82"/>
+      <c r="M59" s="80"/>
+      <c r="N59" s="80"/>
+      <c r="O59" s="80"/>
+      <c r="P59" s="80"/>
+      <c r="Q59" s="80"/>
+      <c r="R59" s="81"/>
+      <c r="S59" s="82"/>
+      <c r="T59" s="80"/>
+      <c r="U59" s="83"/>
+      <c r="V59" s="80"/>
+      <c r="W59" s="80"/>
+      <c r="X59" s="80"/>
+      <c r="Y59" s="81"/>
+      <c r="Z59" s="82"/>
+      <c r="AA59" s="83"/>
+      <c r="AB59" s="80"/>
+      <c r="AC59" s="80"/>
+      <c r="AD59" s="90"/>
+      <c r="AE59" s="91"/>
+      <c r="AF59" s="92"/>
       <c r="AG59" s="10"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.35">
@@ -3716,17 +3714,17 @@
       <c r="R60" s="54"/>
       <c r="S60" s="60"/>
       <c r="T60" s="63"/>
-      <c r="U60" s="66"/>
+      <c r="U60" s="65"/>
       <c r="V60" s="63"/>
       <c r="W60" s="63"/>
       <c r="X60" s="63"/>
       <c r="Y60" s="54"/>
       <c r="Z60" s="60"/>
-      <c r="AA60" s="66"/>
+      <c r="AA60" s="65"/>
       <c r="AB60" s="63"/>
       <c r="AC60" s="63"/>
-      <c r="AD60" s="100"/>
-      <c r="AE60" s="101"/>
+      <c r="AD60" s="96"/>
+      <c r="AE60" s="97"/>
       <c r="AF60" s="56"/>
       <c r="AG60" s="10"/>
     </row>
@@ -3742,27 +3740,27 @@
       <c r="I61" s="5"/>
       <c r="J61" s="6"/>
       <c r="K61" s="39"/>
-      <c r="L61" s="73"/>
-      <c r="M61" s="74"/>
-      <c r="N61" s="74"/>
-      <c r="O61" s="74"/>
-      <c r="P61" s="74"/>
-      <c r="Q61" s="74"/>
-      <c r="R61" s="75"/>
-      <c r="S61" s="73"/>
-      <c r="T61" s="74"/>
-      <c r="U61" s="76"/>
-      <c r="V61" s="74"/>
-      <c r="W61" s="74"/>
-      <c r="X61" s="74"/>
-      <c r="Y61" s="75"/>
-      <c r="Z61" s="73"/>
-      <c r="AA61" s="76"/>
-      <c r="AB61" s="74"/>
-      <c r="AC61" s="74"/>
-      <c r="AD61" s="91"/>
-      <c r="AE61" s="92"/>
-      <c r="AF61" s="93"/>
+      <c r="L61" s="72"/>
+      <c r="M61" s="73"/>
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+      <c r="P61" s="73"/>
+      <c r="Q61" s="73"/>
+      <c r="R61" s="74"/>
+      <c r="S61" s="72"/>
+      <c r="T61" s="73"/>
+      <c r="U61" s="75"/>
+      <c r="V61" s="73"/>
+      <c r="W61" s="73"/>
+      <c r="X61" s="73"/>
+      <c r="Y61" s="74"/>
+      <c r="Z61" s="72"/>
+      <c r="AA61" s="75"/>
+      <c r="AB61" s="73"/>
+      <c r="AC61" s="73"/>
+      <c r="AD61" s="87"/>
+      <c r="AE61" s="88"/>
+      <c r="AF61" s="89"/>
       <c r="AG61" s="10"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.35">
@@ -3779,27 +3777,27 @@
       <c r="I62" s="5"/>
       <c r="J62" s="6"/>
       <c r="K62" s="39"/>
-      <c r="L62" s="83"/>
-      <c r="M62" s="81"/>
-      <c r="N62" s="81"/>
-      <c r="O62" s="81"/>
-      <c r="P62" s="81"/>
-      <c r="Q62" s="81"/>
-      <c r="R62" s="82"/>
-      <c r="S62" s="83"/>
-      <c r="T62" s="81"/>
-      <c r="U62" s="84"/>
-      <c r="V62" s="81"/>
-      <c r="W62" s="81"/>
-      <c r="X62" s="81"/>
-      <c r="Y62" s="82"/>
-      <c r="Z62" s="83"/>
-      <c r="AA62" s="84"/>
-      <c r="AB62" s="81"/>
-      <c r="AC62" s="81"/>
-      <c r="AD62" s="94"/>
-      <c r="AE62" s="95"/>
-      <c r="AF62" s="96"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="80"/>
+      <c r="N62" s="80"/>
+      <c r="O62" s="80"/>
+      <c r="P62" s="80"/>
+      <c r="Q62" s="80"/>
+      <c r="R62" s="81"/>
+      <c r="S62" s="82"/>
+      <c r="T62" s="80"/>
+      <c r="U62" s="83"/>
+      <c r="V62" s="80"/>
+      <c r="W62" s="80"/>
+      <c r="X62" s="80"/>
+      <c r="Y62" s="81"/>
+      <c r="Z62" s="82"/>
+      <c r="AA62" s="83"/>
+      <c r="AB62" s="80"/>
+      <c r="AC62" s="80"/>
+      <c r="AD62" s="90"/>
+      <c r="AE62" s="91"/>
+      <c r="AF62" s="92"/>
       <c r="AG62" s="10"/>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.35">
@@ -3816,29 +3814,29 @@
       <c r="I63" s="5"/>
       <c r="J63" s="6"/>
       <c r="K63" s="39"/>
-      <c r="L63" s="83"/>
-      <c r="M63" s="81"/>
-      <c r="N63" s="81"/>
-      <c r="O63" s="81"/>
-      <c r="P63" s="81"/>
-      <c r="Q63" s="81"/>
-      <c r="R63" s="82"/>
-      <c r="S63" s="83"/>
-      <c r="T63" s="81"/>
-      <c r="U63" s="84"/>
-      <c r="V63" s="81"/>
-      <c r="W63" s="81"/>
-      <c r="X63" s="113">
+      <c r="L63" s="82"/>
+      <c r="M63" s="80"/>
+      <c r="N63" s="80"/>
+      <c r="O63" s="80"/>
+      <c r="P63" s="80"/>
+      <c r="Q63" s="80"/>
+      <c r="R63" s="81"/>
+      <c r="S63" s="82"/>
+      <c r="T63" s="80"/>
+      <c r="U63" s="83"/>
+      <c r="V63" s="80"/>
+      <c r="W63" s="80"/>
+      <c r="X63" s="108">
         <v>1</v>
       </c>
-      <c r="Y63" s="82"/>
-      <c r="Z63" s="83"/>
-      <c r="AA63" s="84"/>
-      <c r="AB63" s="81"/>
-      <c r="AC63" s="81"/>
-      <c r="AD63" s="94"/>
-      <c r="AE63" s="95"/>
-      <c r="AF63" s="96"/>
+      <c r="Y63" s="81"/>
+      <c r="Z63" s="82"/>
+      <c r="AA63" s="83"/>
+      <c r="AB63" s="80"/>
+      <c r="AC63" s="80"/>
+      <c r="AD63" s="90"/>
+      <c r="AE63" s="91"/>
+      <c r="AF63" s="92"/>
       <c r="AG63" s="10"/>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.35">
@@ -3853,27 +3851,27 @@
       <c r="I64" s="5"/>
       <c r="J64" s="6"/>
       <c r="K64" s="39"/>
-      <c r="L64" s="83"/>
-      <c r="M64" s="81"/>
-      <c r="N64" s="81"/>
-      <c r="O64" s="81"/>
-      <c r="P64" s="81"/>
-      <c r="Q64" s="81"/>
-      <c r="R64" s="82"/>
-      <c r="S64" s="83"/>
-      <c r="T64" s="81"/>
-      <c r="U64" s="84"/>
-      <c r="V64" s="81"/>
-      <c r="W64" s="81"/>
-      <c r="X64" s="81"/>
-      <c r="Y64" s="82"/>
-      <c r="Z64" s="83"/>
-      <c r="AA64" s="84"/>
-      <c r="AB64" s="81"/>
-      <c r="AC64" s="81"/>
-      <c r="AD64" s="94"/>
-      <c r="AE64" s="95"/>
-      <c r="AF64" s="96"/>
+      <c r="L64" s="82"/>
+      <c r="M64" s="80"/>
+      <c r="N64" s="80"/>
+      <c r="O64" s="80"/>
+      <c r="P64" s="80"/>
+      <c r="Q64" s="80"/>
+      <c r="R64" s="81"/>
+      <c r="S64" s="82"/>
+      <c r="T64" s="80"/>
+      <c r="U64" s="83"/>
+      <c r="V64" s="80"/>
+      <c r="W64" s="80"/>
+      <c r="X64" s="80"/>
+      <c r="Y64" s="81"/>
+      <c r="Z64" s="82"/>
+      <c r="AA64" s="83"/>
+      <c r="AB64" s="80"/>
+      <c r="AC64" s="80"/>
+      <c r="AD64" s="90"/>
+      <c r="AE64" s="91"/>
+      <c r="AF64" s="92"/>
       <c r="AG64" s="10"/>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
@@ -3894,27 +3892,27 @@
       <c r="I65" s="5"/>
       <c r="J65" s="6"/>
       <c r="K65" s="39"/>
-      <c r="L65" s="83"/>
-      <c r="M65" s="81"/>
-      <c r="N65" s="81"/>
-      <c r="O65" s="81"/>
-      <c r="P65" s="81"/>
-      <c r="Q65" s="81"/>
-      <c r="R65" s="82"/>
-      <c r="S65" s="83"/>
-      <c r="T65" s="81"/>
-      <c r="U65" s="84"/>
-      <c r="V65" s="81"/>
-      <c r="W65" s="81"/>
-      <c r="X65" s="81"/>
-      <c r="Y65" s="82"/>
-      <c r="Z65" s="83"/>
-      <c r="AA65" s="84"/>
-      <c r="AB65" s="81"/>
-      <c r="AC65" s="81"/>
-      <c r="AD65" s="94"/>
-      <c r="AE65" s="95"/>
-      <c r="AF65" s="96"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="80"/>
+      <c r="N65" s="80"/>
+      <c r="O65" s="80"/>
+      <c r="P65" s="80"/>
+      <c r="Q65" s="80"/>
+      <c r="R65" s="81"/>
+      <c r="S65" s="82"/>
+      <c r="T65" s="80"/>
+      <c r="U65" s="83"/>
+      <c r="V65" s="80"/>
+      <c r="W65" s="80"/>
+      <c r="X65" s="80"/>
+      <c r="Y65" s="81"/>
+      <c r="Z65" s="82"/>
+      <c r="AA65" s="83"/>
+      <c r="AB65" s="80"/>
+      <c r="AC65" s="80"/>
+      <c r="AD65" s="90"/>
+      <c r="AE65" s="91"/>
+      <c r="AF65" s="92"/>
       <c r="AG65" s="10"/>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
@@ -3931,29 +3929,29 @@
       <c r="I66" s="5"/>
       <c r="J66" s="6"/>
       <c r="K66" s="39"/>
-      <c r="L66" s="83"/>
-      <c r="M66" s="81"/>
-      <c r="N66" s="81"/>
-      <c r="O66" s="81"/>
-      <c r="P66" s="81"/>
-      <c r="Q66" s="81"/>
-      <c r="R66" s="82"/>
-      <c r="S66" s="83"/>
-      <c r="T66" s="81"/>
-      <c r="U66" s="84"/>
-      <c r="V66" s="81"/>
-      <c r="W66" s="81"/>
-      <c r="X66" s="81"/>
-      <c r="Y66" s="119">
+      <c r="L66" s="82"/>
+      <c r="M66" s="80"/>
+      <c r="N66" s="80"/>
+      <c r="O66" s="80"/>
+      <c r="P66" s="80"/>
+      <c r="Q66" s="80"/>
+      <c r="R66" s="81"/>
+      <c r="S66" s="82"/>
+      <c r="T66" s="80"/>
+      <c r="U66" s="83"/>
+      <c r="V66" s="80"/>
+      <c r="W66" s="80"/>
+      <c r="X66" s="80"/>
+      <c r="Y66" s="114">
         <v>1</v>
       </c>
-      <c r="Z66" s="83"/>
-      <c r="AA66" s="84"/>
-      <c r="AB66" s="81"/>
-      <c r="AC66" s="81"/>
-      <c r="AD66" s="94"/>
-      <c r="AE66" s="95"/>
-      <c r="AF66" s="96"/>
+      <c r="Z66" s="82"/>
+      <c r="AA66" s="83"/>
+      <c r="AB66" s="80"/>
+      <c r="AC66" s="80"/>
+      <c r="AD66" s="90"/>
+      <c r="AE66" s="91"/>
+      <c r="AF66" s="92"/>
       <c r="AG66" s="10"/>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
@@ -3968,27 +3966,27 @@
       <c r="I67" s="5"/>
       <c r="J67" s="6"/>
       <c r="K67" s="39"/>
-      <c r="L67" s="77"/>
-      <c r="M67" s="68"/>
-      <c r="N67" s="68"/>
-      <c r="O67" s="68"/>
-      <c r="P67" s="68"/>
-      <c r="Q67" s="68"/>
-      <c r="R67" s="78"/>
-      <c r="S67" s="77"/>
-      <c r="T67" s="68"/>
-      <c r="U67" s="69"/>
-      <c r="V67" s="68"/>
-      <c r="W67" s="68"/>
-      <c r="X67" s="68"/>
-      <c r="Y67" s="78"/>
-      <c r="Z67" s="77"/>
-      <c r="AA67" s="69"/>
-      <c r="AB67" s="68"/>
-      <c r="AC67" s="68"/>
-      <c r="AD67" s="97"/>
-      <c r="AE67" s="98"/>
-      <c r="AF67" s="99"/>
+      <c r="L67" s="76"/>
+      <c r="M67" s="67"/>
+      <c r="N67" s="67"/>
+      <c r="O67" s="67"/>
+      <c r="P67" s="67"/>
+      <c r="Q67" s="67"/>
+      <c r="R67" s="77"/>
+      <c r="S67" s="76"/>
+      <c r="T67" s="67"/>
+      <c r="U67" s="68"/>
+      <c r="V67" s="67"/>
+      <c r="W67" s="67"/>
+      <c r="X67" s="67"/>
+      <c r="Y67" s="77"/>
+      <c r="Z67" s="76"/>
+      <c r="AA67" s="68"/>
+      <c r="AB67" s="67"/>
+      <c r="AC67" s="67"/>
+      <c r="AD67" s="93"/>
+      <c r="AE67" s="94"/>
+      <c r="AF67" s="95"/>
       <c r="AG67" s="10"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
@@ -4005,27 +4003,27 @@
       <c r="I68" s="5"/>
       <c r="J68" s="6"/>
       <c r="K68" s="39"/>
-      <c r="L68" s="83"/>
-      <c r="M68" s="81"/>
-      <c r="N68" s="81"/>
-      <c r="O68" s="81"/>
-      <c r="P68" s="81"/>
-      <c r="Q68" s="81"/>
-      <c r="R68" s="82"/>
-      <c r="S68" s="83"/>
-      <c r="T68" s="81"/>
-      <c r="U68" s="84"/>
-      <c r="V68" s="81"/>
-      <c r="W68" s="81"/>
-      <c r="X68" s="81"/>
-      <c r="Y68" s="82"/>
-      <c r="Z68" s="83"/>
-      <c r="AA68" s="84"/>
-      <c r="AB68" s="81"/>
-      <c r="AC68" s="81"/>
-      <c r="AD68" s="94"/>
-      <c r="AE68" s="95"/>
-      <c r="AF68" s="96"/>
+      <c r="L68" s="82"/>
+      <c r="M68" s="80"/>
+      <c r="N68" s="80"/>
+      <c r="O68" s="80"/>
+      <c r="P68" s="80"/>
+      <c r="Q68" s="80"/>
+      <c r="R68" s="81"/>
+      <c r="S68" s="82"/>
+      <c r="T68" s="80"/>
+      <c r="U68" s="83"/>
+      <c r="V68" s="80"/>
+      <c r="W68" s="80"/>
+      <c r="X68" s="80"/>
+      <c r="Y68" s="81"/>
+      <c r="Z68" s="82"/>
+      <c r="AA68" s="83"/>
+      <c r="AB68" s="80"/>
+      <c r="AC68" s="80"/>
+      <c r="AD68" s="90"/>
+      <c r="AE68" s="91"/>
+      <c r="AF68" s="92"/>
       <c r="AG68" s="10"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
@@ -4042,27 +4040,27 @@
       <c r="I69" s="5"/>
       <c r="J69" s="6"/>
       <c r="K69" s="39"/>
-      <c r="L69" s="83"/>
-      <c r="M69" s="81"/>
-      <c r="N69" s="81"/>
-      <c r="O69" s="81"/>
-      <c r="P69" s="81"/>
-      <c r="Q69" s="81"/>
-      <c r="R69" s="82"/>
-      <c r="S69" s="83"/>
-      <c r="T69" s="81"/>
-      <c r="U69" s="84"/>
-      <c r="V69" s="81"/>
-      <c r="W69" s="81"/>
-      <c r="X69" s="113"/>
-      <c r="Y69" s="82"/>
-      <c r="Z69" s="83"/>
-      <c r="AA69" s="84"/>
-      <c r="AB69" s="81"/>
-      <c r="AC69" s="81"/>
-      <c r="AD69" s="94"/>
-      <c r="AE69" s="95"/>
-      <c r="AF69" s="96"/>
+      <c r="L69" s="82"/>
+      <c r="M69" s="80"/>
+      <c r="N69" s="80"/>
+      <c r="O69" s="80"/>
+      <c r="P69" s="80"/>
+      <c r="Q69" s="80"/>
+      <c r="R69" s="81"/>
+      <c r="S69" s="82"/>
+      <c r="T69" s="80"/>
+      <c r="U69" s="83"/>
+      <c r="V69" s="80"/>
+      <c r="W69" s="80"/>
+      <c r="X69" s="108"/>
+      <c r="Y69" s="81"/>
+      <c r="Z69" s="82"/>
+      <c r="AA69" s="83"/>
+      <c r="AB69" s="80"/>
+      <c r="AC69" s="80"/>
+      <c r="AD69" s="90"/>
+      <c r="AE69" s="91"/>
+      <c r="AF69" s="92"/>
       <c r="AG69" s="10"/>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
@@ -4086,17 +4084,17 @@
       <c r="R70" s="54"/>
       <c r="S70" s="60"/>
       <c r="T70" s="63"/>
-      <c r="U70" s="66"/>
+      <c r="U70" s="65"/>
       <c r="V70" s="63"/>
       <c r="W70" s="63"/>
       <c r="X70" s="63"/>
       <c r="Y70" s="54"/>
       <c r="Z70" s="60"/>
-      <c r="AA70" s="66"/>
+      <c r="AA70" s="65"/>
       <c r="AB70" s="63"/>
       <c r="AC70" s="63"/>
-      <c r="AD70" s="100"/>
-      <c r="AE70" s="101"/>
+      <c r="AD70" s="96"/>
+      <c r="AE70" s="97"/>
       <c r="AF70" s="56"/>
       <c r="AG70" s="10"/>
     </row>
@@ -4114,27 +4112,27 @@
       <c r="I71" s="2"/>
       <c r="J71" s="3"/>
       <c r="K71" s="39"/>
-      <c r="L71" s="73"/>
-      <c r="M71" s="74"/>
-      <c r="N71" s="74"/>
-      <c r="O71" s="74"/>
-      <c r="P71" s="74"/>
-      <c r="Q71" s="74"/>
-      <c r="R71" s="75"/>
-      <c r="S71" s="73"/>
-      <c r="T71" s="74"/>
-      <c r="U71" s="76"/>
-      <c r="V71" s="74"/>
-      <c r="W71" s="74"/>
-      <c r="X71" s="74"/>
-      <c r="Y71" s="75"/>
-      <c r="Z71" s="73"/>
-      <c r="AA71" s="76"/>
-      <c r="AB71" s="74"/>
-      <c r="AC71" s="74"/>
-      <c r="AD71" s="91"/>
-      <c r="AE71" s="92"/>
-      <c r="AF71" s="93"/>
+      <c r="L71" s="72"/>
+      <c r="M71" s="73"/>
+      <c r="N71" s="73"/>
+      <c r="O71" s="73"/>
+      <c r="P71" s="73"/>
+      <c r="Q71" s="73"/>
+      <c r="R71" s="74"/>
+      <c r="S71" s="72"/>
+      <c r="T71" s="73"/>
+      <c r="U71" s="75"/>
+      <c r="V71" s="73"/>
+      <c r="W71" s="73"/>
+      <c r="X71" s="73"/>
+      <c r="Y71" s="74"/>
+      <c r="Z71" s="72"/>
+      <c r="AA71" s="75"/>
+      <c r="AB71" s="73"/>
+      <c r="AC71" s="73"/>
+      <c r="AD71" s="87"/>
+      <c r="AE71" s="88"/>
+      <c r="AF71" s="89"/>
       <c r="AG71" s="10"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
@@ -4151,27 +4149,27 @@
       <c r="I72" s="5"/>
       <c r="J72" s="6"/>
       <c r="K72" s="39"/>
-      <c r="L72" s="83"/>
-      <c r="M72" s="81"/>
-      <c r="N72" s="81"/>
-      <c r="O72" s="81"/>
-      <c r="P72" s="81"/>
-      <c r="Q72" s="81"/>
-      <c r="R72" s="82"/>
-      <c r="S72" s="83"/>
-      <c r="T72" s="81"/>
-      <c r="U72" s="84"/>
-      <c r="V72" s="81"/>
-      <c r="W72" s="81"/>
-      <c r="X72" s="81"/>
-      <c r="Y72" s="82"/>
-      <c r="Z72" s="80"/>
-      <c r="AA72" s="84"/>
-      <c r="AB72" s="81"/>
-      <c r="AC72" s="81"/>
-      <c r="AD72" s="94"/>
-      <c r="AE72" s="95"/>
-      <c r="AF72" s="96"/>
+      <c r="L72" s="82"/>
+      <c r="M72" s="80"/>
+      <c r="N72" s="80"/>
+      <c r="O72" s="80"/>
+      <c r="P72" s="80"/>
+      <c r="Q72" s="80"/>
+      <c r="R72" s="81"/>
+      <c r="S72" s="82"/>
+      <c r="T72" s="80"/>
+      <c r="U72" s="83"/>
+      <c r="V72" s="80"/>
+      <c r="W72" s="80"/>
+      <c r="X72" s="80"/>
+      <c r="Y72" s="81"/>
+      <c r="Z72" s="79"/>
+      <c r="AA72" s="83"/>
+      <c r="AB72" s="80"/>
+      <c r="AC72" s="80"/>
+      <c r="AD72" s="90"/>
+      <c r="AE72" s="91"/>
+      <c r="AF72" s="92"/>
       <c r="AG72" s="10"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
@@ -4188,27 +4186,27 @@
       <c r="I73" s="5"/>
       <c r="J73" s="6"/>
       <c r="K73" s="39"/>
-      <c r="L73" s="83"/>
-      <c r="M73" s="81"/>
-      <c r="N73" s="81"/>
-      <c r="O73" s="81"/>
-      <c r="P73" s="81"/>
-      <c r="Q73" s="81"/>
-      <c r="R73" s="82"/>
-      <c r="S73" s="83"/>
-      <c r="T73" s="81"/>
-      <c r="U73" s="84"/>
-      <c r="V73" s="81"/>
-      <c r="W73" s="81"/>
-      <c r="X73" s="81"/>
-      <c r="Y73" s="82"/>
-      <c r="Z73" s="84"/>
-      <c r="AA73" s="84"/>
-      <c r="AB73" s="81"/>
-      <c r="AC73" s="81"/>
-      <c r="AD73" s="94"/>
-      <c r="AE73" s="95"/>
-      <c r="AF73" s="96"/>
+      <c r="L73" s="82"/>
+      <c r="M73" s="80"/>
+      <c r="N73" s="80"/>
+      <c r="O73" s="80"/>
+      <c r="P73" s="80"/>
+      <c r="Q73" s="80"/>
+      <c r="R73" s="81"/>
+      <c r="S73" s="82"/>
+      <c r="T73" s="80"/>
+      <c r="U73" s="83"/>
+      <c r="V73" s="80"/>
+      <c r="W73" s="80"/>
+      <c r="X73" s="80"/>
+      <c r="Y73" s="81"/>
+      <c r="Z73" s="83"/>
+      <c r="AA73" s="83"/>
+      <c r="AB73" s="80"/>
+      <c r="AC73" s="80"/>
+      <c r="AD73" s="90"/>
+      <c r="AE73" s="91"/>
+      <c r="AF73" s="92"/>
       <c r="AG73" s="10"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
@@ -4229,27 +4227,27 @@
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="39"/>
-      <c r="L74" s="116"/>
-      <c r="M74" s="81"/>
-      <c r="N74" s="81"/>
-      <c r="O74" s="81"/>
-      <c r="P74" s="81"/>
-      <c r="Q74" s="81"/>
-      <c r="R74" s="82"/>
-      <c r="S74" s="83"/>
-      <c r="T74" s="81"/>
-      <c r="U74" s="84"/>
-      <c r="V74" s="81"/>
-      <c r="W74" s="81"/>
-      <c r="X74" s="81"/>
-      <c r="Y74" s="82"/>
-      <c r="Z74" s="83"/>
-      <c r="AA74" s="84"/>
-      <c r="AB74" s="81"/>
-      <c r="AC74" s="81"/>
-      <c r="AD74" s="107"/>
-      <c r="AE74" s="94"/>
-      <c r="AF74" s="96"/>
+      <c r="L74" s="111"/>
+      <c r="M74" s="80"/>
+      <c r="N74" s="80"/>
+      <c r="O74" s="80"/>
+      <c r="P74" s="80"/>
+      <c r="Q74" s="80"/>
+      <c r="R74" s="81"/>
+      <c r="S74" s="82"/>
+      <c r="T74" s="80"/>
+      <c r="U74" s="83"/>
+      <c r="V74" s="80"/>
+      <c r="W74" s="80"/>
+      <c r="X74" s="80"/>
+      <c r="Y74" s="81"/>
+      <c r="Z74" s="82"/>
+      <c r="AA74" s="83"/>
+      <c r="AB74" s="80"/>
+      <c r="AC74" s="80"/>
+      <c r="AD74" s="103"/>
+      <c r="AE74" s="90"/>
+      <c r="AF74" s="92"/>
       <c r="AG74" s="10"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
@@ -4266,27 +4264,27 @@
       <c r="I75" s="5"/>
       <c r="J75" s="6"/>
       <c r="K75" s="39"/>
-      <c r="L75" s="83"/>
-      <c r="M75" s="81"/>
-      <c r="N75" s="81"/>
-      <c r="O75" s="81"/>
-      <c r="P75" s="81"/>
-      <c r="Q75" s="81"/>
-      <c r="R75" s="89"/>
-      <c r="S75" s="83"/>
-      <c r="T75" s="81"/>
-      <c r="U75" s="84"/>
-      <c r="V75" s="81"/>
-      <c r="W75" s="81"/>
-      <c r="X75" s="81"/>
-      <c r="Y75" s="89"/>
-      <c r="Z75" s="83"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="81"/>
-      <c r="AC75" s="106"/>
-      <c r="AD75" s="108"/>
-      <c r="AE75" s="95"/>
-      <c r="AF75" s="89"/>
+      <c r="L75" s="82"/>
+      <c r="M75" s="80"/>
+      <c r="N75" s="80"/>
+      <c r="O75" s="80"/>
+      <c r="P75" s="80"/>
+      <c r="Q75" s="80"/>
+      <c r="R75" s="85"/>
+      <c r="S75" s="82"/>
+      <c r="T75" s="80"/>
+      <c r="U75" s="83"/>
+      <c r="V75" s="80"/>
+      <c r="W75" s="80"/>
+      <c r="X75" s="80"/>
+      <c r="Y75" s="85"/>
+      <c r="Z75" s="82"/>
+      <c r="AA75" s="83"/>
+      <c r="AB75" s="80"/>
+      <c r="AC75" s="102"/>
+      <c r="AD75" s="104"/>
+      <c r="AE75" s="91"/>
+      <c r="AF75" s="109"/>
       <c r="AG75" s="10"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
@@ -4301,27 +4299,27 @@
       <c r="I76" s="5"/>
       <c r="J76" s="6"/>
       <c r="K76" s="39"/>
-      <c r="L76" s="83"/>
-      <c r="M76" s="81"/>
-      <c r="N76" s="81"/>
-      <c r="O76" s="81"/>
-      <c r="P76" s="81"/>
-      <c r="Q76" s="81"/>
-      <c r="R76" s="82"/>
-      <c r="S76" s="83"/>
-      <c r="T76" s="81"/>
-      <c r="U76" s="84"/>
-      <c r="V76" s="81"/>
-      <c r="W76" s="81"/>
-      <c r="X76" s="81"/>
-      <c r="Y76" s="82"/>
-      <c r="Z76" s="83"/>
-      <c r="AA76" s="84"/>
-      <c r="AB76" s="81"/>
-      <c r="AC76" s="81"/>
-      <c r="AD76" s="97"/>
-      <c r="AE76" s="94"/>
-      <c r="AF76" s="105"/>
+      <c r="L76" s="82"/>
+      <c r="M76" s="80"/>
+      <c r="N76" s="80"/>
+      <c r="O76" s="80"/>
+      <c r="P76" s="80"/>
+      <c r="Q76" s="80"/>
+      <c r="R76" s="81"/>
+      <c r="S76" s="82"/>
+      <c r="T76" s="80"/>
+      <c r="U76" s="83"/>
+      <c r="V76" s="80"/>
+      <c r="W76" s="80"/>
+      <c r="X76" s="80"/>
+      <c r="Y76" s="81"/>
+      <c r="Z76" s="82"/>
+      <c r="AA76" s="83"/>
+      <c r="AB76" s="80"/>
+      <c r="AC76" s="80"/>
+      <c r="AD76" s="93"/>
+      <c r="AE76" s="90"/>
+      <c r="AF76" s="101"/>
       <c r="AG76" s="10"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
@@ -4338,27 +4336,27 @@
       <c r="I77" s="5"/>
       <c r="J77" s="6"/>
       <c r="K77" s="39"/>
-      <c r="L77" s="83"/>
-      <c r="M77" s="81"/>
-      <c r="N77" s="81"/>
-      <c r="O77" s="81"/>
-      <c r="P77" s="81"/>
-      <c r="Q77" s="81"/>
-      <c r="R77" s="82"/>
-      <c r="S77" s="83"/>
-      <c r="T77" s="81"/>
-      <c r="U77" s="81"/>
-      <c r="V77" s="81"/>
-      <c r="W77" s="81"/>
-      <c r="X77" s="81"/>
-      <c r="Y77" s="82"/>
-      <c r="Z77" s="83"/>
-      <c r="AA77" s="84"/>
-      <c r="AB77" s="81"/>
-      <c r="AC77" s="81"/>
-      <c r="AD77" s="94"/>
-      <c r="AE77" s="107"/>
-      <c r="AF77" s="105"/>
+      <c r="L77" s="82"/>
+      <c r="M77" s="80"/>
+      <c r="N77" s="80"/>
+      <c r="O77" s="80"/>
+      <c r="P77" s="80"/>
+      <c r="Q77" s="80"/>
+      <c r="R77" s="81"/>
+      <c r="S77" s="82"/>
+      <c r="T77" s="80"/>
+      <c r="U77" s="80"/>
+      <c r="V77" s="80"/>
+      <c r="W77" s="80"/>
+      <c r="X77" s="80"/>
+      <c r="Y77" s="81"/>
+      <c r="Z77" s="82"/>
+      <c r="AA77" s="83"/>
+      <c r="AB77" s="80"/>
+      <c r="AC77" s="80"/>
+      <c r="AD77" s="90"/>
+      <c r="AE77" s="103"/>
+      <c r="AF77" s="101"/>
       <c r="AG77" s="10"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
@@ -4374,28 +4372,28 @@
       <c r="H78" s="4"/>
       <c r="I78" s="5"/>
       <c r="J78" s="6"/>
-      <c r="K78" s="70"/>
-      <c r="L78" s="80"/>
-      <c r="M78" s="85"/>
-      <c r="N78" s="113"/>
-      <c r="O78" s="113"/>
-      <c r="P78" s="113"/>
-      <c r="Q78" s="113"/>
-      <c r="R78" s="113"/>
-      <c r="S78" s="116"/>
-      <c r="T78" s="85"/>
-      <c r="U78" s="117"/>
-      <c r="V78" s="85"/>
-      <c r="W78" s="85"/>
-      <c r="X78" s="85"/>
-      <c r="Y78" s="118"/>
-      <c r="Z78" s="116"/>
-      <c r="AA78" s="113"/>
-      <c r="AB78" s="113"/>
-      <c r="AC78" s="85"/>
-      <c r="AD78" s="112"/>
-      <c r="AE78" s="57"/>
-      <c r="AF78" s="89"/>
+      <c r="K78" s="69"/>
+      <c r="L78" s="79"/>
+      <c r="M78" s="84"/>
+      <c r="N78" s="108"/>
+      <c r="O78" s="108"/>
+      <c r="P78" s="108"/>
+      <c r="Q78" s="108"/>
+      <c r="R78" s="108"/>
+      <c r="S78" s="111"/>
+      <c r="T78" s="84"/>
+      <c r="U78" s="112"/>
+      <c r="V78" s="84"/>
+      <c r="W78" s="84"/>
+      <c r="X78" s="84"/>
+      <c r="Y78" s="113"/>
+      <c r="Z78" s="111"/>
+      <c r="AA78" s="108"/>
+      <c r="AB78" s="108"/>
+      <c r="AC78" s="84"/>
+      <c r="AD78" s="115"/>
+      <c r="AE78" s="116"/>
+      <c r="AF78" s="109"/>
       <c r="AG78" s="10"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
@@ -4409,28 +4407,28 @@
       <c r="H79" s="4"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6"/>
-      <c r="K79" s="71"/>
-      <c r="L79" s="66"/>
+      <c r="K79" s="70"/>
+      <c r="L79" s="65"/>
       <c r="M79" s="63"/>
       <c r="N79" s="63"/>
       <c r="O79" s="63"/>
       <c r="P79" s="63"/>
       <c r="Q79" s="63"/>
-      <c r="R79" s="72"/>
+      <c r="R79" s="71"/>
       <c r="S79" s="60"/>
       <c r="T79" s="63"/>
       <c r="U79" s="63"/>
       <c r="V79" s="63"/>
-      <c r="W79" s="66"/>
+      <c r="W79" s="65"/>
       <c r="X79" s="63"/>
       <c r="Y79" s="54"/>
-      <c r="Z79" s="66"/>
+      <c r="Z79" s="65"/>
       <c r="AA79" s="63"/>
       <c r="AB79" s="63"/>
       <c r="AC79" s="63"/>
-      <c r="AD79" s="110"/>
-      <c r="AE79" s="100"/>
-      <c r="AF79" s="111"/>
+      <c r="AD79" s="106"/>
+      <c r="AE79" s="96"/>
+      <c r="AF79" s="107"/>
       <c r="AG79" s="10"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
@@ -4449,27 +4447,27 @@
       <c r="I80" s="2"/>
       <c r="J80" s="3"/>
       <c r="K80" s="55"/>
-      <c r="L80" s="73"/>
-      <c r="M80" s="74"/>
-      <c r="N80" s="74"/>
-      <c r="O80" s="74"/>
-      <c r="P80" s="74"/>
-      <c r="Q80" s="74"/>
-      <c r="R80" s="90"/>
-      <c r="S80" s="76"/>
-      <c r="T80" s="74"/>
-      <c r="U80" s="74"/>
-      <c r="V80" s="74"/>
-      <c r="W80" s="74"/>
-      <c r="X80" s="74"/>
-      <c r="Y80" s="90"/>
-      <c r="Z80" s="76"/>
-      <c r="AA80" s="74"/>
-      <c r="AB80" s="74"/>
-      <c r="AC80" s="74"/>
-      <c r="AD80" s="97"/>
-      <c r="AE80" s="97"/>
-      <c r="AF80" s="109"/>
+      <c r="L80" s="72"/>
+      <c r="M80" s="73"/>
+      <c r="N80" s="73"/>
+      <c r="O80" s="73"/>
+      <c r="P80" s="73"/>
+      <c r="Q80" s="73"/>
+      <c r="R80" s="86"/>
+      <c r="S80" s="75"/>
+      <c r="T80" s="73"/>
+      <c r="U80" s="73"/>
+      <c r="V80" s="73"/>
+      <c r="W80" s="73"/>
+      <c r="X80" s="73"/>
+      <c r="Y80" s="86"/>
+      <c r="Z80" s="75"/>
+      <c r="AA80" s="73"/>
+      <c r="AB80" s="73"/>
+      <c r="AC80" s="73"/>
+      <c r="AD80" s="93"/>
+      <c r="AE80" s="93"/>
+      <c r="AF80" s="105"/>
       <c r="AG80" s="10"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
@@ -4494,21 +4492,21 @@
       <c r="O81" s="63"/>
       <c r="P81" s="63"/>
       <c r="Q81" s="63"/>
-      <c r="R81" s="72"/>
-      <c r="S81" s="66"/>
+      <c r="R81" s="71"/>
+      <c r="S81" s="65"/>
       <c r="T81" s="63"/>
       <c r="U81" s="63"/>
       <c r="V81" s="63"/>
       <c r="W81" s="63"/>
       <c r="X81" s="63"/>
-      <c r="Y81" s="72"/>
-      <c r="Z81" s="66"/>
-      <c r="AA81" s="67"/>
-      <c r="AB81" s="67"/>
+      <c r="Y81" s="71"/>
+      <c r="Z81" s="65"/>
+      <c r="AA81" s="66"/>
+      <c r="AB81" s="66"/>
       <c r="AC81" s="63"/>
-      <c r="AD81" s="110"/>
-      <c r="AE81" s="110"/>
-      <c r="AF81" s="111"/>
+      <c r="AD81" s="106"/>
+      <c r="AE81" s="106"/>
+      <c r="AF81" s="107"/>
       <c r="AG81" s="10"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
@@ -4604,13 +4602,13 @@
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C89" s="104"/>
+      <c r="C89" s="100"/>
       <c r="D89" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="C90" s="108"/>
+      <c r="C90" s="104"/>
       <c r="D90" t="s">
         <v>74</v>
       </c>

</xml_diff>